<commit_message>
corrected question number of HBSC and GSHS pages
</commit_message>
<xml_diff>
--- a/GACPAQ pages.xlsx
+++ b/GACPAQ pages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doncastillo/Code/gacpaq/gacpaq-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38E4B249-4D9C-0C43-A4C6-D17B6337DA71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095F386F-8233-1440-95F4-34A143F6CFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18260" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
+    <workbookView xWindow="20300" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,19 +18,18 @@
     <sheet name="Section Pages" sheetId="3" r:id="rId3"/>
     <sheet name="Participant Responses - 120824" sheetId="5" r:id="rId4"/>
     <sheet name="Images" sheetId="4" r:id="rId5"/>
-    <sheet name="HBSC and GSHS" sheetId="7" r:id="rId6"/>
-    <sheet name="Country Status" sheetId="8" r:id="rId7"/>
+    <sheet name="Country Status" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_Hlk120517734" localSheetId="2">'Section Pages'!$J$26</definedName>
     <definedName name="_Hlk122699234" localSheetId="2">'Section Pages'!$J$32</definedName>
     <definedName name="OLE_LINK10" localSheetId="2">'Section Pages'!$K$11</definedName>
-    <definedName name="OLE_LINK109" localSheetId="2">'Section Pages'!$J$67</definedName>
+    <definedName name="OLE_LINK109" localSheetId="2">'Section Pages'!$J$69</definedName>
     <definedName name="OLE_LINK14" localSheetId="2">'Section Pages'!$K$13</definedName>
     <definedName name="OLE_LINK16" localSheetId="2">'Section Pages'!$K$14</definedName>
     <definedName name="OLE_LINK169" localSheetId="2">'Section Pages'!$K$61</definedName>
     <definedName name="OLE_LINK18" localSheetId="2">'Section Pages'!$K$15</definedName>
-    <definedName name="OLE_LINK184" localSheetId="2">'Section Pages'!$K$68</definedName>
+    <definedName name="OLE_LINK184" localSheetId="2">'Section Pages'!$K$70</definedName>
     <definedName name="OLE_LINK23" localSheetId="2">'Section Pages'!$K$11</definedName>
     <definedName name="OLE_LINK25" localSheetId="2">'Section Pages'!$K$12</definedName>
     <definedName name="OLE_LINK33" localSheetId="2">'Section Pages'!$J$19</definedName>
@@ -65,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="395">
   <si>
     <t>Page Number</t>
   </si>
@@ -2584,13 +2583,121 @@
   </si>
   <si>
     <t>awaiting data; narration processing</t>
+  </si>
+  <si>
+    <t>Preamble - PA</t>
+  </si>
+  <si>
+    <t>Preamble - Sitting</t>
+  </si>
+  <si>
+    <t>Preamble - Sleep</t>
+  </si>
+  <si>
+    <t>hbsc_intro</t>
+  </si>
+  <si>
+    <t>hbsc_preamble</t>
+  </si>
+  <si>
+    <t>hbsc_1</t>
+  </si>
+  <si>
+    <t>hbsc_2</t>
+  </si>
+  <si>
+    <t>hbsc_extro</t>
+  </si>
+  <si>
+    <t>gshs_intro</t>
+  </si>
+  <si>
+    <t>gshs_preamble_pa</t>
+  </si>
+  <si>
+    <t>gshs_1</t>
+  </si>
+  <si>
+    <t>gshs_2</t>
+  </si>
+  <si>
+    <t>gshs_3</t>
+  </si>
+  <si>
+    <t>gshs_4</t>
+  </si>
+  <si>
+    <t>gshs_preamble_sitting</t>
+  </si>
+  <si>
+    <t>gshs_5</t>
+  </si>
+  <si>
+    <t>gshs_preamble_sleep</t>
+  </si>
+  <si>
+    <t>gshs_6</t>
+  </si>
+  <si>
+    <t>gshs_extro</t>
+  </si>
+  <si>
+    <t>HBSCIntro</t>
+  </si>
+  <si>
+    <t>HBSCPreamble</t>
+  </si>
+  <si>
+    <t>HBSC1</t>
+  </si>
+  <si>
+    <t>HBSC2</t>
+  </si>
+  <si>
+    <t>HBSCExtro</t>
+  </si>
+  <si>
+    <t>GSHSIntro</t>
+  </si>
+  <si>
+    <t>GSHSPreamble_PA</t>
+  </si>
+  <si>
+    <t>GSHS1</t>
+  </si>
+  <si>
+    <t>GSHS2</t>
+  </si>
+  <si>
+    <t>GSHS3</t>
+  </si>
+  <si>
+    <t>GSHS4</t>
+  </si>
+  <si>
+    <t>GSHSPreamble_Sitting</t>
+  </si>
+  <si>
+    <t>GSHS5</t>
+  </si>
+  <si>
+    <t>GSHSPreamble_Sleep</t>
+  </si>
+  <si>
+    <t>GSHS6</t>
+  </si>
+  <si>
+    <t>GSHSExtro</t>
+  </si>
+  <si>
+    <t>AppExtrp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2748,8 +2855,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="21">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2870,6 +2991,18 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -2955,7 +3088,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3121,6 +3254,11 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4065,19 +4203,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{460A6040-ECD3-3B44-8E8B-CFDB1F40DF24}">
-  <dimension ref="A1:K68"/>
+  <dimension ref="A1:K88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
+      <selection pane="bottomRight" activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" style="14" customWidth="1"/>
-    <col min="2" max="3" width="10.83203125" style="13"/>
+    <col min="2" max="2" width="21.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="13"/>
     <col min="4" max="4" width="14.83203125" style="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.1640625" style="13" bestFit="1" customWidth="1"/>
@@ -5606,54 +5745,308 @@
         <v>110</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="32" x14ac:dyDescent="0.2">
-      <c r="A66" s="22" t="s">
-        <v>61</v>
-      </c>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66" s="22"/>
       <c r="B66" s="13">
         <v>30</v>
       </c>
-      <c r="F66" s="34" t="s">
+      <c r="F66" s="35"/>
+      <c r="G66" s="35"/>
+      <c r="K66" s="11"/>
+    </row>
+    <row r="67" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+      <c r="A67" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="B67" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F67" s="34" t="s">
         <v>253</v>
       </c>
-      <c r="G66" s="34"/>
-      <c r="K66" s="11" t="s">
+      <c r="G67" s="34"/>
+      <c r="K67" s="11" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A67" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="B67" s="13">
-        <v>31</v>
-      </c>
-      <c r="F67" s="35" t="s">
-        <v>254</v>
-      </c>
-      <c r="G67" s="35"/>
-      <c r="J67" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="K67" s="11" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="B68" s="13">
+      <c r="B68" s="13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="A69" s="68" t="s">
+        <v>159</v>
+      </c>
+      <c r="B69" s="13">
+        <v>31</v>
+      </c>
+      <c r="F69" s="35" t="s">
+        <v>254</v>
+      </c>
+      <c r="G69" s="35"/>
+      <c r="J69" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="K69" s="11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="A70" s="68" t="s">
+        <v>159</v>
+      </c>
+      <c r="B70" s="13">
         <v>32</v>
       </c>
-      <c r="F68" s="13" t="s">
+      <c r="F70" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="J68" s="12" t="s">
+      <c r="J70" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="K68" s="11" t="s">
+      <c r="K70" s="11" t="s">
         <v>63</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A71" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="B71" s="13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A72" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="B72" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="F72" s="13" t="s">
+        <v>362</v>
+      </c>
+      <c r="H72" s="13" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A73" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="B73" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="F73" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="H73" s="13" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A74" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="B74" s="13">
+        <v>25</v>
+      </c>
+      <c r="F74" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="H74" s="13" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A75" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="B75" s="13">
+        <v>26</v>
+      </c>
+      <c r="F75" s="13" t="s">
+        <v>365</v>
+      </c>
+      <c r="H75" s="13" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A76" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="B76" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F76" s="13" t="s">
+        <v>366</v>
+      </c>
+      <c r="H76" s="13" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A77" s="69" t="s">
+        <v>343</v>
+      </c>
+      <c r="B77" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="F77" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="H77" s="13" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A78" s="69" t="s">
+        <v>343</v>
+      </c>
+      <c r="B78" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="F78" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="H78" s="13" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79" s="69" t="s">
+        <v>343</v>
+      </c>
+      <c r="B79" s="13">
+        <v>25</v>
+      </c>
+      <c r="F79" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="H79" s="13" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A80" s="69" t="s">
+        <v>343</v>
+      </c>
+      <c r="B80" s="13">
+        <v>26</v>
+      </c>
+      <c r="F80" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="H80" s="13" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="69" t="s">
+        <v>343</v>
+      </c>
+      <c r="B81" s="13">
+        <v>27</v>
+      </c>
+      <c r="F81" s="13" t="s">
+        <v>371</v>
+      </c>
+      <c r="H81" s="13" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="69" t="s">
+        <v>343</v>
+      </c>
+      <c r="B82" s="13">
+        <v>28</v>
+      </c>
+      <c r="F82" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="H82" s="70" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="69" t="s">
+        <v>343</v>
+      </c>
+      <c r="B83" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="F83" s="13" t="s">
+        <v>373</v>
+      </c>
+      <c r="H83" s="13" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="69" t="s">
+        <v>343</v>
+      </c>
+      <c r="B84" s="13">
+        <v>29</v>
+      </c>
+      <c r="F84" s="13" t="s">
+        <v>374</v>
+      </c>
+      <c r="H84" s="13" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="69" t="s">
+        <v>343</v>
+      </c>
+      <c r="B85" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="F85" s="13" t="s">
+        <v>375</v>
+      </c>
+      <c r="H85" s="13" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="69" t="s">
+        <v>343</v>
+      </c>
+      <c r="B86" s="13">
+        <v>30</v>
+      </c>
+      <c r="F86" s="13" t="s">
+        <v>376</v>
+      </c>
+      <c r="H86" s="13" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="69" t="s">
+        <v>343</v>
+      </c>
+      <c r="B87" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F87" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="H87" s="13" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="21" t="s">
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -5960,7 +6353,7 @@
       <pane xSplit="19" ySplit="19" topLeftCell="T20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="T1" sqref="T1"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="O10" sqref="O10"/>
+      <selection pane="bottomRight" activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6943,28 +7336,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53848F23-3158-5043-8031-96F0B937A7F4}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BEEE373-47BE-6F4C-8F66-ACD6798C647F}">
   <dimension ref="A1:AJ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="114" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="24" ySplit="17" topLeftCell="Y18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="T1" sqref="T1"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2:I2"/>
+      <selection pane="bottomRight" activeCell="I23" sqref="I23:I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
reset section total pages when pages are loaded
</commit_message>
<xml_diff>
--- a/GACPAQ pages.xlsx
+++ b/GACPAQ pages.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doncastillo/Code/gacpaq/gacpaq-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095F386F-8233-1440-95F4-34A143F6CFA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73E5751-C56B-9F4D-8BDC-C3A37C7F861F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20300" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
+    <workbookView xWindow="-20140" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="3" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Introductory Pages" sheetId="2" r:id="rId2"/>
     <sheet name="Section Pages" sheetId="3" r:id="rId3"/>
-    <sheet name="Participant Responses - 120824" sheetId="5" r:id="rId4"/>
-    <sheet name="Images" sheetId="4" r:id="rId5"/>
-    <sheet name="Country Status" sheetId="8" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="9" r:id="rId4"/>
+    <sheet name="Participant Responses - 120824" sheetId="5" r:id="rId5"/>
+    <sheet name="Images" sheetId="4" r:id="rId6"/>
+    <sheet name="Country Status" sheetId="8" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_Hlk120517734" localSheetId="2">'Section Pages'!$J$26</definedName>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="399">
   <si>
     <t>Page Number</t>
   </si>
@@ -2690,7 +2691,19 @@
     <t>GSHSExtro</t>
   </si>
   <si>
-    <t>AppExtrp</t>
+    <t>AppExtro</t>
+  </si>
+  <si>
+    <t>Adolescent</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>Extro (demo)</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -3088,7 +3101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3234,6 +3247,11 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3255,11 +3273,10 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4205,11 +4222,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{460A6040-ECD3-3B44-8E8B-CFDB1F40DF24}">
   <dimension ref="A1:K88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B87" sqref="B87"/>
+      <selection pane="bottomRight" activeCell="A61" sqref="A61:XFD66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5778,7 +5795,7 @@
       </c>
     </row>
     <row r="69" spans="1:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="A69" s="68" t="s">
+      <c r="A69" s="61" t="s">
         <v>159</v>
       </c>
       <c r="B69" s="13">
@@ -5796,7 +5813,7 @@
       </c>
     </row>
     <row r="70" spans="1:11" ht="51" x14ac:dyDescent="0.2">
-      <c r="A70" s="68" t="s">
+      <c r="A70" s="61" t="s">
         <v>159</v>
       </c>
       <c r="B70" s="13">
@@ -5891,7 +5908,7 @@
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A77" s="69" t="s">
+      <c r="A77" s="62" t="s">
         <v>343</v>
       </c>
       <c r="B77" s="13" t="s">
@@ -5905,7 +5922,7 @@
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A78" s="69" t="s">
+      <c r="A78" s="62" t="s">
         <v>343</v>
       </c>
       <c r="B78" s="13" t="s">
@@ -5919,7 +5936,7 @@
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A79" s="69" t="s">
+      <c r="A79" s="62" t="s">
         <v>343</v>
       </c>
       <c r="B79" s="13">
@@ -5933,7 +5950,7 @@
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A80" s="69" t="s">
+      <c r="A80" s="62" t="s">
         <v>343</v>
       </c>
       <c r="B80" s="13">
@@ -5946,8 +5963,8 @@
         <v>386</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="69" t="s">
+    <row r="81" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="62" t="s">
         <v>343</v>
       </c>
       <c r="B81" s="13">
@@ -5961,7 +5978,7 @@
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" s="69" t="s">
+      <c r="A82" s="62" t="s">
         <v>343</v>
       </c>
       <c r="B82" s="13">
@@ -5970,12 +5987,12 @@
       <c r="F82" s="13" t="s">
         <v>372</v>
       </c>
-      <c r="H82" s="70" t="s">
+      <c r="H82" s="63" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A83" s="69" t="s">
+      <c r="A83" s="62" t="s">
         <v>343</v>
       </c>
       <c r="B83" s="13" t="s">
@@ -5989,7 +6006,7 @@
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="69" t="s">
+      <c r="A84" s="62" t="s">
         <v>343</v>
       </c>
       <c r="B84" s="13">
@@ -6003,7 +6020,7 @@
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" s="69" t="s">
+      <c r="A85" s="62" t="s">
         <v>343</v>
       </c>
       <c r="B85" s="13" t="s">
@@ -6017,7 +6034,7 @@
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" s="69" t="s">
+      <c r="A86" s="62" t="s">
         <v>343</v>
       </c>
       <c r="B86" s="13">
@@ -6031,7 +6048,7 @@
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A87" s="69" t="s">
+      <c r="A87" s="62" t="s">
         <v>343</v>
       </c>
       <c r="B87" s="13" t="s">
@@ -6057,6 +6074,279 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA2E8CD8-51AA-6248-B595-B0D419C66E18}">
+  <dimension ref="A2:J16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="188" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.83203125" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" style="72" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" t="s">
+        <v>395</v>
+      </c>
+      <c r="E2" t="s">
+        <v>396</v>
+      </c>
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
+        <v>395</v>
+      </c>
+      <c r="J2" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>345</v>
+      </c>
+      <c r="H3" t="s">
+        <v>398</v>
+      </c>
+      <c r="I3" t="s">
+        <v>398</v>
+      </c>
+      <c r="J3" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4" s="73">
+        <v>0</v>
+      </c>
+      <c r="C4" s="71">
+        <v>5</v>
+      </c>
+      <c r="D4" s="74">
+        <v>5</v>
+      </c>
+      <c r="E4" s="9">
+        <v>5</v>
+      </c>
+      <c r="G4" t="s">
+        <v>344</v>
+      </c>
+      <c r="H4" t="s">
+        <v>398</v>
+      </c>
+      <c r="I4" t="s">
+        <v>398</v>
+      </c>
+      <c r="J4" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="73">
+        <v>1</v>
+      </c>
+      <c r="C5" s="71">
+        <v>10</v>
+      </c>
+      <c r="D5" s="74">
+        <v>10</v>
+      </c>
+      <c r="E5" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="73">
+        <v>2</v>
+      </c>
+      <c r="C6" s="71">
+        <v>7</v>
+      </c>
+      <c r="D6" s="74">
+        <v>7</v>
+      </c>
+      <c r="E6" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="73">
+        <v>3</v>
+      </c>
+      <c r="C7" s="71">
+        <v>6</v>
+      </c>
+      <c r="D7" s="74">
+        <v>6</v>
+      </c>
+      <c r="E7" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" s="73">
+        <v>4</v>
+      </c>
+      <c r="C8" s="71">
+        <v>14</v>
+      </c>
+      <c r="D8" s="74">
+        <v>14</v>
+      </c>
+      <c r="E8" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="73">
+        <v>5</v>
+      </c>
+      <c r="C9" s="71">
+        <v>6</v>
+      </c>
+      <c r="D9" s="74">
+        <v>6</v>
+      </c>
+      <c r="E9" s="9">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B10" s="73">
+        <v>6</v>
+      </c>
+      <c r="C10" s="71">
+        <v>5</v>
+      </c>
+      <c r="D10" s="74">
+        <v>5</v>
+      </c>
+      <c r="E10" s="9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="73">
+        <v>7</v>
+      </c>
+      <c r="C11" s="71">
+        <v>4</v>
+      </c>
+      <c r="D11" s="74">
+        <v>4</v>
+      </c>
+      <c r="E11" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
+        <v>397</v>
+      </c>
+      <c r="B12" s="73">
+        <v>8</v>
+      </c>
+      <c r="C12" s="71">
+        <v>3</v>
+      </c>
+      <c r="D12" s="74">
+        <v>3</v>
+      </c>
+      <c r="E12" s="9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="61" t="s">
+        <v>159</v>
+      </c>
+      <c r="B13" s="73"/>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="B14" s="73">
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="62" t="s">
+        <v>343</v>
+      </c>
+      <c r="B15" s="73">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="21" t="s">
+        <v>394</v>
+      </c>
+      <c r="B16" s="73">
+        <v>11</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F1C29E-D3B1-B848-83EE-B290EEFED926}">
   <dimension ref="A1:E17"/>
   <sheetViews>
@@ -6345,7 +6635,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2D16703-2F74-1B47-8687-B2CA15896FA8}">
   <dimension ref="A1:AE24"/>
   <sheetViews>
@@ -6389,38 +6679,38 @@
     <row r="1" spans="1:31" s="39" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="38"/>
       <c r="B1" s="38"/>
-      <c r="C1" s="61" t="s">
+      <c r="C1" s="64" t="s">
         <v>264</v>
       </c>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="66" t="s">
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="69" t="s">
         <v>265</v>
       </c>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="67"/>
-      <c r="K1" s="67"/>
-      <c r="L1" s="67"/>
-      <c r="M1" s="67"/>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-      <c r="P1" s="67"/>
-      <c r="Q1" s="67"/>
-      <c r="R1" s="67"/>
-      <c r="S1" s="67"/>
-      <c r="T1" s="67"/>
-      <c r="U1" s="67"/>
-      <c r="V1" s="67"/>
-      <c r="W1" s="67"/>
-      <c r="X1" s="67"/>
-      <c r="Y1" s="67"/>
-      <c r="Z1" s="67"/>
-      <c r="AA1" s="67"/>
-      <c r="AB1" s="67"/>
-      <c r="AC1" s="67"/>
-      <c r="AD1" s="67"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="70"/>
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70"/>
+      <c r="R1" s="70"/>
+      <c r="S1" s="70"/>
+      <c r="T1" s="70"/>
+      <c r="U1" s="70"/>
+      <c r="V1" s="70"/>
+      <c r="W1" s="70"/>
+      <c r="X1" s="70"/>
+      <c r="Y1" s="70"/>
+      <c r="Z1" s="70"/>
+      <c r="AA1" s="70"/>
+      <c r="AB1" s="70"/>
+      <c r="AC1" s="70"/>
+      <c r="AD1" s="70"/>
       <c r="AE1" s="39" t="s">
         <v>320</v>
       </c>
@@ -6440,46 +6730,46 @@
       <c r="F2" s="40" t="s">
         <v>269</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="65" t="s">
         <v>270</v>
       </c>
-      <c r="H2" s="63"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="62" t="s">
+      <c r="H2" s="66"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="65" t="s">
         <v>271</v>
       </c>
-      <c r="K2" s="63"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="62" t="s">
+      <c r="K2" s="66"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="65" t="s">
         <v>272</v>
       </c>
-      <c r="N2" s="63"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="62" t="s">
+      <c r="N2" s="66"/>
+      <c r="O2" s="67"/>
+      <c r="P2" s="65" t="s">
         <v>273</v>
       </c>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="64"/>
-      <c r="S2" s="62" t="s">
+      <c r="Q2" s="66"/>
+      <c r="R2" s="67"/>
+      <c r="S2" s="65" t="s">
         <v>274</v>
       </c>
-      <c r="T2" s="63"/>
-      <c r="U2" s="64"/>
-      <c r="V2" s="62" t="s">
+      <c r="T2" s="66"/>
+      <c r="U2" s="67"/>
+      <c r="V2" s="65" t="s">
         <v>275</v>
       </c>
-      <c r="W2" s="63"/>
-      <c r="X2" s="64"/>
-      <c r="Y2" s="62" t="s">
+      <c r="W2" s="66"/>
+      <c r="X2" s="67"/>
+      <c r="Y2" s="65" t="s">
         <v>276</v>
       </c>
-      <c r="Z2" s="63"/>
-      <c r="AA2" s="64"/>
-      <c r="AB2" s="65" t="s">
+      <c r="Z2" s="66"/>
+      <c r="AA2" s="67"/>
+      <c r="AB2" s="68" t="s">
         <v>322</v>
       </c>
-      <c r="AC2" s="65"/>
-      <c r="AD2" s="65"/>
+      <c r="AC2" s="68"/>
+      <c r="AD2" s="68"/>
     </row>
     <row r="3" spans="1:31" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="40"/>
@@ -7335,7 +7625,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BEEE373-47BE-6F4C-8F66-ACD6798C647F}">
   <dimension ref="A1:AJ22"/>
   <sheetViews>

</xml_diff>

<commit_message>
updated the GAC-PAQ excel file
</commit_message>
<xml_diff>
--- a/GACPAQ pages.xlsx
+++ b/GACPAQ pages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doncastillo/Code/gacpaq/gacpaq-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC904957-CE60-A840-A966-C0B7DDCC4209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CE2385-7994-234B-9255-B0EFBD509297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18260" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
+    <workbookView xWindow="19900" yWindow="-19140" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="766" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="399">
   <si>
     <t>Page Number</t>
   </si>
@@ -3101,7 +3101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3252,6 +3252,8 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3273,10 +3275,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4223,10 +4221,10 @@
   <dimension ref="A1:K88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A61" sqref="A61:XFD66"/>
+      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6084,7 +6082,7 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.83203125" customWidth="1"/>
-    <col min="2" max="2" width="4.83203125" style="72" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -6125,13 +6123,13 @@
       <c r="A4" s="33" t="s">
         <v>112</v>
       </c>
-      <c r="B4" s="73">
+      <c r="B4" s="35">
         <v>0</v>
       </c>
-      <c r="C4" s="71">
+      <c r="C4" s="64">
         <v>5</v>
       </c>
-      <c r="D4" s="74">
+      <c r="D4" s="65">
         <v>5</v>
       </c>
       <c r="E4" s="9">
@@ -6154,13 +6152,13 @@
       <c r="A5" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="73">
+      <c r="B5" s="35">
         <v>1</v>
       </c>
-      <c r="C5" s="71">
+      <c r="C5" s="64">
         <v>10</v>
       </c>
-      <c r="D5" s="74">
+      <c r="D5" s="65">
         <v>10</v>
       </c>
       <c r="E5" s="9">
@@ -6171,13 +6169,13 @@
       <c r="A6" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="73">
+      <c r="B6" s="35">
         <v>2</v>
       </c>
-      <c r="C6" s="71">
+      <c r="C6" s="64">
         <v>7</v>
       </c>
-      <c r="D6" s="74">
+      <c r="D6" s="65">
         <v>7</v>
       </c>
       <c r="E6" s="9">
@@ -6188,13 +6186,13 @@
       <c r="A7" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="B7" s="73">
+      <c r="B7" s="35">
         <v>3</v>
       </c>
-      <c r="C7" s="71">
+      <c r="C7" s="64">
         <v>6</v>
       </c>
-      <c r="D7" s="74">
+      <c r="D7" s="65">
         <v>6</v>
       </c>
       <c r="E7" s="9">
@@ -6205,13 +6203,13 @@
       <c r="A8" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="B8" s="73">
+      <c r="B8" s="35">
         <v>4</v>
       </c>
-      <c r="C8" s="71">
+      <c r="C8" s="64">
         <v>14</v>
       </c>
-      <c r="D8" s="74">
+      <c r="D8" s="65">
         <v>14</v>
       </c>
       <c r="E8" s="9">
@@ -6222,13 +6220,13 @@
       <c r="A9" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="73">
+      <c r="B9" s="35">
         <v>5</v>
       </c>
-      <c r="C9" s="71">
+      <c r="C9" s="64">
         <v>6</v>
       </c>
-      <c r="D9" s="74">
+      <c r="D9" s="65">
         <v>6</v>
       </c>
       <c r="E9" s="9">
@@ -6239,13 +6237,13 @@
       <c r="A10" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="73">
+      <c r="B10" s="35">
         <v>6</v>
       </c>
-      <c r="C10" s="71">
+      <c r="C10" s="64">
         <v>5</v>
       </c>
-      <c r="D10" s="74">
+      <c r="D10" s="65">
         <v>5</v>
       </c>
       <c r="E10" s="9">
@@ -6256,13 +6254,13 @@
       <c r="A11" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="73">
+      <c r="B11" s="35">
         <v>7</v>
       </c>
-      <c r="C11" s="71">
+      <c r="C11" s="64">
         <v>4</v>
       </c>
-      <c r="D11" s="74">
+      <c r="D11" s="65">
         <v>4</v>
       </c>
       <c r="E11" s="9">
@@ -6273,13 +6271,13 @@
       <c r="A12" s="22" t="s">
         <v>397</v>
       </c>
-      <c r="B12" s="73">
+      <c r="B12" s="35">
         <v>8</v>
       </c>
-      <c r="C12" s="71">
+      <c r="C12" s="64">
         <v>3</v>
       </c>
-      <c r="D12" s="74">
+      <c r="D12" s="65">
         <v>3</v>
       </c>
       <c r="E12" s="9">
@@ -6290,7 +6288,7 @@
       <c r="A13" s="61" t="s">
         <v>159</v>
       </c>
-      <c r="B13" s="73"/>
+      <c r="B13" s="35"/>
       <c r="C13">
         <v>4</v>
       </c>
@@ -6305,7 +6303,7 @@
       <c r="A14" s="18" t="s">
         <v>342</v>
       </c>
-      <c r="B14" s="73">
+      <c r="B14" s="35">
         <v>9</v>
       </c>
       <c r="D14">
@@ -6316,7 +6314,7 @@
       <c r="A15" s="62" t="s">
         <v>343</v>
       </c>
-      <c r="B15" s="73">
+      <c r="B15" s="35">
         <v>10</v>
       </c>
       <c r="D15">
@@ -6327,7 +6325,7 @@
       <c r="A16" s="21" t="s">
         <v>394</v>
       </c>
-      <c r="B16" s="73">
+      <c r="B16" s="35">
         <v>11</v>
       </c>
       <c r="C16">
@@ -6679,38 +6677,38 @@
     <row r="1" spans="1:31" s="39" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="38"/>
       <c r="B1" s="38"/>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="66" t="s">
         <v>264</v>
       </c>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="69" t="s">
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="71" t="s">
         <v>265</v>
       </c>
-      <c r="H1" s="70"/>
-      <c r="I1" s="70"/>
-      <c r="J1" s="70"/>
-      <c r="K1" s="70"/>
-      <c r="L1" s="70"/>
-      <c r="M1" s="70"/>
-      <c r="N1" s="70"/>
-      <c r="O1" s="70"/>
-      <c r="P1" s="70"/>
-      <c r="Q1" s="70"/>
-      <c r="R1" s="70"/>
-      <c r="S1" s="70"/>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
-      <c r="V1" s="70"/>
-      <c r="W1" s="70"/>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
-      <c r="Z1" s="70"/>
-      <c r="AA1" s="70"/>
-      <c r="AB1" s="70"/>
-      <c r="AC1" s="70"/>
-      <c r="AD1" s="70"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
+      <c r="P1" s="72"/>
+      <c r="Q1" s="72"/>
+      <c r="R1" s="72"/>
+      <c r="S1" s="72"/>
+      <c r="T1" s="72"/>
+      <c r="U1" s="72"/>
+      <c r="V1" s="72"/>
+      <c r="W1" s="72"/>
+      <c r="X1" s="72"/>
+      <c r="Y1" s="72"/>
+      <c r="Z1" s="72"/>
+      <c r="AA1" s="72"/>
+      <c r="AB1" s="72"/>
+      <c r="AC1" s="72"/>
+      <c r="AD1" s="72"/>
       <c r="AE1" s="39" t="s">
         <v>320</v>
       </c>
@@ -6730,46 +6728,46 @@
       <c r="F2" s="40" t="s">
         <v>269</v>
       </c>
-      <c r="G2" s="65" t="s">
+      <c r="G2" s="67" t="s">
         <v>270</v>
       </c>
-      <c r="H2" s="66"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="65" t="s">
+      <c r="H2" s="68"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="67" t="s">
         <v>271</v>
       </c>
-      <c r="K2" s="66"/>
-      <c r="L2" s="67"/>
-      <c r="M2" s="65" t="s">
+      <c r="K2" s="68"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="67" t="s">
         <v>272</v>
       </c>
-      <c r="N2" s="66"/>
-      <c r="O2" s="67"/>
-      <c r="P2" s="65" t="s">
+      <c r="N2" s="68"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="67" t="s">
         <v>273</v>
       </c>
-      <c r="Q2" s="66"/>
-      <c r="R2" s="67"/>
-      <c r="S2" s="65" t="s">
+      <c r="Q2" s="68"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="67" t="s">
         <v>274</v>
       </c>
-      <c r="T2" s="66"/>
-      <c r="U2" s="67"/>
-      <c r="V2" s="65" t="s">
+      <c r="T2" s="68"/>
+      <c r="U2" s="69"/>
+      <c r="V2" s="67" t="s">
         <v>275</v>
       </c>
-      <c r="W2" s="66"/>
-      <c r="X2" s="67"/>
-      <c r="Y2" s="65" t="s">
+      <c r="W2" s="68"/>
+      <c r="X2" s="69"/>
+      <c r="Y2" s="67" t="s">
         <v>276</v>
       </c>
-      <c r="Z2" s="66"/>
-      <c r="AA2" s="67"/>
-      <c r="AB2" s="68" t="s">
+      <c r="Z2" s="68"/>
+      <c r="AA2" s="69"/>
+      <c r="AB2" s="70" t="s">
         <v>322</v>
       </c>
-      <c r="AC2" s="68"/>
-      <c r="AD2" s="68"/>
+      <c r="AC2" s="70"/>
+      <c r="AD2" s="70"/>
     </row>
     <row r="3" spans="1:31" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="40"/>
@@ -7633,7 +7631,7 @@
       <pane xSplit="24" ySplit="17" topLeftCell="Y18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="T1" sqref="T1"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8280,7 +8278,9 @@
       <c r="I13" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="J13" s="55"/>
+      <c r="J13" s="56" t="s">
+        <v>349</v>
+      </c>
       <c r="K13" s="55"/>
       <c r="L13" s="48"/>
       <c r="M13" s="48"/>

</xml_diff>

<commit_message>
updated GAC-PAQ pages file, updated main study const
</commit_message>
<xml_diff>
--- a/GACPAQ pages.xlsx
+++ b/GACPAQ pages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doncastillo/Code/gacpaq/gacpaq-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CE2385-7994-234B-9255-B0EFBD509297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A848F92-8A70-4A40-99D3-05105AC9AEC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19900" yWindow="-19140" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
+    <workbookView xWindow="22200" yWindow="-20400" windowWidth="27540" windowHeight="21100" activeTab="6" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="405">
   <si>
     <t>Page Number</t>
   </si>
@@ -2704,6 +2704,24 @@
   </si>
   <si>
     <t>ok</t>
+  </si>
+  <si>
+    <t>in review</t>
+  </si>
+  <si>
+    <t>being revised</t>
+  </si>
+  <si>
+    <t>data received</t>
+  </si>
+  <si>
+    <t>on-going (1)</t>
+  </si>
+  <si>
+    <t>on-going (2)</t>
+  </si>
+  <si>
+    <t>preparing…</t>
   </si>
 </sst>
 </file>
@@ -7627,11 +7645,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BEEE373-47BE-6F4C-8F66-ACD6798C647F}">
   <dimension ref="A1:AJ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="110" workbookViewId="0">
       <pane xSplit="24" ySplit="17" topLeftCell="Y18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="T1" sqref="T1"/>
       <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomRight" activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7750,7 +7768,9 @@
       <c r="I2" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="J2" s="55"/>
+      <c r="J2" s="54" t="s">
+        <v>399</v>
+      </c>
       <c r="K2" s="55"/>
       <c r="L2" s="48"/>
       <c r="M2" s="48"/>
@@ -7802,7 +7822,9 @@
       <c r="I3" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="J3" s="55"/>
+      <c r="J3" s="54" t="s">
+        <v>399</v>
+      </c>
       <c r="K3" s="55"/>
       <c r="L3" s="48"/>
       <c r="M3" s="48"/>
@@ -7851,10 +7873,12 @@
       <c r="H4" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="I4" s="54" t="s">
-        <v>356</v>
-      </c>
-      <c r="J4" s="55"/>
+      <c r="I4" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="J4" s="54" t="s">
+        <v>399</v>
+      </c>
       <c r="K4" s="55"/>
       <c r="L4" s="48"/>
       <c r="M4" s="48"/>
@@ -7894,7 +7918,9 @@
       <c r="E5" s="57" t="s">
         <v>358</v>
       </c>
-      <c r="F5" s="58"/>
+      <c r="F5" s="56" t="s">
+        <v>399</v>
+      </c>
       <c r="G5" s="55"/>
       <c r="H5" s="55"/>
       <c r="I5" s="55"/>
@@ -7941,16 +7967,18 @@
       <c r="F6" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="G6" s="56" t="s">
-        <v>349</v>
-      </c>
-      <c r="H6" s="53" t="s">
-        <v>348</v>
-      </c>
-      <c r="I6" s="53" t="s">
-        <v>348</v>
-      </c>
-      <c r="J6" s="55"/>
+      <c r="G6" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="H6" s="56" t="s">
+        <v>400</v>
+      </c>
+      <c r="I6" s="56" t="s">
+        <v>400</v>
+      </c>
+      <c r="J6" s="54" t="s">
+        <v>399</v>
+      </c>
       <c r="K6" s="55"/>
       <c r="L6" s="48"/>
       <c r="M6" s="48"/>
@@ -7990,12 +8018,18 @@
       <c r="E7" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="F7" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
+      <c r="F7" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="G7" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="H7" s="56" t="s">
+        <v>356</v>
+      </c>
+      <c r="I7" s="56" t="s">
+        <v>356</v>
+      </c>
       <c r="J7" s="55"/>
       <c r="K7" s="55"/>
       <c r="L7" s="48"/>
@@ -8036,12 +8070,18 @@
       <c r="E8" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="F8" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
+      <c r="F8" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="G8" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="H8" s="56" t="s">
+        <v>356</v>
+      </c>
+      <c r="I8" s="56" t="s">
+        <v>356</v>
+      </c>
       <c r="J8" s="55"/>
       <c r="K8" s="55"/>
       <c r="L8" s="48"/>
@@ -8278,10 +8318,12 @@
       <c r="I13" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="J13" s="56" t="s">
-        <v>349</v>
-      </c>
-      <c r="K13" s="55"/>
+      <c r="J13" s="53" t="s">
+        <v>355</v>
+      </c>
+      <c r="K13" s="56" t="s">
+        <v>403</v>
+      </c>
       <c r="L13" s="48"/>
       <c r="M13" s="48"/>
       <c r="N13" s="48"/>
@@ -8523,10 +8565,12 @@
       <c r="H18" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="I18" s="54" t="s">
-        <v>356</v>
-      </c>
-      <c r="J18" s="55"/>
+      <c r="I18" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="J18" s="56" t="s">
+        <v>404</v>
+      </c>
       <c r="K18" s="55"/>
       <c r="L18" s="48"/>
       <c r="M18" s="48"/>
@@ -8582,7 +8626,7 @@
         <v>355</v>
       </c>
       <c r="K19" s="56" t="s">
-        <v>349</v>
+        <v>402</v>
       </c>
       <c r="L19" s="48"/>
       <c r="M19" s="48"/>
@@ -8622,12 +8666,18 @@
       <c r="E20" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="F20" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="G20" s="55"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="55"/>
+      <c r="F20" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="G20" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="H20" s="56" t="s">
+        <v>401</v>
+      </c>
+      <c r="I20" s="56" t="s">
+        <v>401</v>
+      </c>
       <c r="J20" s="55"/>
       <c r="K20" s="55"/>
       <c r="L20" s="48"/>
@@ -8671,11 +8721,15 @@
       <c r="F21" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="G21" s="56" t="s">
-        <v>349</v>
-      </c>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
+      <c r="G21" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="H21" s="54" t="s">
+        <v>356</v>
+      </c>
+      <c r="I21" s="54" t="s">
+        <v>356</v>
+      </c>
       <c r="J21" s="55"/>
       <c r="K21" s="55"/>
       <c r="L21" s="48"/>
@@ -8719,11 +8773,15 @@
       <c r="F22" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="G22" s="56" t="s">
-        <v>349</v>
-      </c>
-      <c r="H22" s="55"/>
-      <c r="I22" s="55"/>
+      <c r="G22" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="H22" s="54" t="s">
+        <v>356</v>
+      </c>
+      <c r="I22" s="54" t="s">
+        <v>356</v>
+      </c>
       <c r="J22" s="55"/>
       <c r="K22" s="55"/>
       <c r="L22" s="48"/>

</xml_diff>

<commit_message>
provided country-specific examples to the HBSC Preamble of en-NG
</commit_message>
<xml_diff>
--- a/GACPAQ pages.xlsx
+++ b/GACPAQ pages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doncastillo/Code/gacpaq/gacpaq-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41CE2385-7994-234B-9255-B0EFBD509297}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4AFB32-2F96-C24A-804E-2272F88B449F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19900" yWindow="-19140" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
+    <workbookView xWindow="25400" yWindow="-19820" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="399">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="405">
   <si>
     <t>Page Number</t>
   </si>
@@ -2704,6 +2704,24 @@
   </si>
   <si>
     <t>ok</t>
+  </si>
+  <si>
+    <t>in review</t>
+  </si>
+  <si>
+    <t>being revised</t>
+  </si>
+  <si>
+    <t>data received</t>
+  </si>
+  <si>
+    <t>on-going (1)</t>
+  </si>
+  <si>
+    <t>on-going (2)</t>
+  </si>
+  <si>
+    <t>on-going (3)</t>
   </si>
 </sst>
 </file>
@@ -7627,11 +7645,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BEEE373-47BE-6F4C-8F66-ACD6798C647F}">
   <dimension ref="A1:AJ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="24" ySplit="17" topLeftCell="Y18" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T1" sqref="T1"/>
-      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7750,7 +7768,9 @@
       <c r="I2" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="J2" s="55"/>
+      <c r="J2" s="54" t="s">
+        <v>399</v>
+      </c>
       <c r="K2" s="55"/>
       <c r="L2" s="48"/>
       <c r="M2" s="48"/>
@@ -7802,7 +7822,9 @@
       <c r="I3" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="J3" s="55"/>
+      <c r="J3" s="54" t="s">
+        <v>399</v>
+      </c>
       <c r="K3" s="55"/>
       <c r="L3" s="48"/>
       <c r="M3" s="48"/>
@@ -7851,10 +7873,12 @@
       <c r="H4" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="I4" s="54" t="s">
-        <v>356</v>
-      </c>
-      <c r="J4" s="55"/>
+      <c r="I4" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="J4" s="54" t="s">
+        <v>399</v>
+      </c>
       <c r="K4" s="55"/>
       <c r="L4" s="48"/>
       <c r="M4" s="48"/>
@@ -7894,7 +7918,9 @@
       <c r="E5" s="57" t="s">
         <v>358</v>
       </c>
-      <c r="F5" s="58"/>
+      <c r="F5" s="56" t="s">
+        <v>399</v>
+      </c>
       <c r="G5" s="55"/>
       <c r="H5" s="55"/>
       <c r="I5" s="55"/>
@@ -7941,16 +7967,18 @@
       <c r="F6" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="G6" s="56" t="s">
-        <v>349</v>
-      </c>
-      <c r="H6" s="53" t="s">
-        <v>348</v>
-      </c>
-      <c r="I6" s="53" t="s">
-        <v>348</v>
-      </c>
-      <c r="J6" s="55"/>
+      <c r="G6" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="H6" s="56" t="s">
+        <v>400</v>
+      </c>
+      <c r="I6" s="56" t="s">
+        <v>400</v>
+      </c>
+      <c r="J6" s="54" t="s">
+        <v>399</v>
+      </c>
       <c r="K6" s="55"/>
       <c r="L6" s="48"/>
       <c r="M6" s="48"/>
@@ -7990,12 +8018,18 @@
       <c r="E7" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="F7" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="G7" s="55"/>
-      <c r="H7" s="55"/>
-      <c r="I7" s="55"/>
+      <c r="F7" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="G7" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="H7" s="56" t="s">
+        <v>356</v>
+      </c>
+      <c r="I7" s="56" t="s">
+        <v>356</v>
+      </c>
       <c r="J7" s="55"/>
       <c r="K7" s="55"/>
       <c r="L7" s="48"/>
@@ -8036,12 +8070,18 @@
       <c r="E8" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="F8" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="G8" s="55"/>
-      <c r="H8" s="55"/>
-      <c r="I8" s="55"/>
+      <c r="F8" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="G8" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="H8" s="56" t="s">
+        <v>356</v>
+      </c>
+      <c r="I8" s="56" t="s">
+        <v>356</v>
+      </c>
       <c r="J8" s="55"/>
       <c r="K8" s="55"/>
       <c r="L8" s="48"/>
@@ -8278,10 +8318,12 @@
       <c r="I13" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="J13" s="56" t="s">
-        <v>349</v>
-      </c>
-      <c r="K13" s="55"/>
+      <c r="J13" s="53" t="s">
+        <v>355</v>
+      </c>
+      <c r="K13" s="56" t="s">
+        <v>403</v>
+      </c>
       <c r="L13" s="48"/>
       <c r="M13" s="48"/>
       <c r="N13" s="48"/>
@@ -8446,7 +8488,7 @@
       <c r="AE16" s="48"/>
       <c r="AF16" s="48"/>
     </row>
-    <row r="17" spans="1:32" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:32" ht="35" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="40" t="s">
         <v>308</v>
       </c>
@@ -8469,10 +8511,10 @@
         <v>348</v>
       </c>
       <c r="H17" s="54" t="s">
-        <v>356</v>
+        <v>401</v>
       </c>
       <c r="I17" s="54" t="s">
-        <v>356</v>
+        <v>401</v>
       </c>
       <c r="J17" s="55"/>
       <c r="K17" s="55"/>
@@ -8523,11 +8565,15 @@
       <c r="H18" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="I18" s="54" t="s">
-        <v>356</v>
-      </c>
-      <c r="J18" s="55"/>
-      <c r="K18" s="55"/>
+      <c r="I18" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="J18" s="53" t="s">
+        <v>355</v>
+      </c>
+      <c r="K18" s="54" t="s">
+        <v>404</v>
+      </c>
       <c r="L18" s="48"/>
       <c r="M18" s="48"/>
       <c r="N18" s="48"/>
@@ -8582,7 +8628,7 @@
         <v>355</v>
       </c>
       <c r="K19" s="56" t="s">
-        <v>349</v>
+        <v>402</v>
       </c>
       <c r="L19" s="48"/>
       <c r="M19" s="48"/>
@@ -8622,12 +8668,18 @@
       <c r="E20" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="F20" s="57" t="s">
-        <v>357</v>
-      </c>
-      <c r="G20" s="55"/>
-      <c r="H20" s="55"/>
-      <c r="I20" s="55"/>
+      <c r="F20" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="G20" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="H20" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="I20" s="53" t="s">
+        <v>348</v>
+      </c>
       <c r="J20" s="55"/>
       <c r="K20" s="55"/>
       <c r="L20" s="48"/>
@@ -8671,11 +8723,15 @@
       <c r="F21" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="G21" s="56" t="s">
-        <v>349</v>
-      </c>
-      <c r="H21" s="55"/>
-      <c r="I21" s="55"/>
+      <c r="G21" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="H21" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="I21" s="53" t="s">
+        <v>348</v>
+      </c>
       <c r="J21" s="55"/>
       <c r="K21" s="55"/>
       <c r="L21" s="48"/>
@@ -8719,11 +8775,15 @@
       <c r="F22" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="G22" s="56" t="s">
-        <v>349</v>
-      </c>
-      <c r="H22" s="55"/>
-      <c r="I22" s="55"/>
+      <c r="G22" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="H22" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="I22" s="53" t="s">
+        <v>348</v>
+      </c>
       <c r="J22" s="55"/>
       <c r="K22" s="55"/>
       <c r="L22" s="48"/>

</xml_diff>

<commit_message>
provided country-specific examples to the GSHS pages of en-NG
</commit_message>
<xml_diff>
--- a/GACPAQ pages.xlsx
+++ b/GACPAQ pages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doncastillo/Code/gacpaq/gacpaq-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4AFB32-2F96-C24A-804E-2272F88B449F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D331A33F-8B7E-DF4F-8D2A-43B10BD9FAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25400" yWindow="-19820" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
   </bookViews>
@@ -7649,7 +7649,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomRight" activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8444,7 +8444,7 @@
       <c r="AE15" s="48"/>
       <c r="AF15" s="48"/>
     </row>
-    <row r="16" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" ht="26" x14ac:dyDescent="0.2">
       <c r="A16" s="40" t="s">
         <v>306</v>
       </c>
@@ -8488,7 +8488,7 @@
       <c r="AE16" s="48"/>
       <c r="AF16" s="48"/>
     </row>
-    <row r="17" spans="1:32" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:32" ht="31" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="40" t="s">
         <v>308</v>
       </c>
@@ -8510,8 +8510,8 @@
       <c r="G17" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="H17" s="54" t="s">
-        <v>401</v>
+      <c r="H17" s="53" t="s">
+        <v>348</v>
       </c>
       <c r="I17" s="54" t="s">
         <v>401</v>

</xml_diff>

<commit_message>
updated GAC-PAQ excel sheet
</commit_message>
<xml_diff>
--- a/GACPAQ pages.xlsx
+++ b/GACPAQ pages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doncastillo/Code/gacpaq/gacpaq-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D331A33F-8B7E-DF4F-8D2A-43B10BD9FAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7952C9E5-C64A-C24E-986A-AA07C9C0C991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25400" yWindow="-19820" windowWidth="38400" windowHeight="21100" activeTab="6" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="788" uniqueCount="405">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="404">
   <si>
     <t>Page Number</t>
   </si>
@@ -2710,9 +2710,6 @@
   </si>
   <si>
     <t>being revised</t>
-  </si>
-  <si>
-    <t>data received</t>
   </si>
   <si>
     <t>on-going (1)</t>
@@ -7645,11 +7642,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BEEE373-47BE-6F4C-8F66-ACD6798C647F}">
   <dimension ref="A1:AJ22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="114" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="114" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A17" sqref="A17:XFD17"/>
+      <selection pane="bottomRight" activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8322,7 +8319,7 @@
         <v>355</v>
       </c>
       <c r="K13" s="56" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="L13" s="48"/>
       <c r="M13" s="48"/>
@@ -8513,10 +8510,12 @@
       <c r="H17" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="I17" s="54" t="s">
-        <v>401</v>
-      </c>
-      <c r="J17" s="55"/>
+      <c r="I17" s="53" t="s">
+        <v>348</v>
+      </c>
+      <c r="J17" s="54" t="s">
+        <v>399</v>
+      </c>
       <c r="K17" s="55"/>
       <c r="L17" s="48"/>
       <c r="M17" s="48"/>
@@ -8572,7 +8571,7 @@
         <v>355</v>
       </c>
       <c r="K18" s="54" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="L18" s="48"/>
       <c r="M18" s="48"/>
@@ -8628,7 +8627,7 @@
         <v>355</v>
       </c>
       <c r="K19" s="56" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="L19" s="48"/>
       <c r="M19" s="48"/>
@@ -8680,7 +8679,9 @@
       <c r="I20" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="J20" s="55"/>
+      <c r="J20" s="54" t="s">
+        <v>399</v>
+      </c>
       <c r="K20" s="55"/>
       <c r="L20" s="48"/>
       <c r="M20" s="48"/>
@@ -8732,7 +8733,9 @@
       <c r="I21" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="J21" s="55"/>
+      <c r="J21" s="54" t="s">
+        <v>399</v>
+      </c>
       <c r="K21" s="55"/>
       <c r="L21" s="48"/>
       <c r="M21" s="48"/>
@@ -8784,7 +8787,9 @@
       <c r="I22" s="53" t="s">
         <v>348</v>
       </c>
-      <c r="J22" s="55"/>
+      <c r="J22" s="54" t="s">
+        <v>399</v>
+      </c>
       <c r="K22" s="55"/>
       <c r="L22" s="48"/>
       <c r="M22" s="48"/>

</xml_diff>

<commit_message>
Added countries to the main study lang; updated GACPAQ pages excel
</commit_message>
<xml_diff>
--- a/GACPAQ pages.xlsx
+++ b/GACPAQ pages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doncastillo/Code/gacpaq/gacpaq-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C287C6-967A-534F-A236-2070DD0C44A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E31E7DC-67C8-4A4E-A693-2A4B0B9EC4E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32960" yWindow="-4420" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
+    <workbookView xWindow="33360" yWindow="-20780" windowWidth="14660" windowHeight="21100" activeTab="5" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="401">
   <si>
     <t>Page Number</t>
   </si>
@@ -2697,6 +2697,18 @@
   </si>
   <si>
     <t>on-going (6)</t>
+  </si>
+  <si>
+    <t>on-going (7)</t>
+  </si>
+  <si>
+    <t>on-going (8)</t>
+  </si>
+  <si>
+    <t>on-going (9)</t>
+  </si>
+  <si>
+    <t>on-going (10)</t>
   </si>
 </sst>
 </file>
@@ -7528,7 +7540,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L8" sqref="L8"/>
+      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7869,10 +7881,12 @@
       <c r="I6" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="J6" s="54" t="s">
-        <v>389</v>
-      </c>
-      <c r="K6" s="55"/>
+      <c r="J6" s="53" t="s">
+        <v>345</v>
+      </c>
+      <c r="K6" s="56" t="s">
+        <v>397</v>
+      </c>
       <c r="L6" s="40" t="s">
         <v>276</v>
       </c>
@@ -7925,10 +7939,12 @@
       <c r="I7" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="J7" s="54" t="s">
-        <v>389</v>
-      </c>
-      <c r="K7" s="55"/>
+      <c r="J7" s="53" t="s">
+        <v>345</v>
+      </c>
+      <c r="K7" s="56" t="s">
+        <v>398</v>
+      </c>
       <c r="L7" s="40" t="s">
         <v>278</v>
       </c>
@@ -8125,8 +8141,12 @@
       <c r="G11" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="H11" s="55"/>
-      <c r="I11" s="55"/>
+      <c r="H11" s="56" t="s">
+        <v>346</v>
+      </c>
+      <c r="I11" s="56" t="s">
+        <v>346</v>
+      </c>
       <c r="J11" s="55"/>
       <c r="K11" s="55"/>
       <c r="L11" s="40" t="s">
@@ -8175,8 +8195,12 @@
       <c r="G12" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="H12" s="55"/>
-      <c r="I12" s="55"/>
+      <c r="H12" s="56" t="s">
+        <v>346</v>
+      </c>
+      <c r="I12" s="56" t="s">
+        <v>346</v>
+      </c>
       <c r="J12" s="55"/>
       <c r="K12" s="55"/>
       <c r="L12" s="40" t="s">
@@ -8289,10 +8313,12 @@
       <c r="I14" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="J14" s="54" t="s">
-        <v>389</v>
-      </c>
-      <c r="K14" s="55"/>
+      <c r="J14" s="53" t="s">
+        <v>345</v>
+      </c>
+      <c r="K14" s="56" t="s">
+        <v>396</v>
+      </c>
       <c r="L14" s="40" t="s">
         <v>292</v>
       </c>
@@ -8613,10 +8639,12 @@
       <c r="I20" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="J20" s="54" t="s">
-        <v>389</v>
-      </c>
-      <c r="K20" s="55"/>
+      <c r="J20" s="53" t="s">
+        <v>345</v>
+      </c>
+      <c r="K20" s="56" t="s">
+        <v>400</v>
+      </c>
       <c r="L20" s="40" t="s">
         <v>304</v>
       </c>
@@ -8669,10 +8697,12 @@
       <c r="I21" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="J21" s="54" t="s">
-        <v>389</v>
-      </c>
-      <c r="K21" s="55"/>
+      <c r="J21" s="53" t="s">
+        <v>345</v>
+      </c>
+      <c r="K21" s="56" t="s">
+        <v>399</v>
+      </c>
       <c r="L21" s="40" t="s">
         <v>306</v>
       </c>
@@ -8725,10 +8755,12 @@
       <c r="I22" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="J22" s="54" t="s">
-        <v>389</v>
-      </c>
-      <c r="K22" s="55"/>
+      <c r="J22" s="53" t="s">
+        <v>345</v>
+      </c>
+      <c r="K22" s="56" t="s">
+        <v>399</v>
+      </c>
       <c r="L22" s="40" t="s">
         <v>308</v>
       </c>

</xml_diff>

<commit_message>
added ch-MW translations of the HBSC and GSHS pages
</commit_message>
<xml_diff>
--- a/GACPAQ pages.xlsx
+++ b/GACPAQ pages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doncastillo/Code/gacpaq/gacpaq-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E31E7DC-67C8-4A4E-A693-2A4B0B9EC4E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E649D3-FDB7-F647-9730-86B3E67C44DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33360" yWindow="-20780" windowWidth="14660" windowHeight="21100" activeTab="5" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
+    <workbookView xWindow="-20140" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Participant Responses - 120824" sheetId="5" r:id="rId4"/>
     <sheet name="Images" sheetId="4" r:id="rId5"/>
     <sheet name="Country Status" sheetId="8" r:id="rId6"/>
+    <sheet name="Submission Page" sheetId="11" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_Hlk120517734" localSheetId="1">'Section Pages'!$J$26</definedName>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="419">
   <si>
     <t>Page Number</t>
   </si>
@@ -2525,9 +2526,6 @@
     <t>completed</t>
   </si>
   <si>
-    <t>on-going</t>
-  </si>
-  <si>
     <t>Narration entered</t>
   </si>
   <si>
@@ -2709,13 +2707,178 @@
   </si>
   <si>
     <t>on-going (10)</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>No pending submissions</t>
+  </si>
+  <si>
+    <t>Nothing to submit</t>
+  </si>
+  <si>
+    <t>Pending Submissions</t>
+  </si>
+  <si>
+    <t>Responses submitted</t>
+  </si>
+  <si>
+    <t>बुझाउनुहोस्</t>
+  </si>
+  <si>
+    <t>बुझाउनु पर्ने केहि बाँकी छैन</t>
+  </si>
+  <si>
+    <r>
+      <t>बुझाउनु</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Preeti"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>पर्ने</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Preeti"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>केहि</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Preeti"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>छैन</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>बुझाउन</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Preeti"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>बाँकी</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Preeti"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>छ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>प्रतिकृया</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Preeti"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">बुझाइयो </t>
+    </r>
+  </si>
+  <si>
+    <t>Enviar</t>
+  </si>
+  <si>
+    <t>No hay envíos pendientes</t>
+  </si>
+  <si>
+    <t>No hay nada para enviar</t>
+  </si>
+  <si>
+    <t>Envíos pendientes</t>
+  </si>
+  <si>
+    <t>Respuestas enviadas</t>
+  </si>
+  <si>
+    <t>Nenhuma submissão pendente</t>
+  </si>
+  <si>
+    <t>Nada a enviar</t>
+  </si>
+  <si>
+    <t>Submissões pendentes</t>
+  </si>
+  <si>
+    <t>Respostas enviadas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="27">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2887,8 +3050,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF212121"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Preeti"/>
+    </font>
   </fonts>
-  <fills count="23">
+  <fills count="24">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3021,6 +3209,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -3106,7 +3300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3279,6 +3473,28 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3600,7 +3816,7 @@
       <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.5" style="1" customWidth="1"/>
@@ -3611,7 +3827,7 @@
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="19">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -3640,7 +3856,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -3663,7 +3879,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -3686,7 +3902,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -3709,7 +3925,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -3729,7 +3945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -3747,7 +3963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -3770,7 +3986,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -3793,7 +4009,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="8" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" s="8" customFormat="1">
       <c r="A9" s="7">
         <v>8</v>
       </c>
@@ -3813,7 +4029,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -3831,7 +4047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -3849,7 +4065,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -3867,7 +4083,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -3885,7 +4101,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -3903,7 +4119,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -3921,7 +4137,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -3939,7 +4155,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -3957,7 +4173,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6">
       <c r="A18" s="5">
         <v>17</v>
       </c>
@@ -3975,7 +4191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -3993,7 +4209,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -4011,7 +4227,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -4029,7 +4245,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -4047,7 +4263,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -4065,7 +4281,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6">
       <c r="A24" s="6">
         <v>23</v>
       </c>
@@ -4083,7 +4299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6">
       <c r="A25" s="6">
         <v>24</v>
       </c>
@@ -4101,7 +4317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6">
       <c r="A26" s="6">
         <v>25</v>
       </c>
@@ -4136,7 +4352,7 @@
       <selection pane="bottomRight" activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="20.6640625" style="14" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" style="13" bestFit="1" customWidth="1"/>
@@ -4151,7 +4367,7 @@
     <col min="12" max="16384" width="10.83203125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="17">
       <c r="C1" s="13" t="s">
         <v>110</v>
       </c>
@@ -4180,7 +4396,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11">
       <c r="A2" s="33" t="s">
         <v>102</v>
       </c>
@@ -4192,7 +4408,7 @@
       </c>
       <c r="K2" s="10"/>
     </row>
-    <row r="3" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="15" customHeight="1">
       <c r="A3" s="33" t="s">
         <v>102</v>
       </c>
@@ -4204,7 +4420,7 @@
       </c>
       <c r="K3" s="10"/>
     </row>
-    <row r="4" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="15" customHeight="1">
       <c r="A4" s="33" t="s">
         <v>102</v>
       </c>
@@ -4216,7 +4432,7 @@
       </c>
       <c r="K4" s="10"/>
     </row>
-    <row r="5" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="15" customHeight="1">
       <c r="A5" s="33" t="s">
         <v>102</v>
       </c>
@@ -4233,7 +4449,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="15" customHeight="1">
       <c r="A6" s="33" t="s">
         <v>102</v>
       </c>
@@ -4251,7 +4467,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="17" customHeight="1">
       <c r="A7" s="15" t="s">
         <v>24</v>
       </c>
@@ -4271,7 +4487,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="17" customHeight="1">
       <c r="A8" s="15" t="s">
         <v>24</v>
       </c>
@@ -4292,7 +4508,7 @@
       </c>
       <c r="K8" s="10"/>
     </row>
-    <row r="9" spans="1:11" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="22" customHeight="1">
       <c r="A9" s="15" t="s">
         <v>24</v>
       </c>
@@ -4324,7 +4540,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="17">
       <c r="A10" s="15" t="s">
         <v>24</v>
       </c>
@@ -4350,7 +4566,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="34">
       <c r="A11" s="15" t="s">
         <v>24</v>
       </c>
@@ -4379,7 +4595,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="17">
       <c r="A12" s="15" t="s">
         <v>24</v>
       </c>
@@ -4405,7 +4621,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="34">
       <c r="A13" s="15" t="s">
         <v>24</v>
       </c>
@@ -4431,7 +4647,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="68" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="68">
       <c r="A14" s="15" t="s">
         <v>24</v>
       </c>
@@ -4457,7 +4673,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="34">
       <c r="A15" s="15" t="s">
         <v>24</v>
       </c>
@@ -4483,7 +4699,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11">
       <c r="A16" s="15" t="s">
         <v>24</v>
       </c>
@@ -4504,7 +4720,7 @@
       </c>
       <c r="K16" s="11"/>
     </row>
-    <row r="17" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="17" customHeight="1">
       <c r="A17" s="16" t="s">
         <v>29</v>
       </c>
@@ -4525,7 +4741,7 @@
       </c>
       <c r="K17" s="11"/>
     </row>
-    <row r="18" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="17" customHeight="1">
       <c r="A18" s="16" t="s">
         <v>29</v>
       </c>
@@ -4546,7 +4762,7 @@
       </c>
       <c r="K18" s="11"/>
     </row>
-    <row r="19" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="17" customHeight="1">
       <c r="A19" s="16" t="s">
         <v>29</v>
       </c>
@@ -4575,7 +4791,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="17">
       <c r="A20" s="16" t="s">
         <v>29</v>
       </c>
@@ -4601,7 +4817,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="34">
       <c r="A21" s="16" t="s">
         <v>29</v>
       </c>
@@ -4627,7 +4843,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="34">
       <c r="A22" s="16" t="s">
         <v>29</v>
       </c>
@@ -4653,7 +4869,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11">
       <c r="A23" s="16" t="s">
         <v>29</v>
       </c>
@@ -4674,7 +4890,7 @@
       </c>
       <c r="K23" s="11"/>
     </row>
-    <row r="24" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="35" customHeight="1">
       <c r="A24" s="17" t="s">
         <v>36</v>
       </c>
@@ -4698,7 +4914,7 @@
       </c>
       <c r="K24" s="11"/>
     </row>
-    <row r="25" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="35" customHeight="1">
       <c r="A25" s="17" t="s">
         <v>36</v>
       </c>
@@ -4720,7 +4936,7 @@
       <c r="I25" s="26"/>
       <c r="K25" s="11"/>
     </row>
-    <row r="26" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="35" customHeight="1">
       <c r="A26" s="17" t="s">
         <v>36</v>
       </c>
@@ -4749,7 +4965,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="35" customHeight="1">
       <c r="A27" s="17" t="s">
         <v>36</v>
       </c>
@@ -4778,7 +4994,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="35" customHeight="1">
       <c r="A28" s="17" t="s">
         <v>36</v>
       </c>
@@ -4807,7 +5023,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="35" customHeight="1">
       <c r="A29" s="17" t="s">
         <v>36</v>
       </c>
@@ -4831,7 +5047,7 @@
       </c>
       <c r="K29" s="11"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11">
       <c r="A30" s="18" t="s">
         <v>46</v>
       </c>
@@ -4852,7 +5068,7 @@
       </c>
       <c r="K30" s="11"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11">
       <c r="A31" s="18" t="s">
         <v>46</v>
       </c>
@@ -4873,7 +5089,7 @@
       </c>
       <c r="K31" s="11"/>
     </row>
-    <row r="32" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="34">
       <c r="A32" s="18" t="s">
         <v>46</v>
       </c>
@@ -4904,7 +5120,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="17">
       <c r="A33" s="18" t="s">
         <v>46</v>
       </c>
@@ -4935,7 +5151,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="17">
       <c r="A34" s="18" t="s">
         <v>46</v>
       </c>
@@ -4966,7 +5182,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="34">
       <c r="A35" s="18" t="s">
         <v>46</v>
       </c>
@@ -4997,7 +5213,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="17">
       <c r="A36" s="18" t="s">
         <v>46</v>
       </c>
@@ -5028,7 +5244,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="17">
       <c r="A37" s="18" t="s">
         <v>46</v>
       </c>
@@ -5059,7 +5275,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="51">
       <c r="A38" s="18" t="s">
         <v>46</v>
       </c>
@@ -5087,7 +5303,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="34">
       <c r="A39" s="18" t="s">
         <v>46</v>
       </c>
@@ -5115,7 +5331,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="34">
       <c r="A40" s="18" t="s">
         <v>46</v>
       </c>
@@ -5143,7 +5359,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="34">
       <c r="A41" s="18" t="s">
         <v>46</v>
       </c>
@@ -5171,7 +5387,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="34">
       <c r="A42" s="18" t="s">
         <v>46</v>
       </c>
@@ -5199,7 +5415,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11">
       <c r="A43" s="18" t="s">
         <v>46</v>
       </c>
@@ -5220,7 +5436,7 @@
       </c>
       <c r="K43" s="11"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11">
       <c r="A44" s="19" t="s">
         <v>47</v>
       </c>
@@ -5241,7 +5457,7 @@
       </c>
       <c r="K44" s="11"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11">
       <c r="A45" s="19" t="s">
         <v>47</v>
       </c>
@@ -5262,7 +5478,7 @@
       </c>
       <c r="K45" s="11"/>
     </row>
-    <row r="46" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="17">
       <c r="A46" s="19" t="s">
         <v>47</v>
       </c>
@@ -5291,7 +5507,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" ht="34">
       <c r="A47" s="19" t="s">
         <v>47</v>
       </c>
@@ -5317,7 +5533,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="34">
       <c r="A48" s="19" t="s">
         <v>47</v>
       </c>
@@ -5343,7 +5559,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11">
       <c r="A49" s="19" t="s">
         <v>47</v>
       </c>
@@ -5364,7 +5580,7 @@
       </c>
       <c r="K49" s="11"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11">
       <c r="A50" s="20" t="s">
         <v>48</v>
       </c>
@@ -5385,7 +5601,7 @@
       </c>
       <c r="K50" s="11"/>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11">
       <c r="A51" s="20" t="s">
         <v>48</v>
       </c>
@@ -5406,7 +5622,7 @@
       </c>
       <c r="K51" s="11"/>
     </row>
-    <row r="52" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" ht="34">
       <c r="A52" s="20" t="s">
         <v>48</v>
       </c>
@@ -5432,7 +5648,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="34">
       <c r="A53" s="20" t="s">
         <v>48</v>
       </c>
@@ -5458,7 +5674,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11">
       <c r="A54" s="20" t="s">
         <v>48</v>
       </c>
@@ -5479,7 +5695,7 @@
       </c>
       <c r="K54" s="11"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11">
       <c r="A55" s="21" t="s">
         <v>49</v>
       </c>
@@ -5500,7 +5716,7 @@
       </c>
       <c r="K55" s="11"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11">
       <c r="A56" s="21" t="s">
         <v>49</v>
       </c>
@@ -5521,7 +5737,7 @@
       </c>
       <c r="K56" s="11"/>
     </row>
-    <row r="57" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" ht="34">
       <c r="A57" s="21" t="s">
         <v>49</v>
       </c>
@@ -5547,7 +5763,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11">
       <c r="A58" s="21" t="s">
         <v>49</v>
       </c>
@@ -5568,7 +5784,7 @@
       </c>
       <c r="K58" s="11"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11">
       <c r="A59" s="22" t="s">
         <v>51</v>
       </c>
@@ -5577,7 +5793,7 @@
       </c>
       <c r="K59" s="11"/>
     </row>
-    <row r="60" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" ht="17" customHeight="1">
       <c r="A60" s="22" t="s">
         <v>51</v>
       </c>
@@ -5594,7 +5810,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" ht="32">
       <c r="A61" s="22" t="s">
         <v>51</v>
       </c>
@@ -5609,7 +5825,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11">
       <c r="A62" s="22" t="s">
         <v>51</v>
       </c>
@@ -5624,7 +5840,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11">
       <c r="A63" s="22" t="s">
         <v>51</v>
       </c>
@@ -5639,7 +5855,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11">
       <c r="A64" s="22" t="s">
         <v>51</v>
       </c>
@@ -5654,7 +5870,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" ht="32">
       <c r="A65" s="22" t="s">
         <v>51</v>
       </c>
@@ -5669,7 +5885,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11">
       <c r="A66" s="22"/>
       <c r="B66" s="13">
         <v>30</v>
@@ -5678,7 +5894,7 @@
       <c r="G66" s="35"/>
       <c r="K66" s="11"/>
     </row>
-    <row r="67" spans="1:11" ht="32" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" ht="32">
       <c r="A67" s="22" t="s">
         <v>51</v>
       </c>
@@ -5693,7 +5909,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11">
       <c r="A68" s="24" t="s">
         <v>149</v>
       </c>
@@ -5701,7 +5917,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" ht="34">
       <c r="A69" s="61" t="s">
         <v>149</v>
       </c>
@@ -5719,7 +5935,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" ht="51">
       <c r="A70" s="61" t="s">
         <v>149</v>
       </c>
@@ -5736,7 +5952,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11">
       <c r="A71" s="24" t="s">
         <v>149</v>
       </c>
@@ -5744,7 +5960,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11">
       <c r="A72" s="18" t="s">
         <v>332</v>
       </c>
@@ -5752,13 +5968,13 @@
         <v>102</v>
       </c>
       <c r="F72" s="13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11">
       <c r="A73" s="18" t="s">
         <v>332</v>
       </c>
@@ -5766,13 +5982,13 @@
         <v>216</v>
       </c>
       <c r="F73" s="13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11">
       <c r="A74" s="18" t="s">
         <v>332</v>
       </c>
@@ -5780,13 +5996,13 @@
         <v>25</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H74" s="13" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11">
       <c r="A75" s="18" t="s">
         <v>332</v>
       </c>
@@ -5794,13 +6010,13 @@
         <v>26</v>
       </c>
       <c r="F75" s="13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H75" s="13" t="s">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11">
       <c r="A76" s="18" t="s">
         <v>332</v>
       </c>
@@ -5808,13 +6024,13 @@
         <v>51</v>
       </c>
       <c r="F76" s="13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H76" s="13" t="s">
-        <v>372</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11">
       <c r="A77" s="62" t="s">
         <v>333</v>
       </c>
@@ -5822,27 +6038,27 @@
         <v>102</v>
       </c>
       <c r="F77" s="13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H77" s="13" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11">
       <c r="A78" s="62" t="s">
         <v>333</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F78" s="13" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H78" s="13" t="s">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11">
       <c r="A79" s="62" t="s">
         <v>333</v>
       </c>
@@ -5850,13 +6066,13 @@
         <v>25</v>
       </c>
       <c r="F79" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H79" s="13" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11">
       <c r="A80" s="62" t="s">
         <v>333</v>
       </c>
@@ -5864,13 +6080,13 @@
         <v>26</v>
       </c>
       <c r="F80" s="13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" ht="17" customHeight="1">
       <c r="A81" s="62" t="s">
         <v>333</v>
       </c>
@@ -5878,13 +6094,13 @@
         <v>27</v>
       </c>
       <c r="F81" s="13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H81" s="13" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8">
       <c r="A82" s="62" t="s">
         <v>333</v>
       </c>
@@ -5892,27 +6108,27 @@
         <v>28</v>
       </c>
       <c r="F82" s="13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H82" s="63" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8">
       <c r="A83" s="62" t="s">
         <v>333</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F83" s="13" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H83" s="13" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8">
       <c r="A84" s="62" t="s">
         <v>333</v>
       </c>
@@ -5920,27 +6136,27 @@
         <v>29</v>
       </c>
       <c r="F84" s="13" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>380</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8">
       <c r="A85" s="62" t="s">
         <v>333</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F85" s="13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8">
       <c r="A86" s="62" t="s">
         <v>333</v>
       </c>
@@ -5948,13 +6164,13 @@
         <v>30</v>
       </c>
       <c r="F86" s="13" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H86" s="13" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8">
       <c r="A87" s="62" t="s">
         <v>333</v>
       </c>
@@ -5962,15 +6178,15 @@
         <v>51</v>
       </c>
       <c r="F87" s="13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H87" s="13" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8">
+      <c r="A88" s="21" t="s">
         <v>383</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A88" s="21" t="s">
-        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -5988,47 +6204,47 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="27.83203125" customWidth="1"/>
     <col min="2" max="2" width="4.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10">
       <c r="C2" t="s">
         <v>25</v>
       </c>
       <c r="D2" t="s">
+        <v>384</v>
+      </c>
+      <c r="E2" t="s">
         <v>385</v>
-      </c>
-      <c r="E2" t="s">
-        <v>386</v>
       </c>
       <c r="H2" t="s">
         <v>25</v>
       </c>
       <c r="I2" t="s">
+        <v>384</v>
+      </c>
+      <c r="J2" t="s">
         <v>385</v>
       </c>
-      <c r="J2" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:10">
       <c r="G3" t="s">
         <v>335</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J3" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="33" t="s">
         <v>102</v>
       </c>
@@ -6048,16 +6264,16 @@
         <v>334</v>
       </c>
       <c r="H4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I4" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J4" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="15" t="s">
         <v>24</v>
       </c>
@@ -6074,7 +6290,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10">
       <c r="A6" s="16" t="s">
         <v>29</v>
       </c>
@@ -6091,7 +6307,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10">
       <c r="A7" s="17" t="s">
         <v>36</v>
       </c>
@@ -6108,7 +6324,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10">
       <c r="A8" s="18" t="s">
         <v>46</v>
       </c>
@@ -6125,7 +6341,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10">
       <c r="A9" s="19" t="s">
         <v>47</v>
       </c>
@@ -6142,7 +6358,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10">
       <c r="A10" s="20" t="s">
         <v>48</v>
       </c>
@@ -6159,7 +6375,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="17" customHeight="1">
       <c r="A11" s="21" t="s">
         <v>49</v>
       </c>
@@ -6176,9 +6392,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10">
       <c r="A12" s="22" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B12" s="35">
         <v>8</v>
@@ -6193,7 +6409,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10">
       <c r="A13" s="61" t="s">
         <v>149</v>
       </c>
@@ -6208,7 +6424,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10">
       <c r="A14" s="18" t="s">
         <v>332</v>
       </c>
@@ -6219,7 +6435,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10">
       <c r="A15" s="62" t="s">
         <v>333</v>
       </c>
@@ -6230,9 +6446,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10">
       <c r="A16" s="21" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B16" s="35">
         <v>11</v>
@@ -6261,27 +6477,27 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="32" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="32" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="5" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="20" customHeight="1">
       <c r="A1" s="38"/>
       <c r="B1" s="46"/>
       <c r="C1" s="46"/>
       <c r="D1" s="46"/>
       <c r="E1" s="46"/>
     </row>
-    <row r="2" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="20" customHeight="1">
       <c r="A2" s="40"/>
       <c r="B2" s="46"/>
       <c r="C2" s="46"/>
       <c r="D2" s="46"/>
       <c r="E2" s="46"/>
     </row>
-    <row r="3" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="20" customHeight="1">
       <c r="A3" s="40"/>
       <c r="B3" s="46" t="s">
         <v>313</v>
@@ -6296,7 +6512,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="20" customHeight="1">
       <c r="A4" s="40" t="s">
         <v>317</v>
       </c>
@@ -6314,7 +6530,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="20" customHeight="1">
       <c r="A5" s="40" t="s">
         <v>318</v>
       </c>
@@ -6332,7 +6548,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="20" customHeight="1">
       <c r="A6" s="40" t="s">
         <v>319</v>
       </c>
@@ -6350,7 +6566,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="20" customHeight="1">
       <c r="A7" s="40" t="s">
         <v>320</v>
       </c>
@@ -6368,7 +6584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="20" customHeight="1">
       <c r="A8" s="40" t="s">
         <v>321</v>
       </c>
@@ -6386,7 +6602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="20" customHeight="1">
       <c r="A9" s="40" t="s">
         <v>322</v>
       </c>
@@ -6404,7 +6620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="20" customHeight="1">
       <c r="A10" s="40" t="s">
         <v>323</v>
       </c>
@@ -6422,7 +6638,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="20" customHeight="1">
       <c r="A11" s="40" t="s">
         <v>324</v>
       </c>
@@ -6440,7 +6656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="20" customHeight="1">
       <c r="A12" s="40" t="s">
         <v>325</v>
       </c>
@@ -6458,7 +6674,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="20" customHeight="1">
       <c r="A13" s="40" t="s">
         <v>326</v>
       </c>
@@ -6476,7 +6692,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="20" customHeight="1">
       <c r="A14" s="40" t="s">
         <v>327</v>
       </c>
@@ -6494,7 +6710,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="20" customHeight="1">
       <c r="A15" s="40" t="s">
         <v>328</v>
       </c>
@@ -6512,7 +6728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="20" customHeight="1">
       <c r="A16" s="40" t="s">
         <v>329</v>
       </c>
@@ -6530,7 +6746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="5:5" ht="35" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="5:5" ht="35" customHeight="1">
       <c r="E17" s="1">
         <f>SUM(E4:E16)</f>
         <v>351</v>
@@ -6553,7 +6769,7 @@
       <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="3" max="4" width="5.6640625" bestFit="1" customWidth="1"/>
@@ -6583,7 +6799,7 @@
     <col min="30" max="30" width="4.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="39" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" s="39" customFormat="1" ht="16" customHeight="1">
       <c r="A1" s="38"/>
       <c r="B1" s="38"/>
       <c r="C1" s="66" t="s">
@@ -6622,7 +6838,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="2" spans="1:31" s="39" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" s="39" customFormat="1" ht="16" customHeight="1">
       <c r="A2" s="40"/>
       <c r="B2" s="40"/>
       <c r="C2" s="40" t="s">
@@ -6678,7 +6894,7 @@
       <c r="AC2" s="70"/>
       <c r="AD2" s="70"/>
     </row>
-    <row r="3" spans="1:31" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" s="39" customFormat="1">
       <c r="A3" s="40"/>
       <c r="B3" s="40"/>
       <c r="C3" s="40"/>
@@ -6758,7 +6974,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31">
       <c r="A4" s="45" t="s">
         <v>269</v>
       </c>
@@ -6794,7 +7010,7 @@
       <c r="AC4" s="44"/>
       <c r="AD4" s="44"/>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31">
       <c r="A5" s="45" t="s">
         <v>271</v>
       </c>
@@ -6830,7 +7046,7 @@
       <c r="AC5" s="44"/>
       <c r="AD5" s="44"/>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31">
       <c r="A6" s="45" t="s">
         <v>273</v>
       </c>
@@ -6866,7 +7082,7 @@
       <c r="AC6" s="44"/>
       <c r="AD6" s="44"/>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31">
       <c r="A7" s="40" t="s">
         <v>275</v>
       </c>
@@ -6902,7 +7118,7 @@
       <c r="AC7" s="43"/>
       <c r="AD7" s="43"/>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31">
       <c r="A8" s="45" t="s">
         <v>276</v>
       </c>
@@ -6938,7 +7154,7 @@
       <c r="AC8" s="44"/>
       <c r="AD8" s="44"/>
     </row>
-    <row r="9" spans="1:31" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" ht="17" customHeight="1">
       <c r="A9" s="45" t="s">
         <v>278</v>
       </c>
@@ -6974,7 +7190,7 @@
       <c r="AC9" s="44"/>
       <c r="AD9" s="44"/>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31">
       <c r="A10" s="40" t="s">
         <v>280</v>
       </c>
@@ -7010,7 +7226,7 @@
       <c r="AC10" s="43"/>
       <c r="AD10" s="43"/>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31">
       <c r="A11" s="45" t="s">
         <v>282</v>
       </c>
@@ -7046,7 +7262,7 @@
       <c r="AC11" s="44"/>
       <c r="AD11" s="44"/>
     </row>
-    <row r="12" spans="1:31" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31" ht="17" customHeight="1">
       <c r="A12" s="45" t="s">
         <v>284</v>
       </c>
@@ -7082,7 +7298,7 @@
       <c r="AC12" s="44"/>
       <c r="AD12" s="44"/>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31">
       <c r="A13" s="45" t="s">
         <v>286</v>
       </c>
@@ -7118,7 +7334,7 @@
       <c r="AC13" s="44"/>
       <c r="AD13" s="44"/>
     </row>
-    <row r="14" spans="1:31" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31" ht="17" customHeight="1">
       <c r="A14" s="45" t="s">
         <v>288</v>
       </c>
@@ -7154,7 +7370,7 @@
       <c r="AC14" s="44"/>
       <c r="AD14" s="44"/>
     </row>
-    <row r="15" spans="1:31" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" ht="17" customHeight="1">
       <c r="A15" s="45" t="s">
         <v>290</v>
       </c>
@@ -7190,7 +7406,7 @@
       <c r="AC15" s="44"/>
       <c r="AD15" s="44"/>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31">
       <c r="A16" s="45" t="s">
         <v>292</v>
       </c>
@@ -7226,7 +7442,7 @@
       <c r="AC16" s="44"/>
       <c r="AD16" s="44"/>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30">
       <c r="A17" s="40" t="s">
         <v>294</v>
       </c>
@@ -7262,7 +7478,7 @@
       <c r="AC17" s="43"/>
       <c r="AD17" s="43"/>
     </row>
-    <row r="18" spans="1:30" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" ht="17" customHeight="1">
       <c r="A18" s="40" t="s">
         <v>296</v>
       </c>
@@ -7298,7 +7514,7 @@
       <c r="AC18" s="43"/>
       <c r="AD18" s="43"/>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30">
       <c r="A19" s="45" t="s">
         <v>298</v>
       </c>
@@ -7334,7 +7550,7 @@
       <c r="AC19" s="44"/>
       <c r="AD19" s="44"/>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30">
       <c r="A20" s="45" t="s">
         <v>300</v>
       </c>
@@ -7370,7 +7586,7 @@
       <c r="AC20" s="44"/>
       <c r="AD20" s="44"/>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30">
       <c r="A21" s="45" t="s">
         <v>302</v>
       </c>
@@ -7406,7 +7622,7 @@
       <c r="AC21" s="44"/>
       <c r="AD21" s="44"/>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30">
       <c r="A22" s="45" t="s">
         <v>304</v>
       </c>
@@ -7442,7 +7658,7 @@
       <c r="AC22" s="44"/>
       <c r="AD22" s="44"/>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30">
       <c r="A23" s="45" t="s">
         <v>306</v>
       </c>
@@ -7478,7 +7694,7 @@
       <c r="AC23" s="44"/>
       <c r="AD23" s="44"/>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30">
       <c r="A24" s="45" t="s">
         <v>308</v>
       </c>
@@ -7540,10 +7756,10 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="3" max="6" width="14.6640625" style="59" customWidth="1"/>
@@ -7573,20 +7789,20 @@
     <col min="35" max="35" width="4.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="50" customFormat="1" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:36" s="50" customFormat="1" ht="49" customHeight="1">
       <c r="A1" s="47"/>
       <c r="B1" s="47"/>
       <c r="C1" s="51" t="s">
+        <v>340</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>342</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>339</v>
+      </c>
+      <c r="F1" s="51" t="s">
         <v>341</v>
-      </c>
-      <c r="D1" s="51" t="s">
-        <v>343</v>
-      </c>
-      <c r="E1" s="51" t="s">
-        <v>340</v>
-      </c>
-      <c r="F1" s="51" t="s">
-        <v>342</v>
       </c>
       <c r="G1" s="51" t="s">
         <v>334</v>
@@ -7598,7 +7814,7 @@
         <v>333</v>
       </c>
       <c r="J1" s="51" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K1" s="51" t="s">
         <v>335</v>
@@ -7631,7 +7847,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:36" ht="27" customHeight="1">
       <c r="A2" s="40" t="s">
         <v>269</v>
       </c>
@@ -7660,10 +7876,10 @@
         <v>338</v>
       </c>
       <c r="J2" s="53" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K2" s="56" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="L2" s="40" t="s">
         <v>269</v>
@@ -7689,7 +7905,7 @@
       <c r="AE2" s="48"/>
       <c r="AF2" s="48"/>
     </row>
-    <row r="3" spans="1:36" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:36" ht="28" customHeight="1">
       <c r="A3" s="40" t="s">
         <v>271</v>
       </c>
@@ -7718,10 +7934,10 @@
         <v>338</v>
       </c>
       <c r="J3" s="53" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K3" s="56" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L3" s="40" t="s">
         <v>271</v>
@@ -7747,7 +7963,7 @@
       <c r="AE3" s="48"/>
       <c r="AF3" s="48"/>
     </row>
-    <row r="4" spans="1:36" ht="28" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:36" ht="28" customHeight="1">
       <c r="A4" s="40" t="s">
         <v>273</v>
       </c>
@@ -7766,8 +7982,8 @@
       <c r="F4" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="G4" s="56" t="s">
-        <v>339</v>
+      <c r="G4" s="53" t="s">
+        <v>338</v>
       </c>
       <c r="H4" s="53" t="s">
         <v>338</v>
@@ -7776,10 +7992,10 @@
         <v>338</v>
       </c>
       <c r="J4" s="53" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K4" s="56" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L4" s="40" t="s">
         <v>273</v>
@@ -7805,7 +8021,7 @@
       <c r="AE4" s="48"/>
       <c r="AF4" s="48"/>
     </row>
-    <row r="5" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:36" ht="27" customHeight="1">
       <c r="A5" s="40" t="s">
         <v>336</v>
       </c>
@@ -7819,10 +8035,10 @@
         <v>338</v>
       </c>
       <c r="E5" s="57" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F5" s="56" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="G5" s="55"/>
       <c r="H5" s="55"/>
@@ -7853,7 +8069,7 @@
       <c r="AE5" s="48"/>
       <c r="AF5" s="48"/>
     </row>
-    <row r="6" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:36" ht="27" customHeight="1">
       <c r="A6" s="40" t="s">
         <v>276</v>
       </c>
@@ -7882,10 +8098,10 @@
         <v>338</v>
       </c>
       <c r="J6" s="53" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K6" s="56" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="L6" s="40" t="s">
         <v>276</v>
@@ -7911,7 +8127,7 @@
       <c r="AE6" s="48"/>
       <c r="AF6" s="48"/>
     </row>
-    <row r="7" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:36" ht="27" customHeight="1">
       <c r="A7" s="40" t="s">
         <v>278</v>
       </c>
@@ -7940,10 +8156,10 @@
         <v>338</v>
       </c>
       <c r="J7" s="53" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K7" s="56" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="L7" s="40" t="s">
         <v>278</v>
@@ -7969,7 +8185,7 @@
       <c r="AE7" s="48"/>
       <c r="AF7" s="48"/>
     </row>
-    <row r="8" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:36" ht="27" customHeight="1">
       <c r="A8" s="40" t="s">
         <v>337</v>
       </c>
@@ -7992,10 +8208,10 @@
         <v>338</v>
       </c>
       <c r="H8" s="56" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I8" s="56" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J8" s="55"/>
       <c r="K8" s="55"/>
@@ -8023,7 +8239,7 @@
       <c r="AE8" s="48"/>
       <c r="AF8" s="48"/>
     </row>
-    <row r="9" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:36" ht="27" customHeight="1">
       <c r="A9" s="40" t="s">
         <v>282</v>
       </c>
@@ -8040,7 +8256,7 @@
         <v>338</v>
       </c>
       <c r="F9" s="57" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G9" s="55"/>
       <c r="H9" s="55"/>
@@ -8071,7 +8287,7 @@
       <c r="AE9" s="48"/>
       <c r="AF9" s="48"/>
     </row>
-    <row r="10" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:36" ht="27" customHeight="1">
       <c r="A10" s="40" t="s">
         <v>284</v>
       </c>
@@ -8088,7 +8304,7 @@
         <v>338</v>
       </c>
       <c r="F10" s="57" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G10" s="55"/>
       <c r="H10" s="55"/>
@@ -8119,7 +8335,7 @@
       <c r="AE10" s="48"/>
       <c r="AF10" s="48"/>
     </row>
-    <row r="11" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:36" ht="27" customHeight="1">
       <c r="A11" s="40" t="s">
         <v>286</v>
       </c>
@@ -8141,11 +8357,11 @@
       <c r="G11" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="H11" s="56" t="s">
-        <v>346</v>
-      </c>
-      <c r="I11" s="56" t="s">
-        <v>346</v>
+      <c r="H11" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="I11" s="53" t="s">
+        <v>338</v>
       </c>
       <c r="J11" s="55"/>
       <c r="K11" s="55"/>
@@ -8173,7 +8389,7 @@
       <c r="AE11" s="48"/>
       <c r="AF11" s="48"/>
     </row>
-    <row r="12" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:36" ht="27" customHeight="1">
       <c r="A12" s="40" t="s">
         <v>288</v>
       </c>
@@ -8196,10 +8412,10 @@
         <v>338</v>
       </c>
       <c r="H12" s="56" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="I12" s="56" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J12" s="55"/>
       <c r="K12" s="55"/>
@@ -8227,7 +8443,7 @@
       <c r="AE12" s="48"/>
       <c r="AF12" s="48"/>
     </row>
-    <row r="13" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:36" ht="27" customHeight="1">
       <c r="A13" s="40" t="s">
         <v>290</v>
       </c>
@@ -8256,10 +8472,10 @@
         <v>338</v>
       </c>
       <c r="J13" s="53" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K13" s="56" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L13" s="40" t="s">
         <v>290</v>
@@ -8285,7 +8501,7 @@
       <c r="AE13" s="48"/>
       <c r="AF13" s="48"/>
     </row>
-    <row r="14" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:36" ht="27" customHeight="1">
       <c r="A14" s="40" t="s">
         <v>292</v>
       </c>
@@ -8314,10 +8530,10 @@
         <v>338</v>
       </c>
       <c r="J14" s="53" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K14" s="56" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L14" s="40" t="s">
         <v>292</v>
@@ -8343,7 +8559,7 @@
       <c r="AE14" s="48"/>
       <c r="AF14" s="48"/>
     </row>
-    <row r="15" spans="1:36" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:36" ht="27" customHeight="1">
       <c r="A15" s="40" t="s">
         <v>294</v>
       </c>
@@ -8354,13 +8570,13 @@
         <v>338</v>
       </c>
       <c r="D15" s="56" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E15" s="53" t="s">
         <v>338</v>
       </c>
       <c r="F15" s="57" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G15" s="55"/>
       <c r="H15" s="55"/>
@@ -8391,7 +8607,7 @@
       <c r="AE15" s="48"/>
       <c r="AF15" s="48"/>
     </row>
-    <row r="16" spans="1:36" ht="26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:36" ht="26">
       <c r="A16" s="40" t="s">
         <v>296</v>
       </c>
@@ -8402,10 +8618,10 @@
         <v>338</v>
       </c>
       <c r="D16" s="56" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E16" s="57" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F16" s="58"/>
       <c r="G16" s="55"/>
@@ -8437,7 +8653,7 @@
       <c r="AE16" s="48"/>
       <c r="AF16" s="48"/>
     </row>
-    <row r="17" spans="1:32" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:32" ht="31" customHeight="1">
       <c r="A17" s="40" t="s">
         <v>298</v>
       </c>
@@ -8466,10 +8682,10 @@
         <v>338</v>
       </c>
       <c r="J17" s="53" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K17" s="56" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L17" s="40" t="s">
         <v>298</v>
@@ -8495,7 +8711,7 @@
       <c r="AE17" s="48"/>
       <c r="AF17" s="48"/>
     </row>
-    <row r="18" spans="1:32" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:32" ht="27" customHeight="1">
       <c r="A18" s="40" t="s">
         <v>300</v>
       </c>
@@ -8524,10 +8740,10 @@
         <v>338</v>
       </c>
       <c r="J18" s="53" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K18" s="54" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L18" s="40" t="s">
         <v>300</v>
@@ -8553,7 +8769,7 @@
       <c r="AE18" s="48"/>
       <c r="AF18" s="48"/>
     </row>
-    <row r="19" spans="1:32" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:32" ht="27" customHeight="1">
       <c r="A19" s="40" t="s">
         <v>302</v>
       </c>
@@ -8582,10 +8798,10 @@
         <v>338</v>
       </c>
       <c r="J19" s="53" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K19" s="56" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="L19" s="40" t="s">
         <v>302</v>
@@ -8611,7 +8827,7 @@
       <c r="AE19" s="48"/>
       <c r="AF19" s="48"/>
     </row>
-    <row r="20" spans="1:32" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:32" ht="27" customHeight="1">
       <c r="A20" s="40" t="s">
         <v>304</v>
       </c>
@@ -8640,10 +8856,10 @@
         <v>338</v>
       </c>
       <c r="J20" s="53" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K20" s="56" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="L20" s="40" t="s">
         <v>304</v>
@@ -8669,7 +8885,7 @@
       <c r="AE20" s="48"/>
       <c r="AF20" s="48"/>
     </row>
-    <row r="21" spans="1:32" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:32" ht="27" customHeight="1">
       <c r="A21" s="40" t="s">
         <v>306</v>
       </c>
@@ -8698,10 +8914,10 @@
         <v>338</v>
       </c>
       <c r="J21" s="53" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K21" s="56" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="L21" s="40" t="s">
         <v>306</v>
@@ -8727,7 +8943,7 @@
       <c r="AE21" s="48"/>
       <c r="AF21" s="48"/>
     </row>
-    <row r="22" spans="1:32" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:32" ht="27" customHeight="1">
       <c r="A22" s="40" t="s">
         <v>308</v>
       </c>
@@ -8756,10 +8972,10 @@
         <v>338</v>
       </c>
       <c r="J22" s="53" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="K22" s="56" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="L22" s="40" t="s">
         <v>308</v>
@@ -8789,4 +9005,963 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61D3E12-BD58-A741-A563-E559C73BCAFB}">
+  <dimension ref="A1:AF22"/>
+  <sheetViews>
+    <sheetView zoomScale="143" zoomScaleNormal="143" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="17.5" style="73" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="73"/>
+    <col min="3" max="7" width="14.6640625" style="78" customWidth="1"/>
+    <col min="8" max="8" width="17.5" style="73" customWidth="1"/>
+    <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5" customWidth="1"/>
+    <col min="11" max="11" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5" customWidth="1"/>
+    <col min="14" max="14" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5" customWidth="1"/>
+    <col min="17" max="17" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5" customWidth="1"/>
+    <col min="20" max="20" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5" customWidth="1"/>
+    <col min="23" max="23" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="5" customWidth="1"/>
+    <col min="26" max="26" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="4.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" s="50" customFormat="1" ht="49" customHeight="1">
+      <c r="A1" s="47"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="74" t="s">
+        <v>400</v>
+      </c>
+      <c r="D1" s="74" t="s">
+        <v>401</v>
+      </c>
+      <c r="E1" s="74" t="s">
+        <v>402</v>
+      </c>
+      <c r="F1" s="74" t="s">
+        <v>403</v>
+      </c>
+      <c r="G1" s="74" t="s">
+        <v>404</v>
+      </c>
+      <c r="H1" s="47"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="49"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="49"/>
+      <c r="Z1" s="49"/>
+      <c r="AA1" s="49"/>
+      <c r="AB1" s="49"/>
+      <c r="AC1" s="49"/>
+      <c r="AD1" s="49"/>
+      <c r="AE1" s="49"/>
+      <c r="AF1" s="50" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" ht="27" customHeight="1">
+      <c r="A2" s="40" t="s">
+        <v>269</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>270</v>
+      </c>
+      <c r="C2" s="75" t="s">
+        <v>410</v>
+      </c>
+      <c r="D2" s="75" t="s">
+        <v>415</v>
+      </c>
+      <c r="E2" s="75" t="s">
+        <v>416</v>
+      </c>
+      <c r="F2" s="75" t="s">
+        <v>417</v>
+      </c>
+      <c r="G2" s="75" t="s">
+        <v>418</v>
+      </c>
+      <c r="H2" s="40" t="s">
+        <v>269</v>
+      </c>
+      <c r="I2" s="48"/>
+      <c r="J2" s="48"/>
+      <c r="K2" s="48"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="48"/>
+      <c r="N2" s="48"/>
+      <c r="O2" s="48"/>
+      <c r="P2" s="48"/>
+      <c r="Q2" s="48"/>
+      <c r="R2" s="48"/>
+      <c r="S2" s="48"/>
+      <c r="T2" s="48"/>
+      <c r="U2" s="48"/>
+      <c r="V2" s="48"/>
+      <c r="W2" s="48"/>
+      <c r="X2" s="48"/>
+      <c r="Y2" s="48"/>
+      <c r="Z2" s="48"/>
+      <c r="AA2" s="48"/>
+      <c r="AB2" s="48"/>
+    </row>
+    <row r="3" spans="1:32" ht="28" customHeight="1">
+      <c r="A3" s="40" t="s">
+        <v>271</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>272</v>
+      </c>
+      <c r="C3" s="77" t="s">
+        <v>400</v>
+      </c>
+      <c r="D3" s="77" t="s">
+        <v>401</v>
+      </c>
+      <c r="E3" s="77" t="s">
+        <v>402</v>
+      </c>
+      <c r="F3" s="77" t="s">
+        <v>403</v>
+      </c>
+      <c r="G3" s="77" t="s">
+        <v>404</v>
+      </c>
+      <c r="H3" s="40" t="s">
+        <v>271</v>
+      </c>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
+      <c r="M3" s="48"/>
+      <c r="N3" s="48"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="48"/>
+      <c r="Q3" s="48"/>
+      <c r="R3" s="48"/>
+      <c r="S3" s="48"/>
+      <c r="T3" s="48"/>
+      <c r="U3" s="48"/>
+      <c r="V3" s="48"/>
+      <c r="W3" s="48"/>
+      <c r="X3" s="48"/>
+      <c r="Y3" s="48"/>
+      <c r="Z3" s="48"/>
+      <c r="AA3" s="48"/>
+      <c r="AB3" s="48"/>
+    </row>
+    <row r="4" spans="1:32" ht="28" customHeight="1">
+      <c r="A4" s="40" t="s">
+        <v>273</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="40" t="s">
+        <v>273</v>
+      </c>
+      <c r="I4" s="48"/>
+      <c r="J4" s="48"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
+      <c r="M4" s="48"/>
+      <c r="N4" s="48"/>
+      <c r="O4" s="48"/>
+      <c r="P4" s="48"/>
+      <c r="Q4" s="48"/>
+      <c r="R4" s="48"/>
+      <c r="S4" s="48"/>
+      <c r="T4" s="48"/>
+      <c r="U4" s="48"/>
+      <c r="V4" s="48"/>
+      <c r="W4" s="48"/>
+      <c r="X4" s="48"/>
+      <c r="Y4" s="48"/>
+      <c r="Z4" s="48"/>
+      <c r="AA4" s="48"/>
+      <c r="AB4" s="48"/>
+    </row>
+    <row r="5" spans="1:32" ht="27" customHeight="1">
+      <c r="A5" s="40" t="s">
+        <v>336</v>
+      </c>
+      <c r="B5" s="41" t="s">
+        <v>330</v>
+      </c>
+      <c r="C5" s="75" t="s">
+        <v>410</v>
+      </c>
+      <c r="D5" s="75" t="s">
+        <v>411</v>
+      </c>
+      <c r="E5" s="75" t="s">
+        <v>412</v>
+      </c>
+      <c r="F5" s="75" t="s">
+        <v>413</v>
+      </c>
+      <c r="G5" s="75" t="s">
+        <v>414</v>
+      </c>
+      <c r="H5" s="40" t="s">
+        <v>336</v>
+      </c>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
+      <c r="N5" s="48"/>
+      <c r="O5" s="48"/>
+      <c r="P5" s="48"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="48"/>
+      <c r="S5" s="48"/>
+      <c r="T5" s="48"/>
+      <c r="U5" s="48"/>
+      <c r="V5" s="48"/>
+      <c r="W5" s="48"/>
+      <c r="X5" s="48"/>
+      <c r="Y5" s="48"/>
+      <c r="Z5" s="48"/>
+      <c r="AA5" s="48"/>
+      <c r="AB5" s="48"/>
+    </row>
+    <row r="6" spans="1:32" ht="27" customHeight="1">
+      <c r="A6" s="40" t="s">
+        <v>276</v>
+      </c>
+      <c r="B6" s="41" t="s">
+        <v>277</v>
+      </c>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="40" t="s">
+        <v>276</v>
+      </c>
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="48"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="48"/>
+      <c r="P6" s="48"/>
+      <c r="Q6" s="48"/>
+      <c r="R6" s="48"/>
+      <c r="S6" s="48"/>
+      <c r="T6" s="48"/>
+      <c r="U6" s="48"/>
+      <c r="V6" s="48"/>
+      <c r="W6" s="48"/>
+      <c r="X6" s="48"/>
+      <c r="Y6" s="48"/>
+      <c r="Z6" s="48"/>
+      <c r="AA6" s="48"/>
+      <c r="AB6" s="48"/>
+    </row>
+    <row r="7" spans="1:32" ht="27" customHeight="1">
+      <c r="A7" s="40" t="s">
+        <v>278</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>279</v>
+      </c>
+      <c r="C7" s="75" t="s">
+        <v>410</v>
+      </c>
+      <c r="D7" s="75" t="s">
+        <v>411</v>
+      </c>
+      <c r="E7" s="75" t="s">
+        <v>412</v>
+      </c>
+      <c r="F7" s="75" t="s">
+        <v>413</v>
+      </c>
+      <c r="G7" s="75" t="s">
+        <v>414</v>
+      </c>
+      <c r="H7" s="40" t="s">
+        <v>278</v>
+      </c>
+      <c r="I7" s="48"/>
+      <c r="J7" s="48"/>
+      <c r="K7" s="48"/>
+      <c r="L7" s="48"/>
+      <c r="M7" s="48"/>
+      <c r="N7" s="48"/>
+      <c r="O7" s="48"/>
+      <c r="P7" s="48"/>
+      <c r="Q7" s="48"/>
+      <c r="R7" s="48"/>
+      <c r="S7" s="48"/>
+      <c r="T7" s="48"/>
+      <c r="U7" s="48"/>
+      <c r="V7" s="48"/>
+      <c r="W7" s="48"/>
+      <c r="X7" s="48"/>
+      <c r="Y7" s="48"/>
+      <c r="Z7" s="48"/>
+      <c r="AA7" s="48"/>
+      <c r="AB7" s="48"/>
+    </row>
+    <row r="8" spans="1:32" ht="27" customHeight="1">
+      <c r="A8" s="40" t="s">
+        <v>337</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>331</v>
+      </c>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="40" t="s">
+        <v>337</v>
+      </c>
+      <c r="I8" s="48"/>
+      <c r="J8" s="48"/>
+      <c r="K8" s="48"/>
+      <c r="L8" s="48"/>
+      <c r="M8" s="48"/>
+      <c r="N8" s="48"/>
+      <c r="O8" s="48"/>
+      <c r="P8" s="48"/>
+      <c r="Q8" s="48"/>
+      <c r="R8" s="48"/>
+      <c r="S8" s="48"/>
+      <c r="T8" s="48"/>
+      <c r="U8" s="48"/>
+      <c r="V8" s="48"/>
+      <c r="W8" s="48"/>
+      <c r="X8" s="48"/>
+      <c r="Y8" s="48"/>
+      <c r="Z8" s="48"/>
+      <c r="AA8" s="48"/>
+      <c r="AB8" s="48"/>
+    </row>
+    <row r="9" spans="1:32" ht="27" customHeight="1">
+      <c r="A9" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="B9" s="41" t="s">
+        <v>283</v>
+      </c>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="I9" s="48"/>
+      <c r="J9" s="48"/>
+      <c r="K9" s="48"/>
+      <c r="L9" s="48"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="48"/>
+      <c r="O9" s="48"/>
+      <c r="P9" s="48"/>
+      <c r="Q9" s="48"/>
+      <c r="R9" s="48"/>
+      <c r="S9" s="48"/>
+      <c r="T9" s="48"/>
+      <c r="U9" s="48"/>
+      <c r="V9" s="48"/>
+      <c r="W9" s="48"/>
+      <c r="X9" s="48"/>
+      <c r="Y9" s="48"/>
+      <c r="Z9" s="48"/>
+      <c r="AA9" s="48"/>
+      <c r="AB9" s="48"/>
+    </row>
+    <row r="10" spans="1:32" ht="27" customHeight="1">
+      <c r="A10" s="40" t="s">
+        <v>284</v>
+      </c>
+      <c r="B10" s="41" t="s">
+        <v>285</v>
+      </c>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="40" t="s">
+        <v>284</v>
+      </c>
+      <c r="I10" s="48"/>
+      <c r="J10" s="48"/>
+      <c r="K10" s="48"/>
+      <c r="L10" s="48"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="48"/>
+      <c r="P10" s="48"/>
+      <c r="Q10" s="48"/>
+      <c r="R10" s="48"/>
+      <c r="S10" s="48"/>
+      <c r="T10" s="48"/>
+      <c r="U10" s="48"/>
+      <c r="V10" s="48"/>
+      <c r="W10" s="48"/>
+      <c r="X10" s="48"/>
+      <c r="Y10" s="48"/>
+      <c r="Z10" s="48"/>
+      <c r="AA10" s="48"/>
+      <c r="AB10" s="48"/>
+    </row>
+    <row r="11" spans="1:32" ht="27" customHeight="1">
+      <c r="A11" s="40" t="s">
+        <v>286</v>
+      </c>
+      <c r="B11" s="41" t="s">
+        <v>287</v>
+      </c>
+      <c r="C11" s="76"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="76"/>
+      <c r="H11" s="40" t="s">
+        <v>286</v>
+      </c>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="48"/>
+      <c r="L11" s="48"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="48"/>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="48"/>
+      <c r="R11" s="48"/>
+      <c r="S11" s="48"/>
+      <c r="T11" s="48"/>
+      <c r="U11" s="48"/>
+      <c r="V11" s="48"/>
+      <c r="W11" s="48"/>
+      <c r="X11" s="48"/>
+      <c r="Y11" s="48"/>
+      <c r="Z11" s="48"/>
+      <c r="AA11" s="48"/>
+      <c r="AB11" s="48"/>
+    </row>
+    <row r="12" spans="1:32" ht="27" customHeight="1">
+      <c r="A12" s="40" t="s">
+        <v>288</v>
+      </c>
+      <c r="B12" s="41" t="s">
+        <v>289</v>
+      </c>
+      <c r="C12" s="77" t="s">
+        <v>400</v>
+      </c>
+      <c r="D12" s="77" t="s">
+        <v>401</v>
+      </c>
+      <c r="E12" s="77" t="s">
+        <v>402</v>
+      </c>
+      <c r="F12" s="77" t="s">
+        <v>403</v>
+      </c>
+      <c r="G12" s="77" t="s">
+        <v>404</v>
+      </c>
+      <c r="H12" s="40" t="s">
+        <v>288</v>
+      </c>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="48"/>
+      <c r="P12" s="48"/>
+      <c r="Q12" s="48"/>
+      <c r="R12" s="48"/>
+      <c r="S12" s="48"/>
+      <c r="T12" s="48"/>
+      <c r="U12" s="48"/>
+      <c r="V12" s="48"/>
+      <c r="W12" s="48"/>
+      <c r="X12" s="48"/>
+      <c r="Y12" s="48"/>
+      <c r="Z12" s="48"/>
+      <c r="AA12" s="48"/>
+      <c r="AB12" s="48"/>
+    </row>
+    <row r="13" spans="1:32" ht="27" customHeight="1">
+      <c r="A13" s="40" t="s">
+        <v>290</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>291</v>
+      </c>
+      <c r="C13" s="75" t="s">
+        <v>410</v>
+      </c>
+      <c r="D13" s="75" t="s">
+        <v>411</v>
+      </c>
+      <c r="E13" s="75" t="s">
+        <v>412</v>
+      </c>
+      <c r="F13" s="75" t="s">
+        <v>413</v>
+      </c>
+      <c r="G13" s="75" t="s">
+        <v>414</v>
+      </c>
+      <c r="H13" s="40" t="s">
+        <v>290</v>
+      </c>
+      <c r="I13" s="48"/>
+      <c r="J13" s="48"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="48"/>
+      <c r="M13" s="48"/>
+      <c r="N13" s="48"/>
+      <c r="O13" s="48"/>
+      <c r="P13" s="48"/>
+      <c r="Q13" s="48"/>
+      <c r="R13" s="48"/>
+      <c r="S13" s="48"/>
+      <c r="T13" s="48"/>
+      <c r="U13" s="48"/>
+      <c r="V13" s="48"/>
+      <c r="W13" s="48"/>
+      <c r="X13" s="48"/>
+      <c r="Y13" s="48"/>
+      <c r="Z13" s="48"/>
+      <c r="AA13" s="48"/>
+      <c r="AB13" s="48"/>
+    </row>
+    <row r="14" spans="1:32" ht="27" customHeight="1">
+      <c r="A14" s="40" t="s">
+        <v>292</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>293</v>
+      </c>
+      <c r="C14" s="79" t="s">
+        <v>405</v>
+      </c>
+      <c r="D14" s="75" t="s">
+        <v>406</v>
+      </c>
+      <c r="E14" s="80" t="s">
+        <v>407</v>
+      </c>
+      <c r="F14" s="80" t="s">
+        <v>408</v>
+      </c>
+      <c r="G14" s="80" t="s">
+        <v>409</v>
+      </c>
+      <c r="H14" s="40" t="s">
+        <v>292</v>
+      </c>
+      <c r="I14" s="48"/>
+      <c r="J14" s="48"/>
+      <c r="K14" s="48"/>
+      <c r="L14" s="48"/>
+      <c r="M14" s="48"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="48"/>
+      <c r="P14" s="48"/>
+      <c r="Q14" s="48"/>
+      <c r="R14" s="48"/>
+      <c r="S14" s="48"/>
+      <c r="T14" s="48"/>
+      <c r="U14" s="48"/>
+      <c r="V14" s="48"/>
+      <c r="W14" s="48"/>
+      <c r="X14" s="48"/>
+      <c r="Y14" s="48"/>
+      <c r="Z14" s="48"/>
+      <c r="AA14" s="48"/>
+      <c r="AB14" s="48"/>
+    </row>
+    <row r="15" spans="1:32" ht="27" customHeight="1">
+      <c r="A15" s="40" t="s">
+        <v>294</v>
+      </c>
+      <c r="B15" s="41" t="s">
+        <v>295</v>
+      </c>
+      <c r="C15" s="77" t="s">
+        <v>400</v>
+      </c>
+      <c r="D15" s="77" t="s">
+        <v>401</v>
+      </c>
+      <c r="E15" s="77" t="s">
+        <v>402</v>
+      </c>
+      <c r="F15" s="77" t="s">
+        <v>403</v>
+      </c>
+      <c r="G15" s="77" t="s">
+        <v>404</v>
+      </c>
+      <c r="H15" s="40" t="s">
+        <v>294</v>
+      </c>
+      <c r="I15" s="48"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="48"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="48"/>
+      <c r="N15" s="48"/>
+      <c r="O15" s="48"/>
+      <c r="P15" s="48"/>
+      <c r="Q15" s="48"/>
+      <c r="R15" s="48"/>
+      <c r="S15" s="48"/>
+      <c r="T15" s="48"/>
+      <c r="U15" s="48"/>
+      <c r="V15" s="48"/>
+      <c r="W15" s="48"/>
+      <c r="X15" s="48"/>
+      <c r="Y15" s="48"/>
+      <c r="Z15" s="48"/>
+      <c r="AA15" s="48"/>
+      <c r="AB15" s="48"/>
+    </row>
+    <row r="16" spans="1:32">
+      <c r="A16" s="40" t="s">
+        <v>296</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>297</v>
+      </c>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="40" t="s">
+        <v>296</v>
+      </c>
+      <c r="I16" s="48"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="48"/>
+      <c r="L16" s="48"/>
+      <c r="M16" s="48"/>
+      <c r="N16" s="48"/>
+      <c r="O16" s="48"/>
+      <c r="P16" s="48"/>
+      <c r="Q16" s="48"/>
+      <c r="R16" s="48"/>
+      <c r="S16" s="48"/>
+      <c r="T16" s="48"/>
+      <c r="U16" s="48"/>
+      <c r="V16" s="48"/>
+      <c r="W16" s="48"/>
+      <c r="X16" s="48"/>
+      <c r="Y16" s="48"/>
+      <c r="Z16" s="48"/>
+      <c r="AA16" s="48"/>
+      <c r="AB16" s="48"/>
+    </row>
+    <row r="17" spans="1:28" ht="31" customHeight="1">
+      <c r="A17" s="40" t="s">
+        <v>298</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>299</v>
+      </c>
+      <c r="C17" s="77" t="s">
+        <v>400</v>
+      </c>
+      <c r="D17" s="77" t="s">
+        <v>401</v>
+      </c>
+      <c r="E17" s="77" t="s">
+        <v>402</v>
+      </c>
+      <c r="F17" s="77" t="s">
+        <v>403</v>
+      </c>
+      <c r="G17" s="77" t="s">
+        <v>404</v>
+      </c>
+      <c r="H17" s="40" t="s">
+        <v>298</v>
+      </c>
+      <c r="I17" s="48"/>
+      <c r="J17" s="48"/>
+      <c r="K17" s="48"/>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="48"/>
+      <c r="O17" s="48"/>
+      <c r="P17" s="48"/>
+      <c r="Q17" s="48"/>
+      <c r="R17" s="48"/>
+      <c r="S17" s="48"/>
+      <c r="T17" s="48"/>
+      <c r="U17" s="48"/>
+      <c r="V17" s="48"/>
+      <c r="W17" s="48"/>
+      <c r="X17" s="48"/>
+      <c r="Y17" s="48"/>
+      <c r="Z17" s="48"/>
+      <c r="AA17" s="48"/>
+      <c r="AB17" s="48"/>
+    </row>
+    <row r="18" spans="1:28" ht="27" customHeight="1">
+      <c r="A18" s="40" t="s">
+        <v>300</v>
+      </c>
+      <c r="B18" s="41" t="s">
+        <v>301</v>
+      </c>
+      <c r="C18" s="75" t="s">
+        <v>410</v>
+      </c>
+      <c r="D18" s="75" t="s">
+        <v>411</v>
+      </c>
+      <c r="E18" s="75" t="s">
+        <v>412</v>
+      </c>
+      <c r="F18" s="75" t="s">
+        <v>413</v>
+      </c>
+      <c r="G18" s="75" t="s">
+        <v>414</v>
+      </c>
+      <c r="H18" s="40" t="s">
+        <v>300</v>
+      </c>
+      <c r="I18" s="48"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="48"/>
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
+      <c r="N18" s="48"/>
+      <c r="O18" s="48"/>
+      <c r="P18" s="48"/>
+      <c r="Q18" s="48"/>
+      <c r="R18" s="48"/>
+      <c r="S18" s="48"/>
+      <c r="T18" s="48"/>
+      <c r="U18" s="48"/>
+      <c r="V18" s="48"/>
+      <c r="W18" s="48"/>
+      <c r="X18" s="48"/>
+      <c r="Y18" s="48"/>
+      <c r="Z18" s="48"/>
+      <c r="AA18" s="48"/>
+      <c r="AB18" s="48"/>
+    </row>
+    <row r="19" spans="1:28" ht="27" customHeight="1">
+      <c r="A19" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="B19" s="41" t="s">
+        <v>303</v>
+      </c>
+      <c r="C19" s="76"/>
+      <c r="D19" s="76"/>
+      <c r="E19" s="76"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="48"/>
+      <c r="L19" s="48"/>
+      <c r="M19" s="48"/>
+      <c r="N19" s="48"/>
+      <c r="O19" s="48"/>
+      <c r="P19" s="48"/>
+      <c r="Q19" s="48"/>
+      <c r="R19" s="48"/>
+      <c r="S19" s="48"/>
+      <c r="T19" s="48"/>
+      <c r="U19" s="48"/>
+      <c r="V19" s="48"/>
+      <c r="W19" s="48"/>
+      <c r="X19" s="48"/>
+      <c r="Y19" s="48"/>
+      <c r="Z19" s="48"/>
+      <c r="AA19" s="48"/>
+      <c r="AB19" s="48"/>
+    </row>
+    <row r="20" spans="1:28" ht="27" customHeight="1">
+      <c r="A20" s="40" t="s">
+        <v>304</v>
+      </c>
+      <c r="B20" s="41" t="s">
+        <v>305</v>
+      </c>
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="76"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="40" t="s">
+        <v>304</v>
+      </c>
+      <c r="I20" s="48"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="48"/>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
+      <c r="N20" s="48"/>
+      <c r="O20" s="48"/>
+      <c r="P20" s="48"/>
+      <c r="Q20" s="48"/>
+      <c r="R20" s="48"/>
+      <c r="S20" s="48"/>
+      <c r="T20" s="48"/>
+      <c r="U20" s="48"/>
+      <c r="V20" s="48"/>
+      <c r="W20" s="48"/>
+      <c r="X20" s="48"/>
+      <c r="Y20" s="48"/>
+      <c r="Z20" s="48"/>
+      <c r="AA20" s="48"/>
+      <c r="AB20" s="48"/>
+    </row>
+    <row r="21" spans="1:28" ht="27" customHeight="1">
+      <c r="A21" s="40" t="s">
+        <v>306</v>
+      </c>
+      <c r="B21" s="41" t="s">
+        <v>307</v>
+      </c>
+      <c r="C21" s="76"/>
+      <c r="D21" s="76"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="76"/>
+      <c r="H21" s="40" t="s">
+        <v>306</v>
+      </c>
+      <c r="I21" s="48"/>
+      <c r="J21" s="48"/>
+      <c r="K21" s="48"/>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
+      <c r="N21" s="48"/>
+      <c r="O21" s="48"/>
+      <c r="P21" s="48"/>
+      <c r="Q21" s="48"/>
+      <c r="R21" s="48"/>
+      <c r="S21" s="48"/>
+      <c r="T21" s="48"/>
+      <c r="U21" s="48"/>
+      <c r="V21" s="48"/>
+      <c r="W21" s="48"/>
+      <c r="X21" s="48"/>
+      <c r="Y21" s="48"/>
+      <c r="Z21" s="48"/>
+      <c r="AA21" s="48"/>
+      <c r="AB21" s="48"/>
+    </row>
+    <row r="22" spans="1:28" ht="27" customHeight="1">
+      <c r="A22" s="40" t="s">
+        <v>308</v>
+      </c>
+      <c r="B22" s="41" t="s">
+        <v>309</v>
+      </c>
+      <c r="C22" s="77" t="s">
+        <v>400</v>
+      </c>
+      <c r="D22" s="77" t="s">
+        <v>401</v>
+      </c>
+      <c r="E22" s="77" t="s">
+        <v>402</v>
+      </c>
+      <c r="F22" s="77" t="s">
+        <v>403</v>
+      </c>
+      <c r="G22" s="77" t="s">
+        <v>404</v>
+      </c>
+      <c r="H22" s="40" t="s">
+        <v>308</v>
+      </c>
+      <c r="I22" s="48"/>
+      <c r="J22" s="48"/>
+      <c r="K22" s="48"/>
+      <c r="L22" s="48"/>
+      <c r="M22" s="48"/>
+      <c r="N22" s="48"/>
+      <c r="O22" s="48"/>
+      <c r="P22" s="48"/>
+      <c r="Q22" s="48"/>
+      <c r="R22" s="48"/>
+      <c r="S22" s="48"/>
+      <c r="T22" s="48"/>
+      <c r="U22" s="48"/>
+      <c r="V22" s="48"/>
+      <c r="W22" s="48"/>
+      <c r="X22" s="48"/>
+      <c r="Y22" s="48"/>
+      <c r="Z22" s="48"/>
+      <c r="AA22" s="48"/>
+      <c r="AB22" s="48"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
corrected en-MW translations of the GSHS and HBSC pages
</commit_message>
<xml_diff>
--- a/GACPAQ pages.xlsx
+++ b/GACPAQ pages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doncastillo/Code/gacpaq/gacpaq-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E649D3-FDB7-F647-9730-86B3E67C44DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2474C901-9DBF-E649-BF77-9C99C3197DB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20140" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="934" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="420">
   <si>
     <t>Page Number</t>
   </si>
@@ -2872,6 +2872,9 @@
   </si>
   <si>
     <t>Respostas enviadas</t>
+  </si>
+  <si>
+    <t>on-going</t>
   </si>
 </sst>
 </file>
@@ -7756,7 +7759,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomRight" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8258,7 +8261,9 @@
       <c r="F9" s="57" t="s">
         <v>346</v>
       </c>
-      <c r="G9" s="55"/>
+      <c r="G9" s="53" t="s">
+        <v>338</v>
+      </c>
       <c r="H9" s="55"/>
       <c r="I9" s="55"/>
       <c r="J9" s="55"/>
@@ -8306,7 +8311,9 @@
       <c r="F10" s="57" t="s">
         <v>346</v>
       </c>
-      <c r="G10" s="55"/>
+      <c r="G10" s="56" t="s">
+        <v>419</v>
+      </c>
       <c r="H10" s="55"/>
       <c r="I10" s="55"/>
       <c r="J10" s="55"/>
@@ -8363,7 +8370,9 @@
       <c r="I11" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="J11" s="55"/>
+      <c r="J11" s="56" t="s">
+        <v>419</v>
+      </c>
       <c r="K11" s="55"/>
       <c r="L11" s="40" t="s">
         <v>286</v>
@@ -8411,13 +8420,15 @@
       <c r="G12" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="H12" s="56" t="s">
-        <v>345</v>
-      </c>
-      <c r="I12" s="56" t="s">
-        <v>345</v>
-      </c>
-      <c r="J12" s="55"/>
+      <c r="H12" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="I12" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="J12" s="56" t="s">
+        <v>419</v>
+      </c>
       <c r="K12" s="55"/>
       <c r="L12" s="40" t="s">
         <v>288</v>

</xml_diff>

<commit_message>
use en-CA narrations for en-IN
</commit_message>
<xml_diff>
--- a/GACPAQ pages.xlsx
+++ b/GACPAQ pages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doncastillo/Code/gacpaq/gacpaq-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE3377E-131D-E04C-A3A4-24FB9ECD47E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4135D3-E23E-244F-A21D-C8033B9E2865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12740" yWindow="-21100" windowWidth="38400" windowHeight="19500" activeTab="5" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
+    <workbookView xWindow="-20140" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="422">
   <si>
     <t>Page Number</t>
   </si>
@@ -2877,7 +2877,10 @@
     <t>on-going</t>
   </si>
   <si>
-    <t>in progress</t>
+    <t>India - English</t>
+  </si>
+  <si>
+    <t>en-IN</t>
   </si>
 </sst>
 </file>
@@ -3459,6 +3462,28 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3479,28 +3504,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6808,38 +6811,38 @@
     <row r="1" spans="1:31" s="39" customFormat="1" ht="16" customHeight="1">
       <c r="A1" s="38"/>
       <c r="B1" s="38"/>
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="74" t="s">
         <v>254</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="71" t="s">
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="79" t="s">
         <v>255</v>
       </c>
-      <c r="H1" s="72"/>
-      <c r="I1" s="72"/>
-      <c r="J1" s="72"/>
-      <c r="K1" s="72"/>
-      <c r="L1" s="72"/>
-      <c r="M1" s="72"/>
-      <c r="N1" s="72"/>
-      <c r="O1" s="72"/>
-      <c r="P1" s="72"/>
-      <c r="Q1" s="72"/>
-      <c r="R1" s="72"/>
-      <c r="S1" s="72"/>
-      <c r="T1" s="72"/>
-      <c r="U1" s="72"/>
-      <c r="V1" s="72"/>
-      <c r="W1" s="72"/>
-      <c r="X1" s="72"/>
-      <c r="Y1" s="72"/>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="72"/>
-      <c r="AB1" s="72"/>
-      <c r="AC1" s="72"/>
-      <c r="AD1" s="72"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="80"/>
+      <c r="P1" s="80"/>
+      <c r="Q1" s="80"/>
+      <c r="R1" s="80"/>
+      <c r="S1" s="80"/>
+      <c r="T1" s="80"/>
+      <c r="U1" s="80"/>
+      <c r="V1" s="80"/>
+      <c r="W1" s="80"/>
+      <c r="X1" s="80"/>
+      <c r="Y1" s="80"/>
+      <c r="Z1" s="80"/>
+      <c r="AA1" s="80"/>
+      <c r="AB1" s="80"/>
+      <c r="AC1" s="80"/>
+      <c r="AD1" s="80"/>
       <c r="AE1" s="39" t="s">
         <v>310</v>
       </c>
@@ -6859,46 +6862,46 @@
       <c r="F2" s="40" t="s">
         <v>259</v>
       </c>
-      <c r="G2" s="67" t="s">
+      <c r="G2" s="75" t="s">
         <v>260</v>
       </c>
-      <c r="H2" s="68"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="67" t="s">
+      <c r="H2" s="76"/>
+      <c r="I2" s="77"/>
+      <c r="J2" s="75" t="s">
         <v>261</v>
       </c>
-      <c r="K2" s="68"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="67" t="s">
+      <c r="K2" s="76"/>
+      <c r="L2" s="77"/>
+      <c r="M2" s="75" t="s">
         <v>262</v>
       </c>
-      <c r="N2" s="68"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="67" t="s">
+      <c r="N2" s="76"/>
+      <c r="O2" s="77"/>
+      <c r="P2" s="75" t="s">
         <v>263</v>
       </c>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="69"/>
-      <c r="S2" s="67" t="s">
+      <c r="Q2" s="76"/>
+      <c r="R2" s="77"/>
+      <c r="S2" s="75" t="s">
         <v>264</v>
       </c>
-      <c r="T2" s="68"/>
-      <c r="U2" s="69"/>
-      <c r="V2" s="67" t="s">
+      <c r="T2" s="76"/>
+      <c r="U2" s="77"/>
+      <c r="V2" s="75" t="s">
         <v>265</v>
       </c>
-      <c r="W2" s="68"/>
-      <c r="X2" s="69"/>
-      <c r="Y2" s="67" t="s">
+      <c r="W2" s="76"/>
+      <c r="X2" s="77"/>
+      <c r="Y2" s="75" t="s">
         <v>266</v>
       </c>
-      <c r="Z2" s="68"/>
-      <c r="AA2" s="69"/>
-      <c r="AB2" s="70" t="s">
+      <c r="Z2" s="76"/>
+      <c r="AA2" s="77"/>
+      <c r="AB2" s="78" t="s">
         <v>312</v>
       </c>
-      <c r="AC2" s="70"/>
-      <c r="AD2" s="70"/>
+      <c r="AC2" s="78"/>
+      <c r="AD2" s="78"/>
     </row>
     <row r="3" spans="1:31" s="39" customFormat="1">
       <c r="A3" s="40"/>
@@ -7756,13 +7759,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BEEE373-47BE-6F4C-8F66-ACD6798C647F}">
-  <dimension ref="A1:AJ22"/>
+  <dimension ref="A1:AJ23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="114" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H16" sqref="H16:I16"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8247,10 +8250,10 @@
     </row>
     <row r="9" spans="1:36" ht="27" customHeight="1">
       <c r="A9" s="40" t="s">
-        <v>282</v>
+        <v>420</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>283</v>
+        <v>421</v>
       </c>
       <c r="C9" s="53" t="s">
         <v>338</v>
@@ -8261,8 +8264,8 @@
       <c r="E9" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="F9" s="57" t="s">
-        <v>346</v>
+      <c r="F9" s="53" t="s">
+        <v>338</v>
       </c>
       <c r="G9" s="53" t="s">
         <v>338</v>
@@ -8272,7 +8275,7 @@
       <c r="J9" s="55"/>
       <c r="K9" s="55"/>
       <c r="L9" s="40" t="s">
-        <v>282</v>
+        <v>420</v>
       </c>
       <c r="M9" s="48"/>
       <c r="N9" s="48"/>
@@ -8297,10 +8300,10 @@
     </row>
     <row r="10" spans="1:36" ht="27" customHeight="1">
       <c r="A10" s="40" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C10" s="53" t="s">
         <v>338</v>
@@ -8314,15 +8317,15 @@
       <c r="F10" s="57" t="s">
         <v>346</v>
       </c>
-      <c r="G10" s="56" t="s">
-        <v>419</v>
+      <c r="G10" s="53" t="s">
+        <v>338</v>
       </c>
       <c r="H10" s="55"/>
       <c r="I10" s="55"/>
       <c r="J10" s="55"/>
       <c r="K10" s="55"/>
       <c r="L10" s="40" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="M10" s="48"/>
       <c r="N10" s="48"/>
@@ -8347,10 +8350,10 @@
     </row>
     <row r="11" spans="1:36" ht="27" customHeight="1">
       <c r="A11" s="40" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B11" s="41" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C11" s="53" t="s">
         <v>338</v>
@@ -8361,24 +8364,18 @@
       <c r="E11" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="F11" s="53" t="s">
-        <v>338</v>
-      </c>
-      <c r="G11" s="53" t="s">
-        <v>338</v>
-      </c>
-      <c r="H11" s="53" t="s">
-        <v>338</v>
-      </c>
-      <c r="I11" s="53" t="s">
-        <v>338</v>
-      </c>
-      <c r="J11" s="56" t="s">
+      <c r="F11" s="57" t="s">
+        <v>346</v>
+      </c>
+      <c r="G11" s="56" t="s">
         <v>419</v>
       </c>
+      <c r="H11" s="55"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="55"/>
       <c r="K11" s="55"/>
       <c r="L11" s="40" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="M11" s="48"/>
       <c r="N11" s="48"/>
@@ -8403,10 +8400,10 @@
     </row>
     <row r="12" spans="1:36" ht="27" customHeight="1">
       <c r="A12" s="40" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B12" s="41" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C12" s="53" t="s">
         <v>338</v>
@@ -8434,7 +8431,7 @@
       </c>
       <c r="K12" s="55"/>
       <c r="L12" s="40" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="M12" s="48"/>
       <c r="N12" s="48"/>
@@ -8459,10 +8456,10 @@
     </row>
     <row r="13" spans="1:36" ht="27" customHeight="1">
       <c r="A13" s="40" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="B13" s="41" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C13" s="53" t="s">
         <v>338</v>
@@ -8485,14 +8482,12 @@
       <c r="I13" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="J13" s="53" t="s">
-        <v>344</v>
-      </c>
-      <c r="K13" s="56" t="s">
-        <v>390</v>
-      </c>
+      <c r="J13" s="56" t="s">
+        <v>419</v>
+      </c>
+      <c r="K13" s="55"/>
       <c r="L13" s="40" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="M13" s="48"/>
       <c r="N13" s="48"/>
@@ -8517,10 +8512,10 @@
     </row>
     <row r="14" spans="1:36" ht="27" customHeight="1">
       <c r="A14" s="40" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="B14" s="41" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C14" s="53" t="s">
         <v>338</v>
@@ -8547,10 +8542,10 @@
         <v>344</v>
       </c>
       <c r="K14" s="56" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="L14" s="40" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="M14" s="48"/>
       <c r="N14" s="48"/>
@@ -8575,34 +8570,40 @@
     </row>
     <row r="15" spans="1:36" ht="27" customHeight="1">
       <c r="A15" s="40" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B15" s="41" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C15" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="D15" s="56" t="s">
-        <v>392</v>
+      <c r="D15" s="53" t="s">
+        <v>338</v>
       </c>
       <c r="E15" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="F15" s="57" t="s">
-        <v>346</v>
-      </c>
-      <c r="G15" s="55"/>
-      <c r="H15" s="56" t="s">
-        <v>420</v>
-      </c>
-      <c r="I15" s="56" t="s">
-        <v>420</v>
-      </c>
-      <c r="J15" s="55"/>
-      <c r="K15" s="55"/>
+      <c r="F15" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="G15" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="H15" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="I15" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="J15" s="53" t="s">
+        <v>344</v>
+      </c>
+      <c r="K15" s="56" t="s">
+        <v>395</v>
+      </c>
       <c r="L15" s="40" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="M15" s="48"/>
       <c r="N15" s="48"/>
@@ -8625,12 +8626,12 @@
       <c r="AE15" s="48"/>
       <c r="AF15" s="48"/>
     </row>
-    <row r="16" spans="1:36" ht="26">
+    <row r="16" spans="1:36" ht="27" customHeight="1">
       <c r="A16" s="40" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B16" s="41" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C16" s="53" t="s">
         <v>338</v>
@@ -8638,10 +8639,12 @@
       <c r="D16" s="56" t="s">
         <v>392</v>
       </c>
-      <c r="E16" s="57" t="s">
-        <v>347</v>
-      </c>
-      <c r="F16" s="58"/>
+      <c r="E16" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="F16" s="57" t="s">
+        <v>346</v>
+      </c>
       <c r="G16" s="55"/>
       <c r="H16" s="53" t="s">
         <v>338</v>
@@ -8652,7 +8655,7 @@
       <c r="J16" s="55"/>
       <c r="K16" s="55"/>
       <c r="L16" s="40" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="M16" s="48"/>
       <c r="N16" s="48"/>
@@ -8675,42 +8678,34 @@
       <c r="AE16" s="48"/>
       <c r="AF16" s="48"/>
     </row>
-    <row r="17" spans="1:32" ht="31" customHeight="1">
+    <row r="17" spans="1:32" ht="26">
       <c r="A17" s="40" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="C17" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="D17" s="53" t="s">
-        <v>338</v>
-      </c>
-      <c r="E17" s="53" t="s">
-        <v>338</v>
-      </c>
-      <c r="F17" s="53" t="s">
-        <v>338</v>
-      </c>
-      <c r="G17" s="53" t="s">
-        <v>338</v>
-      </c>
+      <c r="D17" s="56" t="s">
+        <v>392</v>
+      </c>
+      <c r="E17" s="57" t="s">
+        <v>347</v>
+      </c>
+      <c r="F17" s="58"/>
+      <c r="G17" s="55"/>
       <c r="H17" s="53" t="s">
         <v>338</v>
       </c>
       <c r="I17" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="J17" s="53" t="s">
-        <v>344</v>
-      </c>
-      <c r="K17" s="56" t="s">
-        <v>395</v>
-      </c>
+      <c r="J17" s="55"/>
+      <c r="K17" s="55"/>
       <c r="L17" s="40" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="M17" s="48"/>
       <c r="N17" s="48"/>
@@ -8733,12 +8728,12 @@
       <c r="AE17" s="48"/>
       <c r="AF17" s="48"/>
     </row>
-    <row r="18" spans="1:32" ht="27" customHeight="1">
+    <row r="18" spans="1:32" ht="31" customHeight="1">
       <c r="A18" s="40" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C18" s="53" t="s">
         <v>338</v>
@@ -8764,11 +8759,11 @@
       <c r="J18" s="53" t="s">
         <v>344</v>
       </c>
-      <c r="K18" s="54" t="s">
-        <v>391</v>
+      <c r="K18" s="56" t="s">
+        <v>395</v>
       </c>
       <c r="L18" s="40" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="M18" s="48"/>
       <c r="N18" s="48"/>
@@ -8793,10 +8788,10 @@
     </row>
     <row r="19" spans="1:32" ht="27" customHeight="1">
       <c r="A19" s="40" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C19" s="53" t="s">
         <v>338</v>
@@ -8822,11 +8817,11 @@
       <c r="J19" s="53" t="s">
         <v>344</v>
       </c>
-      <c r="K19" s="56" t="s">
-        <v>389</v>
+      <c r="K19" s="54" t="s">
+        <v>391</v>
       </c>
       <c r="L19" s="40" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="M19" s="48"/>
       <c r="N19" s="48"/>
@@ -8851,10 +8846,10 @@
     </row>
     <row r="20" spans="1:32" ht="27" customHeight="1">
       <c r="A20" s="40" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C20" s="53" t="s">
         <v>338</v>
@@ -8881,10 +8876,10 @@
         <v>344</v>
       </c>
       <c r="K20" s="56" t="s">
-        <v>399</v>
+        <v>389</v>
       </c>
       <c r="L20" s="40" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="M20" s="48"/>
       <c r="N20" s="48"/>
@@ -8909,10 +8904,10 @@
     </row>
     <row r="21" spans="1:32" ht="27" customHeight="1">
       <c r="A21" s="40" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B21" s="41" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C21" s="53" t="s">
         <v>338</v>
@@ -8939,10 +8934,10 @@
         <v>344</v>
       </c>
       <c r="K21" s="56" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="L21" s="40" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="M21" s="48"/>
       <c r="N21" s="48"/>
@@ -8967,10 +8962,10 @@
     </row>
     <row r="22" spans="1:32" ht="27" customHeight="1">
       <c r="A22" s="40" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="B22" s="41" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C22" s="53" t="s">
         <v>338</v>
@@ -9000,7 +8995,7 @@
         <v>398</v>
       </c>
       <c r="L22" s="40" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="M22" s="48"/>
       <c r="N22" s="48"/>
@@ -9023,6 +9018,64 @@
       <c r="AE22" s="48"/>
       <c r="AF22" s="48"/>
     </row>
+    <row r="23" spans="1:32" ht="27" customHeight="1">
+      <c r="A23" s="40" t="s">
+        <v>308</v>
+      </c>
+      <c r="B23" s="41" t="s">
+        <v>309</v>
+      </c>
+      <c r="C23" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="D23" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="E23" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="F23" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="G23" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="H23" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="I23" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="J23" s="53" t="s">
+        <v>344</v>
+      </c>
+      <c r="K23" s="56" t="s">
+        <v>398</v>
+      </c>
+      <c r="L23" s="40" t="s">
+        <v>308</v>
+      </c>
+      <c r="M23" s="48"/>
+      <c r="N23" s="48"/>
+      <c r="O23" s="48"/>
+      <c r="P23" s="48"/>
+      <c r="Q23" s="48"/>
+      <c r="R23" s="48"/>
+      <c r="S23" s="48"/>
+      <c r="T23" s="48"/>
+      <c r="U23" s="48"/>
+      <c r="V23" s="48"/>
+      <c r="W23" s="48"/>
+      <c r="X23" s="48"/>
+      <c r="Y23" s="48"/>
+      <c r="Z23" s="48"/>
+      <c r="AA23" s="48"/>
+      <c r="AB23" s="48"/>
+      <c r="AC23" s="48"/>
+      <c r="AD23" s="48"/>
+      <c r="AE23" s="48"/>
+      <c r="AF23" s="48"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -9042,10 +9095,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="73" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="73"/>
-    <col min="3" max="7" width="14.6640625" style="78" customWidth="1"/>
-    <col min="8" max="8" width="17.5" style="73" customWidth="1"/>
+    <col min="1" max="1" width="17.5" style="66" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="66"/>
+    <col min="3" max="7" width="14.6640625" style="71" customWidth="1"/>
+    <col min="8" max="8" width="17.5" style="66" customWidth="1"/>
     <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5" customWidth="1"/>
     <col min="11" max="11" width="5.33203125" bestFit="1" customWidth="1"/>
@@ -9073,19 +9126,19 @@
     <row r="1" spans="1:32" s="50" customFormat="1" ht="49" customHeight="1">
       <c r="A1" s="47"/>
       <c r="B1" s="47"/>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="67" t="s">
         <v>400</v>
       </c>
-      <c r="D1" s="74" t="s">
+      <c r="D1" s="67" t="s">
         <v>401</v>
       </c>
-      <c r="E1" s="74" t="s">
+      <c r="E1" s="67" t="s">
         <v>402</v>
       </c>
-      <c r="F1" s="74" t="s">
+      <c r="F1" s="67" t="s">
         <v>403</v>
       </c>
-      <c r="G1" s="74" t="s">
+      <c r="G1" s="67" t="s">
         <v>404</v>
       </c>
       <c r="H1" s="47"/>
@@ -9123,19 +9176,19 @@
       <c r="B2" s="41" t="s">
         <v>270</v>
       </c>
-      <c r="C2" s="75" t="s">
+      <c r="C2" s="68" t="s">
         <v>410</v>
       </c>
-      <c r="D2" s="75" t="s">
+      <c r="D2" s="68" t="s">
         <v>415</v>
       </c>
-      <c r="E2" s="75" t="s">
+      <c r="E2" s="68" t="s">
         <v>416</v>
       </c>
-      <c r="F2" s="75" t="s">
+      <c r="F2" s="68" t="s">
         <v>417</v>
       </c>
-      <c r="G2" s="75" t="s">
+      <c r="G2" s="68" t="s">
         <v>418</v>
       </c>
       <c r="H2" s="40" t="s">
@@ -9169,19 +9222,19 @@
       <c r="B3" s="41" t="s">
         <v>272</v>
       </c>
-      <c r="C3" s="77" t="s">
+      <c r="C3" s="70" t="s">
         <v>400</v>
       </c>
-      <c r="D3" s="77" t="s">
+      <c r="D3" s="70" t="s">
         <v>401</v>
       </c>
-      <c r="E3" s="77" t="s">
+      <c r="E3" s="70" t="s">
         <v>402</v>
       </c>
-      <c r="F3" s="77" t="s">
+      <c r="F3" s="70" t="s">
         <v>403</v>
       </c>
-      <c r="G3" s="77" t="s">
+      <c r="G3" s="70" t="s">
         <v>404</v>
       </c>
       <c r="H3" s="40" t="s">
@@ -9215,11 +9268,11 @@
       <c r="B4" s="41" t="s">
         <v>274</v>
       </c>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
-      <c r="F4" s="76"/>
-      <c r="G4" s="76"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
       <c r="H4" s="40" t="s">
         <v>273</v>
       </c>
@@ -9251,19 +9304,19 @@
       <c r="B5" s="41" t="s">
         <v>330</v>
       </c>
-      <c r="C5" s="75" t="s">
+      <c r="C5" s="68" t="s">
         <v>410</v>
       </c>
-      <c r="D5" s="75" t="s">
+      <c r="D5" s="68" t="s">
         <v>411</v>
       </c>
-      <c r="E5" s="75" t="s">
+      <c r="E5" s="68" t="s">
         <v>412</v>
       </c>
-      <c r="F5" s="75" t="s">
+      <c r="F5" s="68" t="s">
         <v>413</v>
       </c>
-      <c r="G5" s="75" t="s">
+      <c r="G5" s="68" t="s">
         <v>414</v>
       </c>
       <c r="H5" s="40" t="s">
@@ -9297,11 +9350,11 @@
       <c r="B6" s="41" t="s">
         <v>277</v>
       </c>
-      <c r="C6" s="76"/>
-      <c r="D6" s="76"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="76"/>
-      <c r="G6" s="76"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
       <c r="H6" s="40" t="s">
         <v>276</v>
       </c>
@@ -9333,19 +9386,19 @@
       <c r="B7" s="41" t="s">
         <v>279</v>
       </c>
-      <c r="C7" s="75" t="s">
+      <c r="C7" s="68" t="s">
         <v>410</v>
       </c>
-      <c r="D7" s="75" t="s">
+      <c r="D7" s="68" t="s">
         <v>411</v>
       </c>
-      <c r="E7" s="75" t="s">
+      <c r="E7" s="68" t="s">
         <v>412</v>
       </c>
-      <c r="F7" s="75" t="s">
+      <c r="F7" s="68" t="s">
         <v>413</v>
       </c>
-      <c r="G7" s="75" t="s">
+      <c r="G7" s="68" t="s">
         <v>414</v>
       </c>
       <c r="H7" s="40" t="s">
@@ -9379,11 +9432,11 @@
       <c r="B8" s="41" t="s">
         <v>331</v>
       </c>
-      <c r="C8" s="76"/>
-      <c r="D8" s="76"/>
-      <c r="E8" s="76"/>
-      <c r="F8" s="76"/>
-      <c r="G8" s="76"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="69"/>
       <c r="H8" s="40" t="s">
         <v>337</v>
       </c>
@@ -9415,11 +9468,11 @@
       <c r="B9" s="41" t="s">
         <v>283</v>
       </c>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="76"/>
-      <c r="F9" s="76"/>
-      <c r="G9" s="76"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
       <c r="H9" s="40" t="s">
         <v>282</v>
       </c>
@@ -9451,11 +9504,11 @@
       <c r="B10" s="41" t="s">
         <v>285</v>
       </c>
-      <c r="C10" s="76"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="76"/>
-      <c r="G10" s="76"/>
+      <c r="C10" s="69"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
       <c r="H10" s="40" t="s">
         <v>284</v>
       </c>
@@ -9487,11 +9540,11 @@
       <c r="B11" s="41" t="s">
         <v>287</v>
       </c>
-      <c r="C11" s="76"/>
-      <c r="D11" s="76"/>
-      <c r="E11" s="76"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76"/>
+      <c r="C11" s="69"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69"/>
       <c r="H11" s="40" t="s">
         <v>286</v>
       </c>
@@ -9523,19 +9576,19 @@
       <c r="B12" s="41" t="s">
         <v>289</v>
       </c>
-      <c r="C12" s="77" t="s">
+      <c r="C12" s="70" t="s">
         <v>400</v>
       </c>
-      <c r="D12" s="77" t="s">
+      <c r="D12" s="70" t="s">
         <v>401</v>
       </c>
-      <c r="E12" s="77" t="s">
+      <c r="E12" s="70" t="s">
         <v>402</v>
       </c>
-      <c r="F12" s="77" t="s">
+      <c r="F12" s="70" t="s">
         <v>403</v>
       </c>
-      <c r="G12" s="77" t="s">
+      <c r="G12" s="70" t="s">
         <v>404</v>
       </c>
       <c r="H12" s="40" t="s">
@@ -9569,19 +9622,19 @@
       <c r="B13" s="41" t="s">
         <v>291</v>
       </c>
-      <c r="C13" s="75" t="s">
+      <c r="C13" s="68" t="s">
         <v>410</v>
       </c>
-      <c r="D13" s="75" t="s">
+      <c r="D13" s="68" t="s">
         <v>411</v>
       </c>
-      <c r="E13" s="75" t="s">
+      <c r="E13" s="68" t="s">
         <v>412</v>
       </c>
-      <c r="F13" s="75" t="s">
+      <c r="F13" s="68" t="s">
         <v>413</v>
       </c>
-      <c r="G13" s="75" t="s">
+      <c r="G13" s="68" t="s">
         <v>414</v>
       </c>
       <c r="H13" s="40" t="s">
@@ -9615,19 +9668,19 @@
       <c r="B14" s="41" t="s">
         <v>293</v>
       </c>
-      <c r="C14" s="79" t="s">
+      <c r="C14" s="72" t="s">
         <v>405</v>
       </c>
-      <c r="D14" s="75" t="s">
+      <c r="D14" s="68" t="s">
         <v>406</v>
       </c>
-      <c r="E14" s="80" t="s">
+      <c r="E14" s="73" t="s">
         <v>407</v>
       </c>
-      <c r="F14" s="80" t="s">
+      <c r="F14" s="73" t="s">
         <v>408</v>
       </c>
-      <c r="G14" s="80" t="s">
+      <c r="G14" s="73" t="s">
         <v>409</v>
       </c>
       <c r="H14" s="40" t="s">
@@ -9661,19 +9714,19 @@
       <c r="B15" s="41" t="s">
         <v>295</v>
       </c>
-      <c r="C15" s="77" t="s">
+      <c r="C15" s="70" t="s">
         <v>400</v>
       </c>
-      <c r="D15" s="77" t="s">
+      <c r="D15" s="70" t="s">
         <v>401</v>
       </c>
-      <c r="E15" s="77" t="s">
+      <c r="E15" s="70" t="s">
         <v>402</v>
       </c>
-      <c r="F15" s="77" t="s">
+      <c r="F15" s="70" t="s">
         <v>403</v>
       </c>
-      <c r="G15" s="77" t="s">
+      <c r="G15" s="70" t="s">
         <v>404</v>
       </c>
       <c r="H15" s="40" t="s">
@@ -9707,11 +9760,11 @@
       <c r="B16" s="41" t="s">
         <v>297</v>
       </c>
-      <c r="C16" s="76"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="76"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="69"/>
       <c r="H16" s="40" t="s">
         <v>296</v>
       </c>
@@ -9743,19 +9796,19 @@
       <c r="B17" s="41" t="s">
         <v>299</v>
       </c>
-      <c r="C17" s="77" t="s">
+      <c r="C17" s="70" t="s">
         <v>400</v>
       </c>
-      <c r="D17" s="77" t="s">
+      <c r="D17" s="70" t="s">
         <v>401</v>
       </c>
-      <c r="E17" s="77" t="s">
+      <c r="E17" s="70" t="s">
         <v>402</v>
       </c>
-      <c r="F17" s="77" t="s">
+      <c r="F17" s="70" t="s">
         <v>403</v>
       </c>
-      <c r="G17" s="77" t="s">
+      <c r="G17" s="70" t="s">
         <v>404</v>
       </c>
       <c r="H17" s="40" t="s">
@@ -9789,19 +9842,19 @@
       <c r="B18" s="41" t="s">
         <v>301</v>
       </c>
-      <c r="C18" s="75" t="s">
+      <c r="C18" s="68" t="s">
         <v>410</v>
       </c>
-      <c r="D18" s="75" t="s">
+      <c r="D18" s="68" t="s">
         <v>411</v>
       </c>
-      <c r="E18" s="75" t="s">
+      <c r="E18" s="68" t="s">
         <v>412</v>
       </c>
-      <c r="F18" s="75" t="s">
+      <c r="F18" s="68" t="s">
         <v>413</v>
       </c>
-      <c r="G18" s="75" t="s">
+      <c r="G18" s="68" t="s">
         <v>414</v>
       </c>
       <c r="H18" s="40" t="s">
@@ -9835,11 +9888,11 @@
       <c r="B19" s="41" t="s">
         <v>303</v>
       </c>
-      <c r="C19" s="76"/>
-      <c r="D19" s="76"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="76"/>
-      <c r="G19" s="76"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
       <c r="H19" s="40" t="s">
         <v>302</v>
       </c>
@@ -9871,11 +9924,11 @@
       <c r="B20" s="41" t="s">
         <v>305</v>
       </c>
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="76"/>
-      <c r="G20" s="76"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="69"/>
       <c r="H20" s="40" t="s">
         <v>304</v>
       </c>
@@ -9907,11 +9960,11 @@
       <c r="B21" s="41" t="s">
         <v>307</v>
       </c>
-      <c r="C21" s="76"/>
-      <c r="D21" s="76"/>
-      <c r="E21" s="76"/>
-      <c r="F21" s="76"/>
-      <c r="G21" s="76"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
       <c r="H21" s="40" t="s">
         <v>306</v>
       </c>
@@ -9943,19 +9996,19 @@
       <c r="B22" s="41" t="s">
         <v>309</v>
       </c>
-      <c r="C22" s="77" t="s">
+      <c r="C22" s="70" t="s">
         <v>400</v>
       </c>
-      <c r="D22" s="77" t="s">
+      <c r="D22" s="70" t="s">
         <v>401</v>
       </c>
-      <c r="E22" s="77" t="s">
+      <c r="E22" s="70" t="s">
         <v>402</v>
       </c>
-      <c r="F22" s="77" t="s">
+      <c r="F22" s="70" t="s">
         <v>403</v>
       </c>
-      <c r="G22" s="77" t="s">
+      <c r="G22" s="70" t="s">
         <v>404</v>
       </c>
       <c r="H22" s="40" t="s">

</xml_diff>

<commit_message>
added hi-IN translations of the hbsc pages
</commit_message>
<xml_diff>
--- a/GACPAQ pages.xlsx
+++ b/GACPAQ pages.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doncastillo/Code/gacpaq/gacpaq-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4135D3-E23E-244F-A21D-C8033B9E2865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9311C3C1-6F9B-B14D-B01D-82E8BE979850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20140" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24100" activeTab="5" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="423">
   <si>
     <t>Page Number</t>
   </si>
@@ -2881,6 +2881,9 @@
   </si>
   <si>
     <t>en-IN</t>
+  </si>
+  <si>
+    <t>available</t>
   </si>
 </sst>
 </file>
@@ -7765,7 +7768,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8320,8 +8323,12 @@
       <c r="G10" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="H10" s="55"/>
-      <c r="I10" s="55"/>
+      <c r="H10" s="54" t="s">
+        <v>422</v>
+      </c>
+      <c r="I10" s="54" t="s">
+        <v>422</v>
+      </c>
       <c r="J10" s="55"/>
       <c r="K10" s="55"/>
       <c r="L10" s="40" t="s">

</xml_diff>

<commit_message>
added hi-IN translations of the gshs pages
</commit_message>
<xml_diff>
--- a/GACPAQ pages.xlsx
+++ b/GACPAQ pages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doncastillo/Code/gacpaq/gacpaq-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9311C3C1-6F9B-B14D-B01D-82E8BE979850}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9155F6DF-D721-054E-8C5F-91177BD651F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="24100" activeTab="5" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
+    <workbookView xWindow="-20140" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="952" uniqueCount="422">
   <si>
     <t>Page Number</t>
   </si>
@@ -2881,9 +2881,6 @@
   </si>
   <si>
     <t>en-IN</t>
-  </si>
-  <si>
-    <t>available</t>
   </si>
 </sst>
 </file>
@@ -7768,7 +7765,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8323,11 +8320,11 @@
       <c r="G10" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="H10" s="54" t="s">
-        <v>422</v>
-      </c>
-      <c r="I10" s="54" t="s">
-        <v>422</v>
+      <c r="H10" s="53" t="s">
+        <v>338</v>
+      </c>
+      <c r="I10" s="53" t="s">
+        <v>338</v>
       </c>
       <c r="J10" s="55"/>
       <c r="K10" s="55"/>

</xml_diff>

<commit_message>
added NZ adolescent/parent section images
</commit_message>
<xml_diff>
--- a/GACPAQ pages.xlsx
+++ b/GACPAQ pages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doncastillo/Code/gacpaq/gacpaq-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECCE7CA-C054-E74D-8639-9023F34E85A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBF6F88-2805-B94A-A752-705BDD541E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18800" yWindow="-20800" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
+    <workbookView xWindow="-20140" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="422">
   <si>
     <t>Page Number</t>
   </si>
@@ -2544,9 +2544,6 @@
     <t>deployed</t>
   </si>
   <si>
-    <t>awaiting  data</t>
-  </si>
-  <si>
     <t>collecting feedback, revision ongoing</t>
   </si>
   <si>
@@ -2685,9 +2682,6 @@
     <t>on-going (3)</t>
   </si>
   <si>
-    <t>waiting for images to be processed</t>
-  </si>
-  <si>
     <t>on-going (4)</t>
   </si>
   <si>
@@ -2881,6 +2875,12 @@
   </si>
   <si>
     <t>en-IN</t>
+  </si>
+  <si>
+    <t>available</t>
+  </si>
+  <si>
+    <t>adopt from es-ES</t>
   </si>
 </sst>
 </file>
@@ -5977,10 +5977,10 @@
         <v>102</v>
       </c>
       <c r="F72" s="13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="73" spans="1:11">
@@ -5991,10 +5991,10 @@
         <v>216</v>
       </c>
       <c r="F73" s="13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="74" spans="1:11">
@@ -6005,10 +6005,10 @@
         <v>25</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H74" s="13" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="75" spans="1:11">
@@ -6019,10 +6019,10 @@
         <v>26</v>
       </c>
       <c r="F75" s="13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H75" s="13" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="76" spans="1:11">
@@ -6033,10 +6033,10 @@
         <v>51</v>
       </c>
       <c r="F76" s="13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H76" s="13" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="77" spans="1:11">
@@ -6047,10 +6047,10 @@
         <v>102</v>
       </c>
       <c r="F77" s="13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H77" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="78" spans="1:11">
@@ -6058,13 +6058,13 @@
         <v>333</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F78" s="13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H78" s="13" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="79" spans="1:11">
@@ -6075,10 +6075,10 @@
         <v>25</v>
       </c>
       <c r="F79" s="13" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H79" s="13" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="80" spans="1:11">
@@ -6089,10 +6089,10 @@
         <v>26</v>
       </c>
       <c r="F80" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="17" customHeight="1">
@@ -6103,10 +6103,10 @@
         <v>27</v>
       </c>
       <c r="F81" s="13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H81" s="13" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -6117,10 +6117,10 @@
         <v>28</v>
       </c>
       <c r="F82" s="13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H82" s="63" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -6128,13 +6128,13 @@
         <v>333</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F83" s="13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H83" s="13" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="84" spans="1:8">
@@ -6145,10 +6145,10 @@
         <v>29</v>
       </c>
       <c r="F84" s="13" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="85" spans="1:8">
@@ -6156,13 +6156,13 @@
         <v>333</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F85" s="13" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="86" spans="1:8">
@@ -6173,10 +6173,10 @@
         <v>30</v>
       </c>
       <c r="F86" s="13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H86" s="13" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="87" spans="1:8">
@@ -6187,15 +6187,15 @@
         <v>51</v>
       </c>
       <c r="F87" s="13" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H87" s="13" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="88" spans="1:8">
       <c r="A88" s="21" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -6224,19 +6224,19 @@
         <v>25</v>
       </c>
       <c r="D2" t="s">
+        <v>383</v>
+      </c>
+      <c r="E2" t="s">
         <v>384</v>
-      </c>
-      <c r="E2" t="s">
-        <v>385</v>
       </c>
       <c r="H2" t="s">
         <v>25</v>
       </c>
       <c r="I2" t="s">
+        <v>383</v>
+      </c>
+      <c r="J2" t="s">
         <v>384</v>
-      </c>
-      <c r="J2" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -6244,13 +6244,13 @@
         <v>335</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="J3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -6273,13 +6273,13 @@
         <v>334</v>
       </c>
       <c r="H4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="J4" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -6403,7 +6403,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="22" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B12" s="35">
         <v>8</v>
@@ -6457,7 +6457,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="21" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B16" s="35">
         <v>11</v>
@@ -7765,7 +7765,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9:I9"/>
+      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7888,7 +7888,7 @@
         <v>344</v>
       </c>
       <c r="K2" s="56" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="L2" s="40" t="s">
         <v>269</v>
@@ -7946,7 +7946,7 @@
         <v>344</v>
       </c>
       <c r="K3" s="56" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="L3" s="40" t="s">
         <v>271</v>
@@ -8004,7 +8004,7 @@
         <v>344</v>
       </c>
       <c r="K4" s="56" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="L4" s="40" t="s">
         <v>273</v>
@@ -8044,14 +8044,18 @@
         <v>338</v>
       </c>
       <c r="E5" s="57" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F5" s="56" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="G5" s="55"/>
-      <c r="H5" s="55"/>
-      <c r="I5" s="55"/>
+      <c r="H5" s="55" t="s">
+        <v>421</v>
+      </c>
+      <c r="I5" s="55" t="s">
+        <v>421</v>
+      </c>
       <c r="J5" s="55"/>
       <c r="K5" s="55"/>
       <c r="L5" s="40" t="s">
@@ -8110,7 +8114,7 @@
         <v>344</v>
       </c>
       <c r="K6" s="56" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="L6" s="40" t="s">
         <v>276</v>
@@ -8168,7 +8172,7 @@
         <v>344</v>
       </c>
       <c r="K7" s="56" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="L7" s="40" t="s">
         <v>278</v>
@@ -8217,10 +8221,10 @@
         <v>338</v>
       </c>
       <c r="H8" s="56" t="s">
-        <v>345</v>
+        <v>420</v>
       </c>
       <c r="I8" s="56" t="s">
-        <v>345</v>
+        <v>420</v>
       </c>
       <c r="J8" s="55"/>
       <c r="K8" s="55"/>
@@ -8250,10 +8254,10 @@
     </row>
     <row r="9" spans="1:36" ht="27" customHeight="1">
       <c r="A9" s="40" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="B9" s="41" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C9" s="53" t="s">
         <v>338</v>
@@ -8279,7 +8283,7 @@
       <c r="J9" s="55"/>
       <c r="K9" s="55"/>
       <c r="L9" s="40" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="M9" s="48"/>
       <c r="N9" s="48"/>
@@ -8319,7 +8323,7 @@
         <v>338</v>
       </c>
       <c r="F10" s="57" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G10" s="53" t="s">
         <v>338</v>
@@ -8373,10 +8377,10 @@
         <v>338</v>
       </c>
       <c r="F11" s="57" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G11" s="56" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="H11" s="55"/>
       <c r="I11" s="55"/>
@@ -8435,7 +8439,7 @@
         <v>338</v>
       </c>
       <c r="J12" s="56" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="K12" s="55"/>
       <c r="L12" s="40" t="s">
@@ -8491,7 +8495,7 @@
         <v>338</v>
       </c>
       <c r="J13" s="56" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="K13" s="55"/>
       <c r="L13" s="40" t="s">
@@ -8550,7 +8554,7 @@
         <v>344</v>
       </c>
       <c r="K14" s="56" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="L14" s="40" t="s">
         <v>290</v>
@@ -8608,7 +8612,7 @@
         <v>344</v>
       </c>
       <c r="K15" s="56" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="L15" s="40" t="s">
         <v>292</v>
@@ -8644,14 +8648,14 @@
       <c r="C16" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="D16" s="56" t="s">
-        <v>392</v>
+      <c r="D16" s="53" t="s">
+        <v>338</v>
       </c>
       <c r="E16" s="53" t="s">
         <v>338</v>
       </c>
       <c r="F16" s="57" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G16" s="55"/>
       <c r="H16" s="53" t="s">
@@ -8696,11 +8700,11 @@
       <c r="C17" s="53" t="s">
         <v>338</v>
       </c>
-      <c r="D17" s="56" t="s">
-        <v>392</v>
+      <c r="D17" s="53" t="s">
+        <v>338</v>
       </c>
       <c r="E17" s="57" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F17" s="58"/>
       <c r="G17" s="55"/>
@@ -8768,7 +8772,7 @@
         <v>344</v>
       </c>
       <c r="K18" s="56" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="L18" s="40" t="s">
         <v>298</v>
@@ -8826,7 +8830,7 @@
         <v>344</v>
       </c>
       <c r="K19" s="54" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L19" s="40" t="s">
         <v>300</v>
@@ -8884,7 +8888,7 @@
         <v>344</v>
       </c>
       <c r="K20" s="56" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L20" s="40" t="s">
         <v>302</v>
@@ -8942,7 +8946,7 @@
         <v>344</v>
       </c>
       <c r="K21" s="56" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="L21" s="40" t="s">
         <v>304</v>
@@ -9000,7 +9004,7 @@
         <v>344</v>
       </c>
       <c r="K22" s="56" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="L22" s="40" t="s">
         <v>306</v>
@@ -9058,7 +9062,7 @@
         <v>344</v>
       </c>
       <c r="K23" s="56" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="L23" s="40" t="s">
         <v>308</v>
@@ -9135,19 +9139,19 @@
       <c r="A1" s="47"/>
       <c r="B1" s="47"/>
       <c r="C1" s="67" t="s">
+        <v>398</v>
+      </c>
+      <c r="D1" s="67" t="s">
+        <v>399</v>
+      </c>
+      <c r="E1" s="67" t="s">
         <v>400</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="F1" s="67" t="s">
         <v>401</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="G1" s="67" t="s">
         <v>402</v>
-      </c>
-      <c r="F1" s="67" t="s">
-        <v>403</v>
-      </c>
-      <c r="G1" s="67" t="s">
-        <v>404</v>
       </c>
       <c r="H1" s="47"/>
       <c r="I1" s="49"/>
@@ -9185,19 +9189,19 @@
         <v>270</v>
       </c>
       <c r="C2" s="68" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="D2" s="68" t="s">
+        <v>413</v>
+      </c>
+      <c r="E2" s="68" t="s">
+        <v>414</v>
+      </c>
+      <c r="F2" s="68" t="s">
         <v>415</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="G2" s="68" t="s">
         <v>416</v>
-      </c>
-      <c r="F2" s="68" t="s">
-        <v>417</v>
-      </c>
-      <c r="G2" s="68" t="s">
-        <v>418</v>
       </c>
       <c r="H2" s="40" t="s">
         <v>269</v>
@@ -9231,19 +9235,19 @@
         <v>272</v>
       </c>
       <c r="C3" s="70" t="s">
+        <v>398</v>
+      </c>
+      <c r="D3" s="70" t="s">
+        <v>399</v>
+      </c>
+      <c r="E3" s="70" t="s">
         <v>400</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="F3" s="70" t="s">
         <v>401</v>
       </c>
-      <c r="E3" s="70" t="s">
+      <c r="G3" s="70" t="s">
         <v>402</v>
-      </c>
-      <c r="F3" s="70" t="s">
-        <v>403</v>
-      </c>
-      <c r="G3" s="70" t="s">
-        <v>404</v>
       </c>
       <c r="H3" s="40" t="s">
         <v>271</v>
@@ -9313,19 +9317,19 @@
         <v>330</v>
       </c>
       <c r="C5" s="68" t="s">
+        <v>408</v>
+      </c>
+      <c r="D5" s="68" t="s">
+        <v>409</v>
+      </c>
+      <c r="E5" s="68" t="s">
         <v>410</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="F5" s="68" t="s">
         <v>411</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="G5" s="68" t="s">
         <v>412</v>
-      </c>
-      <c r="F5" s="68" t="s">
-        <v>413</v>
-      </c>
-      <c r="G5" s="68" t="s">
-        <v>414</v>
       </c>
       <c r="H5" s="40" t="s">
         <v>336</v>
@@ -9395,19 +9399,19 @@
         <v>279</v>
       </c>
       <c r="C7" s="68" t="s">
+        <v>408</v>
+      </c>
+      <c r="D7" s="68" t="s">
+        <v>409</v>
+      </c>
+      <c r="E7" s="68" t="s">
         <v>410</v>
       </c>
-      <c r="D7" s="68" t="s">
+      <c r="F7" s="68" t="s">
         <v>411</v>
       </c>
-      <c r="E7" s="68" t="s">
+      <c r="G7" s="68" t="s">
         <v>412</v>
-      </c>
-      <c r="F7" s="68" t="s">
-        <v>413</v>
-      </c>
-      <c r="G7" s="68" t="s">
-        <v>414</v>
       </c>
       <c r="H7" s="40" t="s">
         <v>278</v>
@@ -9585,19 +9589,19 @@
         <v>289</v>
       </c>
       <c r="C12" s="70" t="s">
+        <v>398</v>
+      </c>
+      <c r="D12" s="70" t="s">
+        <v>399</v>
+      </c>
+      <c r="E12" s="70" t="s">
         <v>400</v>
       </c>
-      <c r="D12" s="70" t="s">
+      <c r="F12" s="70" t="s">
         <v>401</v>
       </c>
-      <c r="E12" s="70" t="s">
+      <c r="G12" s="70" t="s">
         <v>402</v>
-      </c>
-      <c r="F12" s="70" t="s">
-        <v>403</v>
-      </c>
-      <c r="G12" s="70" t="s">
-        <v>404</v>
       </c>
       <c r="H12" s="40" t="s">
         <v>288</v>
@@ -9631,19 +9635,19 @@
         <v>291</v>
       </c>
       <c r="C13" s="68" t="s">
+        <v>408</v>
+      </c>
+      <c r="D13" s="68" t="s">
+        <v>409</v>
+      </c>
+      <c r="E13" s="68" t="s">
         <v>410</v>
       </c>
-      <c r="D13" s="68" t="s">
+      <c r="F13" s="68" t="s">
         <v>411</v>
       </c>
-      <c r="E13" s="68" t="s">
+      <c r="G13" s="68" t="s">
         <v>412</v>
-      </c>
-      <c r="F13" s="68" t="s">
-        <v>413</v>
-      </c>
-      <c r="G13" s="68" t="s">
-        <v>414</v>
       </c>
       <c r="H13" s="40" t="s">
         <v>290</v>
@@ -9677,19 +9681,19 @@
         <v>293</v>
       </c>
       <c r="C14" s="72" t="s">
+        <v>403</v>
+      </c>
+      <c r="D14" s="68" t="s">
+        <v>404</v>
+      </c>
+      <c r="E14" s="73" t="s">
         <v>405</v>
       </c>
-      <c r="D14" s="68" t="s">
+      <c r="F14" s="73" t="s">
         <v>406</v>
       </c>
-      <c r="E14" s="73" t="s">
+      <c r="G14" s="73" t="s">
         <v>407</v>
-      </c>
-      <c r="F14" s="73" t="s">
-        <v>408</v>
-      </c>
-      <c r="G14" s="73" t="s">
-        <v>409</v>
       </c>
       <c r="H14" s="40" t="s">
         <v>292</v>
@@ -9723,19 +9727,19 @@
         <v>295</v>
       </c>
       <c r="C15" s="70" t="s">
+        <v>398</v>
+      </c>
+      <c r="D15" s="70" t="s">
+        <v>399</v>
+      </c>
+      <c r="E15" s="70" t="s">
         <v>400</v>
       </c>
-      <c r="D15" s="70" t="s">
+      <c r="F15" s="70" t="s">
         <v>401</v>
       </c>
-      <c r="E15" s="70" t="s">
+      <c r="G15" s="70" t="s">
         <v>402</v>
-      </c>
-      <c r="F15" s="70" t="s">
-        <v>403</v>
-      </c>
-      <c r="G15" s="70" t="s">
-        <v>404</v>
       </c>
       <c r="H15" s="40" t="s">
         <v>294</v>
@@ -9805,19 +9809,19 @@
         <v>299</v>
       </c>
       <c r="C17" s="70" t="s">
+        <v>398</v>
+      </c>
+      <c r="D17" s="70" t="s">
+        <v>399</v>
+      </c>
+      <c r="E17" s="70" t="s">
         <v>400</v>
       </c>
-      <c r="D17" s="70" t="s">
+      <c r="F17" s="70" t="s">
         <v>401</v>
       </c>
-      <c r="E17" s="70" t="s">
+      <c r="G17" s="70" t="s">
         <v>402</v>
-      </c>
-      <c r="F17" s="70" t="s">
-        <v>403</v>
-      </c>
-      <c r="G17" s="70" t="s">
-        <v>404</v>
       </c>
       <c r="H17" s="40" t="s">
         <v>298</v>
@@ -9851,19 +9855,19 @@
         <v>301</v>
       </c>
       <c r="C18" s="68" t="s">
+        <v>408</v>
+      </c>
+      <c r="D18" s="68" t="s">
+        <v>409</v>
+      </c>
+      <c r="E18" s="68" t="s">
         <v>410</v>
       </c>
-      <c r="D18" s="68" t="s">
+      <c r="F18" s="68" t="s">
         <v>411</v>
       </c>
-      <c r="E18" s="68" t="s">
+      <c r="G18" s="68" t="s">
         <v>412</v>
-      </c>
-      <c r="F18" s="68" t="s">
-        <v>413</v>
-      </c>
-      <c r="G18" s="68" t="s">
-        <v>414</v>
       </c>
       <c r="H18" s="40" t="s">
         <v>300</v>
@@ -10005,19 +10009,19 @@
         <v>309</v>
       </c>
       <c r="C22" s="70" t="s">
+        <v>398</v>
+      </c>
+      <c r="D22" s="70" t="s">
+        <v>399</v>
+      </c>
+      <c r="E22" s="70" t="s">
         <v>400</v>
       </c>
-      <c r="D22" s="70" t="s">
+      <c r="F22" s="70" t="s">
         <v>401</v>
       </c>
-      <c r="E22" s="70" t="s">
+      <c r="G22" s="70" t="s">
         <v>402</v>
-      </c>
-      <c r="F22" s="70" t="s">
-        <v>403</v>
-      </c>
-      <c r="G22" s="70" t="s">
-        <v>404</v>
       </c>
       <c r="H22" s="40" t="s">
         <v>308</v>

</xml_diff>

<commit_message>
updated the GAC-PAQ pages
</commit_message>
<xml_diff>
--- a/GACPAQ pages.xlsx
+++ b/GACPAQ pages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doncastillo/Code/gacpaq/gacpaq-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DBF6F88-2805-B94A-A752-705BDD541E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B92EE8-3CAD-5C45-9825-9858025E5563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20140" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
+    <workbookView xWindow="21660" yWindow="-17960" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2267,620 +2267,620 @@
     <t>14 - Work / Volunteering</t>
   </si>
   <si>
-    <t>transportation_10
+    <t>Option Images</t>
+  </si>
+  <si>
+    <t>Section Images</t>
+  </si>
+  <si>
+    <t>page 5</t>
+  </si>
+  <si>
+    <t>page 7</t>
+  </si>
+  <si>
+    <t>page 11</t>
+  </si>
+  <si>
+    <t>page 14</t>
+  </si>
+  <si>
+    <t>school</t>
+  </si>
+  <si>
+    <t>chores</t>
+  </si>
+  <si>
+    <t>work</t>
+  </si>
+  <si>
+    <t>transportation</t>
+  </si>
+  <si>
+    <t>organized activities</t>
+  </si>
+  <si>
+    <t>play or free time</t>
+  </si>
+  <si>
+    <t>outdoors</t>
+  </si>
+  <si>
+    <t>phone</t>
+  </si>
+  <si>
+    <t>tablet</t>
+  </si>
+  <si>
+    <t>Brazil - Portugese</t>
+  </si>
+  <si>
+    <t>pt-BR</t>
+  </si>
+  <si>
+    <t>Canada - English</t>
+  </si>
+  <si>
+    <t>en-CA</t>
+  </si>
+  <si>
+    <t>Canada - French</t>
+  </si>
+  <si>
+    <t>fr-CA</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>China - Chinese</t>
+  </si>
+  <si>
+    <t>zh-CN</t>
+  </si>
+  <si>
+    <t>Colombia - Spanish</t>
+  </si>
+  <si>
+    <t>es-CO</t>
+  </si>
+  <si>
+    <t>Czech Republic</t>
+  </si>
+  <si>
+    <t>CZ</t>
+  </si>
+  <si>
+    <t>India - Hindi</t>
+  </si>
+  <si>
+    <t>hi-IN</t>
+  </si>
+  <si>
+    <t>India - Marathi</t>
+  </si>
+  <si>
+    <t>ma-IN</t>
+  </si>
+  <si>
+    <t>Malawi - Chichewa</t>
+  </si>
+  <si>
+    <t>ch-MW</t>
+  </si>
+  <si>
+    <t>Malawi - English</t>
+  </si>
+  <si>
+    <t>en-MW</t>
+  </si>
+  <si>
+    <t>Mexico - Spanish</t>
+  </si>
+  <si>
+    <t>es-MX</t>
+  </si>
+  <si>
+    <t>Nepal - Nepali</t>
+  </si>
+  <si>
+    <t>ne-NP</t>
+  </si>
+  <si>
+    <t>New Zealand - English</t>
+  </si>
+  <si>
+    <t>en-NZ</t>
+  </si>
+  <si>
+    <t>New Zealand - Maori</t>
+  </si>
+  <si>
+    <t>mi-NZ</t>
+  </si>
+  <si>
+    <t>Nigeria - English</t>
+  </si>
+  <si>
+    <t>en-NG</t>
+  </si>
+  <si>
+    <t>Spain - Spanish</t>
+  </si>
+  <si>
+    <t>es-ES</t>
+  </si>
+  <si>
+    <t>Sweden - Swedish</t>
+  </si>
+  <si>
+    <t>sv-SE</t>
+  </si>
+  <si>
+    <t>Thailand - Thai</t>
+  </si>
+  <si>
+    <t>th-TH</t>
+  </si>
+  <si>
+    <t>UAE - Arabic</t>
+  </si>
+  <si>
+    <t>ar-AE</t>
+  </si>
+  <si>
+    <t>UAE - English</t>
+  </si>
+  <si>
+    <t>en-AE</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>extro</t>
+  </si>
+  <si>
+    <t>demographics</t>
+  </si>
+  <si>
+    <t>child</t>
+  </si>
+  <si>
+    <t>adolescent</t>
+  </si>
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Malawi</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Sweden</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>UAE</t>
+  </si>
+  <si>
+    <t>es-CL</t>
+  </si>
+  <si>
+    <t>cz-CR</t>
+  </si>
+  <si>
+    <t>HBSC</t>
+  </si>
+  <si>
+    <t>GSHS</t>
+  </si>
+  <si>
+    <t>Pilot Study</t>
+  </si>
+  <si>
+    <t>Main Study</t>
+  </si>
+  <si>
+    <t>Chile - Spanish</t>
+  </si>
+  <si>
+    <t>Czech Republic - Czech</t>
+  </si>
+  <si>
+    <t>completed</t>
+  </si>
+  <si>
+    <t>Narration entered</t>
+  </si>
+  <si>
+    <t>Text translations entered</t>
+  </si>
+  <si>
+    <t>App Review</t>
+  </si>
+  <si>
+    <t>Images entered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Preparing app for Main Study </t>
+  </si>
+  <si>
+    <t>deployed</t>
+  </si>
+  <si>
+    <t>collecting feedback, revision ongoing</t>
+  </si>
+  <si>
+    <t>awaiting data; narration processing</t>
+  </si>
+  <si>
+    <t>Preamble - PA</t>
+  </si>
+  <si>
+    <t>Preamble - Sitting</t>
+  </si>
+  <si>
+    <t>Preamble - Sleep</t>
+  </si>
+  <si>
+    <t>hbsc_intro</t>
+  </si>
+  <si>
+    <t>hbsc_preamble</t>
+  </si>
+  <si>
+    <t>hbsc_1</t>
+  </si>
+  <si>
+    <t>hbsc_2</t>
+  </si>
+  <si>
+    <t>hbsc_extro</t>
+  </si>
+  <si>
+    <t>gshs_intro</t>
+  </si>
+  <si>
+    <t>gshs_preamble_pa</t>
+  </si>
+  <si>
+    <t>gshs_1</t>
+  </si>
+  <si>
+    <t>gshs_2</t>
+  </si>
+  <si>
+    <t>gshs_3</t>
+  </si>
+  <si>
+    <t>gshs_4</t>
+  </si>
+  <si>
+    <t>gshs_preamble_sitting</t>
+  </si>
+  <si>
+    <t>gshs_5</t>
+  </si>
+  <si>
+    <t>gshs_preamble_sleep</t>
+  </si>
+  <si>
+    <t>gshs_6</t>
+  </si>
+  <si>
+    <t>gshs_extro</t>
+  </si>
+  <si>
+    <t>HBSCIntro</t>
+  </si>
+  <si>
+    <t>HBSCPreamble</t>
+  </si>
+  <si>
+    <t>HBSC1</t>
+  </si>
+  <si>
+    <t>HBSC2</t>
+  </si>
+  <si>
+    <t>HBSCExtro</t>
+  </si>
+  <si>
+    <t>GSHSIntro</t>
+  </si>
+  <si>
+    <t>GSHSPreamble_PA</t>
+  </si>
+  <si>
+    <t>GSHS1</t>
+  </si>
+  <si>
+    <t>GSHS2</t>
+  </si>
+  <si>
+    <t>GSHS3</t>
+  </si>
+  <si>
+    <t>GSHS4</t>
+  </si>
+  <si>
+    <t>GSHSPreamble_Sitting</t>
+  </si>
+  <si>
+    <t>GSHS5</t>
+  </si>
+  <si>
+    <t>GSHSPreamble_Sleep</t>
+  </si>
+  <si>
+    <t>GSHS6</t>
+  </si>
+  <si>
+    <t>GSHSExtro</t>
+  </si>
+  <si>
+    <t>AppExtro</t>
+  </si>
+  <si>
+    <t>Adolescent</t>
+  </si>
+  <si>
+    <t>Parent</t>
+  </si>
+  <si>
+    <t>Extro (demo)</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>in review</t>
+  </si>
+  <si>
+    <t>on-going (1)</t>
+  </si>
+  <si>
+    <t>on-going (2)</t>
+  </si>
+  <si>
+    <t>on-going (3)</t>
+  </si>
+  <si>
+    <t>on-going (4)</t>
+  </si>
+  <si>
+    <t>on-going (5)</t>
+  </si>
+  <si>
+    <t>on-going (6)</t>
+  </si>
+  <si>
+    <t>on-going (7)</t>
+  </si>
+  <si>
+    <t>on-going (8)</t>
+  </si>
+  <si>
+    <t>on-going (9)</t>
+  </si>
+  <si>
+    <t>on-going (10)</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>No pending submissions</t>
+  </si>
+  <si>
+    <t>Nothing to submit</t>
+  </si>
+  <si>
+    <t>Pending Submissions</t>
+  </si>
+  <si>
+    <t>Responses submitted</t>
+  </si>
+  <si>
+    <t>बुझाउनुहोस्</t>
+  </si>
+  <si>
+    <t>बुझाउनु पर्ने केहि बाँकी छैन</t>
+  </si>
+  <si>
+    <r>
+      <t>बुझाउनु</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Preeti"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>पर्ने</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Preeti"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>केहि</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Preeti"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>छैन</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>बुझाउन</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Preeti"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>बाँकी</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Preeti"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>छ</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>प्रतिकृया</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Preeti"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">बुझाइयो </t>
+    </r>
+  </si>
+  <si>
+    <t>Enviar</t>
+  </si>
+  <si>
+    <t>No hay envíos pendientes</t>
+  </si>
+  <si>
+    <t>No hay nada para enviar</t>
+  </si>
+  <si>
+    <t>Envíos pendientes</t>
+  </si>
+  <si>
+    <t>Respuestas enviadas</t>
+  </si>
+  <si>
+    <t>Nenhuma submissão pendente</t>
+  </si>
+  <si>
+    <t>Nada a enviar</t>
+  </si>
+  <si>
+    <t>Submissões pendentes</t>
+  </si>
+  <si>
+    <t>Respostas enviadas</t>
+  </si>
+  <si>
+    <t>on-going</t>
+  </si>
+  <si>
+    <t>India - English</t>
+  </si>
+  <si>
+    <t>en-IN</t>
+  </si>
+  <si>
+    <t>available</t>
+  </si>
+  <si>
+    <t>adopt from es-ES</t>
+  </si>
+  <si>
+    <t>transportation_9
 (walk)</t>
-  </si>
-  <si>
-    <t>Option Images</t>
-  </si>
-  <si>
-    <t>Section Images</t>
-  </si>
-  <si>
-    <t>page 5</t>
-  </si>
-  <si>
-    <t>page 7</t>
-  </si>
-  <si>
-    <t>page 11</t>
-  </si>
-  <si>
-    <t>page 14</t>
-  </si>
-  <si>
-    <t>school</t>
-  </si>
-  <si>
-    <t>chores</t>
-  </si>
-  <si>
-    <t>work</t>
-  </si>
-  <si>
-    <t>transportation</t>
-  </si>
-  <si>
-    <t>organized activities</t>
-  </si>
-  <si>
-    <t>play or free time</t>
-  </si>
-  <si>
-    <t>outdoors</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>tablet</t>
-  </si>
-  <si>
-    <t>Brazil - Portugese</t>
-  </si>
-  <si>
-    <t>pt-BR</t>
-  </si>
-  <si>
-    <t>Canada - English</t>
-  </si>
-  <si>
-    <t>en-CA</t>
-  </si>
-  <si>
-    <t>Canada - French</t>
-  </si>
-  <si>
-    <t>fr-CA</t>
-  </si>
-  <si>
-    <t>Chile</t>
-  </si>
-  <si>
-    <t>China - Chinese</t>
-  </si>
-  <si>
-    <t>zh-CN</t>
-  </si>
-  <si>
-    <t>Colombia - Spanish</t>
-  </si>
-  <si>
-    <t>es-CO</t>
-  </si>
-  <si>
-    <t>Czech Republic</t>
-  </si>
-  <si>
-    <t>CZ</t>
-  </si>
-  <si>
-    <t>India - Hindi</t>
-  </si>
-  <si>
-    <t>hi-IN</t>
-  </si>
-  <si>
-    <t>India - Marathi</t>
-  </si>
-  <si>
-    <t>ma-IN</t>
-  </si>
-  <si>
-    <t>Malawi - Chichewa</t>
-  </si>
-  <si>
-    <t>ch-MW</t>
-  </si>
-  <si>
-    <t>Malawi - English</t>
-  </si>
-  <si>
-    <t>en-MW</t>
-  </si>
-  <si>
-    <t>Mexico - Spanish</t>
-  </si>
-  <si>
-    <t>es-MX</t>
-  </si>
-  <si>
-    <t>Nepal - Nepali</t>
-  </si>
-  <si>
-    <t>ne-NP</t>
-  </si>
-  <si>
-    <t>New Zealand - English</t>
-  </si>
-  <si>
-    <t>en-NZ</t>
-  </si>
-  <si>
-    <t>New Zealand - Maori</t>
-  </si>
-  <si>
-    <t>mi-NZ</t>
-  </si>
-  <si>
-    <t>Nigeria - English</t>
-  </si>
-  <si>
-    <t>en-NG</t>
-  </si>
-  <si>
-    <t>Spain - Spanish</t>
-  </si>
-  <si>
-    <t>es-ES</t>
-  </si>
-  <si>
-    <t>Sweden - Swedish</t>
-  </si>
-  <si>
-    <t>sv-SE</t>
-  </si>
-  <si>
-    <t>Thailand - Thai</t>
-  </si>
-  <si>
-    <t>th-TH</t>
-  </si>
-  <si>
-    <t>UAE - Arabic</t>
-  </si>
-  <si>
-    <t>ar-AE</t>
-  </si>
-  <si>
-    <t>UAE - English</t>
-  </si>
-  <si>
-    <t>en-AE</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
-    <t>extro</t>
-  </si>
-  <si>
-    <t>demographics</t>
-  </si>
-  <si>
-    <t>child</t>
-  </si>
-  <si>
-    <t>adolescent</t>
-  </si>
-  <si>
-    <t>parent</t>
-  </si>
-  <si>
-    <t>total</t>
-  </si>
-  <si>
-    <t>Brazil</t>
-  </si>
-  <si>
-    <t>Canada</t>
-  </si>
-  <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>Colombia</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>Malawi</t>
-  </si>
-  <si>
-    <t>Mexico</t>
-  </si>
-  <si>
-    <t>Nepal</t>
-  </si>
-  <si>
-    <t>Nigeria</t>
-  </si>
-  <si>
-    <t>Spain</t>
-  </si>
-  <si>
-    <t>Sweden</t>
-  </si>
-  <si>
-    <t>Thailand</t>
-  </si>
-  <si>
-    <t>UAE</t>
-  </si>
-  <si>
-    <t>es-CL</t>
-  </si>
-  <si>
-    <t>cz-CR</t>
-  </si>
-  <si>
-    <t>HBSC</t>
-  </si>
-  <si>
-    <t>GSHS</t>
-  </si>
-  <si>
-    <t>Pilot Study</t>
-  </si>
-  <si>
-    <t>Main Study</t>
-  </si>
-  <si>
-    <t>Chile - Spanish</t>
-  </si>
-  <si>
-    <t>Czech Republic - Czech</t>
-  </si>
-  <si>
-    <t>completed</t>
-  </si>
-  <si>
-    <t>Narration entered</t>
-  </si>
-  <si>
-    <t>Text translations entered</t>
-  </si>
-  <si>
-    <t>App Review</t>
-  </si>
-  <si>
-    <t>Images entered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Preparing app for Main Study </t>
-  </si>
-  <si>
-    <t>deployed</t>
-  </si>
-  <si>
-    <t>collecting feedback, revision ongoing</t>
-  </si>
-  <si>
-    <t>awaiting data; narration processing</t>
-  </si>
-  <si>
-    <t>Preamble - PA</t>
-  </si>
-  <si>
-    <t>Preamble - Sitting</t>
-  </si>
-  <si>
-    <t>Preamble - Sleep</t>
-  </si>
-  <si>
-    <t>hbsc_intro</t>
-  </si>
-  <si>
-    <t>hbsc_preamble</t>
-  </si>
-  <si>
-    <t>hbsc_1</t>
-  </si>
-  <si>
-    <t>hbsc_2</t>
-  </si>
-  <si>
-    <t>hbsc_extro</t>
-  </si>
-  <si>
-    <t>gshs_intro</t>
-  </si>
-  <si>
-    <t>gshs_preamble_pa</t>
-  </si>
-  <si>
-    <t>gshs_1</t>
-  </si>
-  <si>
-    <t>gshs_2</t>
-  </si>
-  <si>
-    <t>gshs_3</t>
-  </si>
-  <si>
-    <t>gshs_4</t>
-  </si>
-  <si>
-    <t>gshs_preamble_sitting</t>
-  </si>
-  <si>
-    <t>gshs_5</t>
-  </si>
-  <si>
-    <t>gshs_preamble_sleep</t>
-  </si>
-  <si>
-    <t>gshs_6</t>
-  </si>
-  <si>
-    <t>gshs_extro</t>
-  </si>
-  <si>
-    <t>HBSCIntro</t>
-  </si>
-  <si>
-    <t>HBSCPreamble</t>
-  </si>
-  <si>
-    <t>HBSC1</t>
-  </si>
-  <si>
-    <t>HBSC2</t>
-  </si>
-  <si>
-    <t>HBSCExtro</t>
-  </si>
-  <si>
-    <t>GSHSIntro</t>
-  </si>
-  <si>
-    <t>GSHSPreamble_PA</t>
-  </si>
-  <si>
-    <t>GSHS1</t>
-  </si>
-  <si>
-    <t>GSHS2</t>
-  </si>
-  <si>
-    <t>GSHS3</t>
-  </si>
-  <si>
-    <t>GSHS4</t>
-  </si>
-  <si>
-    <t>GSHSPreamble_Sitting</t>
-  </si>
-  <si>
-    <t>GSHS5</t>
-  </si>
-  <si>
-    <t>GSHSPreamble_Sleep</t>
-  </si>
-  <si>
-    <t>GSHS6</t>
-  </si>
-  <si>
-    <t>GSHSExtro</t>
-  </si>
-  <si>
-    <t>AppExtro</t>
-  </si>
-  <si>
-    <t>Adolescent</t>
-  </si>
-  <si>
-    <t>Parent</t>
-  </si>
-  <si>
-    <t>Extro (demo)</t>
-  </si>
-  <si>
-    <t>ok</t>
-  </si>
-  <si>
-    <t>in review</t>
-  </si>
-  <si>
-    <t>on-going (1)</t>
-  </si>
-  <si>
-    <t>on-going (2)</t>
-  </si>
-  <si>
-    <t>on-going (3)</t>
-  </si>
-  <si>
-    <t>on-going (4)</t>
-  </si>
-  <si>
-    <t>on-going (5)</t>
-  </si>
-  <si>
-    <t>on-going (6)</t>
-  </si>
-  <si>
-    <t>on-going (7)</t>
-  </si>
-  <si>
-    <t>on-going (8)</t>
-  </si>
-  <si>
-    <t>on-going (9)</t>
-  </si>
-  <si>
-    <t>on-going (10)</t>
-  </si>
-  <si>
-    <t>Submit</t>
-  </si>
-  <si>
-    <t>No pending submissions</t>
-  </si>
-  <si>
-    <t>Nothing to submit</t>
-  </si>
-  <si>
-    <t>Pending Submissions</t>
-  </si>
-  <si>
-    <t>Responses submitted</t>
-  </si>
-  <si>
-    <t>बुझाउनुहोस्</t>
-  </si>
-  <si>
-    <t>बुझाउनु पर्ने केहि बाँकी छैन</t>
-  </si>
-  <si>
-    <r>
-      <t>बुझाउनु</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Preeti"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>पर्ने</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Preeti"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>केहि</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Preeti"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>छैन</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>बुझाउन</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Preeti"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>बाँकी</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Preeti"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>छ</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>प्रतिकृया</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Preeti"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">बुझाइयो </t>
-    </r>
-  </si>
-  <si>
-    <t>Enviar</t>
-  </si>
-  <si>
-    <t>No hay envíos pendientes</t>
-  </si>
-  <si>
-    <t>No hay nada para enviar</t>
-  </si>
-  <si>
-    <t>Envíos pendientes</t>
-  </si>
-  <si>
-    <t>Respuestas enviadas</t>
-  </si>
-  <si>
-    <t>Nenhuma submissão pendente</t>
-  </si>
-  <si>
-    <t>Nada a enviar</t>
-  </si>
-  <si>
-    <t>Submissões pendentes</t>
-  </si>
-  <si>
-    <t>Respostas enviadas</t>
-  </si>
-  <si>
-    <t>on-going</t>
-  </si>
-  <si>
-    <t>India - English</t>
-  </si>
-  <si>
-    <t>en-IN</t>
-  </si>
-  <si>
-    <t>available</t>
-  </si>
-  <si>
-    <t>adopt from es-ES</t>
   </si>
 </sst>
 </file>
@@ -4354,11 +4354,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{460A6040-ECD3-3B44-8E8B-CFDB1F40DF24}">
   <dimension ref="A1:K88"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B40" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15:XFD15"/>
+      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5355,7 +5355,7 @@
       </c>
       <c r="E40" s="31"/>
       <c r="F40" s="32" t="s">
-        <v>253</v>
+        <v>421</v>
       </c>
       <c r="G40" s="32"/>
       <c r="H40" s="31" t="s">
@@ -5971,231 +5971,231 @@
     </row>
     <row r="72" spans="1:11">
       <c r="A72" s="18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B72" s="13" t="s">
         <v>102</v>
       </c>
       <c r="F72" s="13" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="73" spans="1:11">
       <c r="A73" s="18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B73" s="13" t="s">
         <v>216</v>
       </c>
       <c r="F73" s="13" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="74" spans="1:11">
       <c r="A74" s="18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B74" s="13">
         <v>25</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="H74" s="13" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="75" spans="1:11">
       <c r="A75" s="18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B75" s="13">
         <v>26</v>
       </c>
       <c r="F75" s="13" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H75" s="13" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="76" spans="1:11">
       <c r="A76" s="18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B76" s="13" t="s">
         <v>51</v>
       </c>
       <c r="F76" s="13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H76" s="13" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="77" spans="1:11">
       <c r="A77" s="62" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B77" s="13" t="s">
         <v>102</v>
       </c>
       <c r="F77" s="13" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="H77" s="13" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="78" spans="1:11">
       <c r="A78" s="62" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B78" s="13" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F78" s="13" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="H78" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="79" spans="1:11">
       <c r="A79" s="62" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B79" s="13">
         <v>25</v>
       </c>
       <c r="F79" s="13" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H79" s="13" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="80" spans="1:11">
       <c r="A80" s="62" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B80" s="13">
         <v>26</v>
       </c>
       <c r="F80" s="13" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="17" customHeight="1">
       <c r="A81" s="62" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B81" s="13">
         <v>27</v>
       </c>
       <c r="F81" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H81" s="13" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="82" spans="1:8">
       <c r="A82" s="62" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B82" s="13">
         <v>28</v>
       </c>
       <c r="F82" s="13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H82" s="63" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="83" spans="1:8">
       <c r="A83" s="62" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B83" s="13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F83" s="13" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H83" s="13" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="84" spans="1:8">
       <c r="A84" s="62" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B84" s="13">
         <v>29</v>
       </c>
       <c r="F84" s="13" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="85" spans="1:8">
       <c r="A85" s="62" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B85" s="13" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F85" s="13" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="86" spans="1:8">
       <c r="A86" s="62" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B86" s="13">
         <v>30</v>
       </c>
       <c r="F86" s="13" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H86" s="13" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="87" spans="1:8">
       <c r="A87" s="62" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B87" s="13" t="s">
         <v>51</v>
       </c>
       <c r="F87" s="13" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H87" s="13" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="88" spans="1:8">
       <c r="A88" s="21" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>
@@ -6224,33 +6224,33 @@
         <v>25</v>
       </c>
       <c r="D2" t="s">
+        <v>382</v>
+      </c>
+      <c r="E2" t="s">
         <v>383</v>
-      </c>
-      <c r="E2" t="s">
-        <v>384</v>
       </c>
       <c r="H2" t="s">
         <v>25</v>
       </c>
       <c r="I2" t="s">
+        <v>382</v>
+      </c>
+      <c r="J2" t="s">
         <v>383</v>
-      </c>
-      <c r="J2" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="G3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -6270,16 +6270,16 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="J4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -6403,7 +6403,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="22" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B12" s="35">
         <v>8</v>
@@ -6435,7 +6435,7 @@
     </row>
     <row r="14" spans="1:10">
       <c r="A14" s="18" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B14" s="35">
         <v>9</v>
@@ -6446,7 +6446,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="62" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B15" s="35">
         <v>10</v>
@@ -6457,7 +6457,7 @@
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="21" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B16" s="35">
         <v>11</v>
@@ -6509,21 +6509,21 @@
     <row r="3" spans="1:5" ht="20" customHeight="1">
       <c r="A3" s="40"/>
       <c r="B3" s="46" t="s">
+        <v>312</v>
+      </c>
+      <c r="C3" s="46" t="s">
         <v>313</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="D3" s="46" t="s">
         <v>314</v>
       </c>
-      <c r="D3" s="46" t="s">
+      <c r="E3" s="46" t="s">
         <v>315</v>
-      </c>
-      <c r="E3" s="46" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="20" customHeight="1">
       <c r="A4" s="40" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B4" s="46">
         <v>23</v>
@@ -6541,7 +6541,7 @@
     </row>
     <row r="5" spans="1:5" ht="20" customHeight="1">
       <c r="A5" s="40" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B5" s="46">
         <v>13</v>
@@ -6559,7 +6559,7 @@
     </row>
     <row r="6" spans="1:5" ht="20" customHeight="1">
       <c r="A6" s="40" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B6" s="46">
         <v>0</v>
@@ -6577,7 +6577,7 @@
     </row>
     <row r="7" spans="1:5" ht="20" customHeight="1">
       <c r="A7" s="40" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B7" s="46">
         <v>1</v>
@@ -6595,7 +6595,7 @@
     </row>
     <row r="8" spans="1:5" ht="20" customHeight="1">
       <c r="A8" s="40" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B8" s="46">
         <v>0</v>
@@ -6613,7 +6613,7 @@
     </row>
     <row r="9" spans="1:5" ht="20" customHeight="1">
       <c r="A9" s="40" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B9" s="46">
         <v>1</v>
@@ -6631,7 +6631,7 @@
     </row>
     <row r="10" spans="1:5" ht="20" customHeight="1">
       <c r="A10" s="40" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B10" s="46">
         <v>15</v>
@@ -6649,7 +6649,7 @@
     </row>
     <row r="11" spans="1:5" ht="20" customHeight="1">
       <c r="A11" s="40" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B11" s="46">
         <v>0</v>
@@ -6667,7 +6667,7 @@
     </row>
     <row r="12" spans="1:5" ht="20" customHeight="1">
       <c r="A12" s="40" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B12" s="46">
         <v>18</v>
@@ -6685,7 +6685,7 @@
     </row>
     <row r="13" spans="1:5" ht="20" customHeight="1">
       <c r="A13" s="40" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B13" s="46">
         <v>11</v>
@@ -6703,7 +6703,7 @@
     </row>
     <row r="14" spans="1:5" ht="20" customHeight="1">
       <c r="A14" s="40" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B14" s="46">
         <v>16</v>
@@ -6721,7 +6721,7 @@
     </row>
     <row r="15" spans="1:5" ht="20" customHeight="1">
       <c r="A15" s="40" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B15" s="46">
         <v>0</v>
@@ -6739,7 +6739,7 @@
     </row>
     <row r="16" spans="1:5" ht="20" customHeight="1">
       <c r="A16" s="40" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B16" s="46">
         <v>0</v>
@@ -6812,13 +6812,13 @@
       <c r="A1" s="38"/>
       <c r="B1" s="38"/>
       <c r="C1" s="74" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D1" s="74"/>
       <c r="E1" s="74"/>
       <c r="F1" s="74"/>
       <c r="G1" s="79" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H1" s="80"/>
       <c r="I1" s="80"/>
@@ -6844,61 +6844,61 @@
       <c r="AC1" s="80"/>
       <c r="AD1" s="80"/>
       <c r="AE1" s="39" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:31" s="39" customFormat="1" ht="16" customHeight="1">
       <c r="A2" s="40"/>
       <c r="B2" s="40"/>
       <c r="C2" s="40" t="s">
+        <v>255</v>
+      </c>
+      <c r="D2" s="40" t="s">
         <v>256</v>
       </c>
-      <c r="D2" s="40" t="s">
+      <c r="E2" s="40" t="s">
         <v>257</v>
       </c>
-      <c r="E2" s="40" t="s">
+      <c r="F2" s="40" t="s">
         <v>258</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="G2" s="75" t="s">
         <v>259</v>
-      </c>
-      <c r="G2" s="75" t="s">
-        <v>260</v>
       </c>
       <c r="H2" s="76"/>
       <c r="I2" s="77"/>
       <c r="J2" s="75" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="K2" s="76"/>
       <c r="L2" s="77"/>
       <c r="M2" s="75" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="N2" s="76"/>
       <c r="O2" s="77"/>
       <c r="P2" s="75" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q2" s="76"/>
       <c r="R2" s="77"/>
       <c r="S2" s="75" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="T2" s="76"/>
       <c r="U2" s="77"/>
       <c r="V2" s="75" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="W2" s="76"/>
       <c r="X2" s="77"/>
       <c r="Y2" s="75" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="Z2" s="76"/>
       <c r="AA2" s="77"/>
       <c r="AB2" s="78" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="AC2" s="78"/>
       <c r="AD2" s="78"/>
@@ -6911,84 +6911,84 @@
       <c r="E3" s="40"/>
       <c r="F3" s="40"/>
       <c r="G3" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="H3" s="40" t="s">
         <v>267</v>
       </c>
-      <c r="H3" s="40" t="s">
-        <v>268</v>
-      </c>
       <c r="I3" s="40" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="J3" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="K3" s="40" t="s">
         <v>267</v>
       </c>
-      <c r="K3" s="40" t="s">
-        <v>268</v>
-      </c>
       <c r="L3" s="40" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M3" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="N3" s="40" t="s">
         <v>267</v>
       </c>
-      <c r="N3" s="40" t="s">
-        <v>268</v>
-      </c>
       <c r="O3" s="40" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P3" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="Q3" s="40" t="s">
         <v>267</v>
       </c>
-      <c r="Q3" s="40" t="s">
-        <v>268</v>
-      </c>
       <c r="R3" s="40" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="S3" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="T3" s="40" t="s">
         <v>267</v>
       </c>
-      <c r="T3" s="40" t="s">
-        <v>268</v>
-      </c>
       <c r="U3" s="40" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="V3" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="W3" s="40" t="s">
         <v>267</v>
       </c>
-      <c r="W3" s="40" t="s">
-        <v>268</v>
-      </c>
       <c r="X3" s="40" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="Y3" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="Z3" s="40" t="s">
         <v>267</v>
       </c>
-      <c r="Z3" s="40" t="s">
-        <v>268</v>
-      </c>
       <c r="AA3" s="40" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="AB3" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="AC3" s="40" t="s">
         <v>267</v>
       </c>
-      <c r="AC3" s="40" t="s">
-        <v>268</v>
-      </c>
       <c r="AD3" s="40" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="4" spans="1:31">
       <c r="A4" s="45" t="s">
+        <v>268</v>
+      </c>
+      <c r="B4" s="41" t="s">
         <v>269</v>
-      </c>
-      <c r="B4" s="41" t="s">
-        <v>270</v>
       </c>
       <c r="C4" s="42"/>
       <c r="D4" s="42"/>
@@ -7021,10 +7021,10 @@
     </row>
     <row r="5" spans="1:31">
       <c r="A5" s="45" t="s">
+        <v>270</v>
+      </c>
+      <c r="B5" s="41" t="s">
         <v>271</v>
-      </c>
-      <c r="B5" s="41" t="s">
-        <v>272</v>
       </c>
       <c r="C5" s="42"/>
       <c r="D5" s="42"/>
@@ -7057,10 +7057,10 @@
     </row>
     <row r="6" spans="1:31">
       <c r="A6" s="45" t="s">
+        <v>272</v>
+      </c>
+      <c r="B6" s="41" t="s">
         <v>273</v>
-      </c>
-      <c r="B6" s="41" t="s">
-        <v>274</v>
       </c>
       <c r="C6" s="42"/>
       <c r="D6" s="42"/>
@@ -7093,10 +7093,10 @@
     </row>
     <row r="7" spans="1:31">
       <c r="A7" s="40" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B7" s="41" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C7" s="41"/>
       <c r="D7" s="41"/>
@@ -7129,10 +7129,10 @@
     </row>
     <row r="8" spans="1:31">
       <c r="A8" s="45" t="s">
+        <v>275</v>
+      </c>
+      <c r="B8" s="41" t="s">
         <v>276</v>
-      </c>
-      <c r="B8" s="41" t="s">
-        <v>277</v>
       </c>
       <c r="C8" s="42"/>
       <c r="D8" s="42"/>
@@ -7165,10 +7165,10 @@
     </row>
     <row r="9" spans="1:31" ht="17" customHeight="1">
       <c r="A9" s="45" t="s">
+        <v>277</v>
+      </c>
+      <c r="B9" s="41" t="s">
         <v>278</v>
-      </c>
-      <c r="B9" s="41" t="s">
-        <v>279</v>
       </c>
       <c r="C9" s="42"/>
       <c r="D9" s="42"/>
@@ -7201,10 +7201,10 @@
     </row>
     <row r="10" spans="1:31">
       <c r="A10" s="40" t="s">
+        <v>279</v>
+      </c>
+      <c r="B10" s="41" t="s">
         <v>280</v>
-      </c>
-      <c r="B10" s="41" t="s">
-        <v>281</v>
       </c>
       <c r="C10" s="41"/>
       <c r="D10" s="41"/>
@@ -7237,10 +7237,10 @@
     </row>
     <row r="11" spans="1:31">
       <c r="A11" s="45" t="s">
+        <v>281</v>
+      </c>
+      <c r="B11" s="41" t="s">
         <v>282</v>
-      </c>
-      <c r="B11" s="41" t="s">
-        <v>283</v>
       </c>
       <c r="C11" s="42"/>
       <c r="D11" s="42"/>
@@ -7273,10 +7273,10 @@
     </row>
     <row r="12" spans="1:31" ht="17" customHeight="1">
       <c r="A12" s="45" t="s">
+        <v>283</v>
+      </c>
+      <c r="B12" s="41" t="s">
         <v>284</v>
-      </c>
-      <c r="B12" s="41" t="s">
-        <v>285</v>
       </c>
       <c r="C12" s="42"/>
       <c r="D12" s="42"/>
@@ -7309,10 +7309,10 @@
     </row>
     <row r="13" spans="1:31">
       <c r="A13" s="45" t="s">
+        <v>285</v>
+      </c>
+      <c r="B13" s="41" t="s">
         <v>286</v>
-      </c>
-      <c r="B13" s="41" t="s">
-        <v>287</v>
       </c>
       <c r="C13" s="42"/>
       <c r="D13" s="42"/>
@@ -7345,10 +7345,10 @@
     </row>
     <row r="14" spans="1:31" ht="17" customHeight="1">
       <c r="A14" s="45" t="s">
+        <v>287</v>
+      </c>
+      <c r="B14" s="41" t="s">
         <v>288</v>
-      </c>
-      <c r="B14" s="41" t="s">
-        <v>289</v>
       </c>
       <c r="C14" s="42"/>
       <c r="D14" s="42"/>
@@ -7381,10 +7381,10 @@
     </row>
     <row r="15" spans="1:31" ht="17" customHeight="1">
       <c r="A15" s="45" t="s">
+        <v>289</v>
+      </c>
+      <c r="B15" s="41" t="s">
         <v>290</v>
-      </c>
-      <c r="B15" s="41" t="s">
-        <v>291</v>
       </c>
       <c r="C15" s="42"/>
       <c r="D15" s="42"/>
@@ -7417,10 +7417,10 @@
     </row>
     <row r="16" spans="1:31">
       <c r="A16" s="45" t="s">
+        <v>291</v>
+      </c>
+      <c r="B16" s="41" t="s">
         <v>292</v>
-      </c>
-      <c r="B16" s="41" t="s">
-        <v>293</v>
       </c>
       <c r="C16" s="42"/>
       <c r="D16" s="42"/>
@@ -7453,10 +7453,10 @@
     </row>
     <row r="17" spans="1:30">
       <c r="A17" s="40" t="s">
+        <v>293</v>
+      </c>
+      <c r="B17" s="41" t="s">
         <v>294</v>
-      </c>
-      <c r="B17" s="41" t="s">
-        <v>295</v>
       </c>
       <c r="C17" s="41"/>
       <c r="D17" s="41"/>
@@ -7489,10 +7489,10 @@
     </row>
     <row r="18" spans="1:30" ht="17" customHeight="1">
       <c r="A18" s="40" t="s">
+        <v>295</v>
+      </c>
+      <c r="B18" s="41" t="s">
         <v>296</v>
-      </c>
-      <c r="B18" s="41" t="s">
-        <v>297</v>
       </c>
       <c r="C18" s="41"/>
       <c r="D18" s="41"/>
@@ -7525,10 +7525,10 @@
     </row>
     <row r="19" spans="1:30">
       <c r="A19" s="45" t="s">
+        <v>297</v>
+      </c>
+      <c r="B19" s="41" t="s">
         <v>298</v>
-      </c>
-      <c r="B19" s="41" t="s">
-        <v>299</v>
       </c>
       <c r="C19" s="42"/>
       <c r="D19" s="42"/>
@@ -7561,10 +7561,10 @@
     </row>
     <row r="20" spans="1:30">
       <c r="A20" s="45" t="s">
+        <v>299</v>
+      </c>
+      <c r="B20" s="41" t="s">
         <v>300</v>
-      </c>
-      <c r="B20" s="41" t="s">
-        <v>301</v>
       </c>
       <c r="C20" s="42"/>
       <c r="D20" s="42"/>
@@ -7597,10 +7597,10 @@
     </row>
     <row r="21" spans="1:30">
       <c r="A21" s="45" t="s">
+        <v>301</v>
+      </c>
+      <c r="B21" s="41" t="s">
         <v>302</v>
-      </c>
-      <c r="B21" s="41" t="s">
-        <v>303</v>
       </c>
       <c r="C21" s="42"/>
       <c r="D21" s="42"/>
@@ -7633,10 +7633,10 @@
     </row>
     <row r="22" spans="1:30">
       <c r="A22" s="45" t="s">
+        <v>303</v>
+      </c>
+      <c r="B22" s="41" t="s">
         <v>304</v>
-      </c>
-      <c r="B22" s="41" t="s">
-        <v>305</v>
       </c>
       <c r="C22" s="42"/>
       <c r="D22" s="42"/>
@@ -7669,10 +7669,10 @@
     </row>
     <row r="23" spans="1:30">
       <c r="A23" s="45" t="s">
+        <v>305</v>
+      </c>
+      <c r="B23" s="41" t="s">
         <v>306</v>
-      </c>
-      <c r="B23" s="41" t="s">
-        <v>307</v>
       </c>
       <c r="C23" s="42"/>
       <c r="D23" s="42"/>
@@ -7705,10 +7705,10 @@
     </row>
     <row r="24" spans="1:30">
       <c r="A24" s="45" t="s">
+        <v>307</v>
+      </c>
+      <c r="B24" s="41" t="s">
         <v>308</v>
-      </c>
-      <c r="B24" s="41" t="s">
-        <v>309</v>
       </c>
       <c r="C24" s="42"/>
       <c r="D24" s="42"/>
@@ -7761,7 +7761,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BEEE373-47BE-6F4C-8F66-ACD6798C647F}">
   <dimension ref="A1:AJ23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="114" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="114" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -7802,31 +7802,31 @@
       <c r="A1" s="47"/>
       <c r="B1" s="47"/>
       <c r="C1" s="51" t="s">
+        <v>339</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>341</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>338</v>
+      </c>
+      <c r="F1" s="51" t="s">
         <v>340</v>
       </c>
-      <c r="D1" s="51" t="s">
+      <c r="G1" s="51" t="s">
+        <v>333</v>
+      </c>
+      <c r="H1" s="52" t="s">
+        <v>331</v>
+      </c>
+      <c r="I1" s="51" t="s">
+        <v>332</v>
+      </c>
+      <c r="J1" s="51" t="s">
         <v>342</v>
       </c>
-      <c r="E1" s="51" t="s">
-        <v>339</v>
-      </c>
-      <c r="F1" s="51" t="s">
-        <v>341</v>
-      </c>
-      <c r="G1" s="51" t="s">
+      <c r="K1" s="51" t="s">
         <v>334</v>
-      </c>
-      <c r="H1" s="52" t="s">
-        <v>332</v>
-      </c>
-      <c r="I1" s="51" t="s">
-        <v>333</v>
-      </c>
-      <c r="J1" s="51" t="s">
-        <v>343</v>
-      </c>
-      <c r="K1" s="51" t="s">
-        <v>335</v>
       </c>
       <c r="L1" s="47"/>
       <c r="M1" s="49"/>
@@ -7853,45 +7853,45 @@
       <c r="AH1" s="49"/>
       <c r="AI1" s="49"/>
       <c r="AJ1" s="50" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:36" ht="27" customHeight="1">
       <c r="A2" s="40" t="s">
+        <v>268</v>
+      </c>
+      <c r="B2" s="41" t="s">
         <v>269</v>
       </c>
-      <c r="B2" s="41" t="s">
-        <v>270</v>
-      </c>
       <c r="C2" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D2" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E2" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F2" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G2" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H2" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I2" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J2" s="53" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K2" s="56" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L2" s="40" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="M2" s="48"/>
       <c r="N2" s="48"/>
@@ -7916,40 +7916,40 @@
     </row>
     <row r="3" spans="1:36" ht="28" customHeight="1">
       <c r="A3" s="40" t="s">
+        <v>270</v>
+      </c>
+      <c r="B3" s="41" t="s">
         <v>271</v>
       </c>
-      <c r="B3" s="41" t="s">
-        <v>272</v>
-      </c>
       <c r="C3" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D3" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E3" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F3" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G3" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H3" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I3" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J3" s="53" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K3" s="56" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L3" s="40" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="M3" s="48"/>
       <c r="N3" s="48"/>
@@ -7974,40 +7974,40 @@
     </row>
     <row r="4" spans="1:36" ht="28" customHeight="1">
       <c r="A4" s="40" t="s">
+        <v>272</v>
+      </c>
+      <c r="B4" s="41" t="s">
         <v>273</v>
       </c>
-      <c r="B4" s="41" t="s">
-        <v>274</v>
-      </c>
       <c r="C4" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D4" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E4" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F4" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G4" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H4" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I4" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J4" s="53" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K4" s="56" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L4" s="40" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="M4" s="48"/>
       <c r="N4" s="48"/>
@@ -8032,34 +8032,34 @@
     </row>
     <row r="5" spans="1:36" ht="27" customHeight="1">
       <c r="A5" s="40" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D5" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E5" s="57" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F5" s="56" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="G5" s="55"/>
       <c r="H5" s="55" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="I5" s="55" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="J5" s="55"/>
       <c r="K5" s="55"/>
       <c r="L5" s="40" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="M5" s="48"/>
       <c r="N5" s="48"/>
@@ -8084,40 +8084,40 @@
     </row>
     <row r="6" spans="1:36" ht="27" customHeight="1">
       <c r="A6" s="40" t="s">
+        <v>275</v>
+      </c>
+      <c r="B6" s="41" t="s">
         <v>276</v>
       </c>
-      <c r="B6" s="41" t="s">
-        <v>277</v>
-      </c>
       <c r="C6" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D6" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E6" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F6" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G6" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H6" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I6" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J6" s="53" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K6" s="56" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="L6" s="40" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="M6" s="48"/>
       <c r="N6" s="48"/>
@@ -8142,40 +8142,40 @@
     </row>
     <row r="7" spans="1:36" ht="27" customHeight="1">
       <c r="A7" s="40" t="s">
+        <v>277</v>
+      </c>
+      <c r="B7" s="41" t="s">
         <v>278</v>
       </c>
-      <c r="B7" s="41" t="s">
-        <v>279</v>
-      </c>
       <c r="C7" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D7" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E7" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F7" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G7" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H7" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I7" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J7" s="53" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K7" s="56" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L7" s="40" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="M7" s="48"/>
       <c r="N7" s="48"/>
@@ -8200,36 +8200,36 @@
     </row>
     <row r="8" spans="1:36" ht="27" customHeight="1">
       <c r="A8" s="40" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C8" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D8" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E8" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F8" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G8" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H8" s="56" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I8" s="56" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="J8" s="55"/>
       <c r="K8" s="55"/>
       <c r="L8" s="40" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="M8" s="48"/>
       <c r="N8" s="48"/>
@@ -8254,36 +8254,36 @@
     </row>
     <row r="9" spans="1:36" ht="27" customHeight="1">
       <c r="A9" s="40" t="s">
+        <v>417</v>
+      </c>
+      <c r="B9" s="41" t="s">
         <v>418</v>
       </c>
-      <c r="B9" s="41" t="s">
-        <v>419</v>
-      </c>
       <c r="C9" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D9" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F9" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G9" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H9" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I9" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J9" s="55"/>
       <c r="K9" s="55"/>
       <c r="L9" s="40" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="M9" s="48"/>
       <c r="N9" s="48"/>
@@ -8308,36 +8308,36 @@
     </row>
     <row r="10" spans="1:36" ht="27" customHeight="1">
       <c r="A10" s="40" t="s">
+        <v>281</v>
+      </c>
+      <c r="B10" s="41" t="s">
         <v>282</v>
       </c>
-      <c r="B10" s="41" t="s">
-        <v>283</v>
-      </c>
       <c r="C10" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D10" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E10" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F10" s="57" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G10" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H10" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I10" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J10" s="55"/>
       <c r="K10" s="55"/>
       <c r="L10" s="40" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="M10" s="48"/>
       <c r="N10" s="48"/>
@@ -8362,32 +8362,32 @@
     </row>
     <row r="11" spans="1:36" ht="27" customHeight="1">
       <c r="A11" s="40" t="s">
+        <v>283</v>
+      </c>
+      <c r="B11" s="41" t="s">
         <v>284</v>
       </c>
-      <c r="B11" s="41" t="s">
-        <v>285</v>
-      </c>
       <c r="C11" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D11" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E11" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F11" s="57" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G11" s="56" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H11" s="55"/>
       <c r="I11" s="55"/>
       <c r="J11" s="55"/>
       <c r="K11" s="55"/>
       <c r="L11" s="40" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="M11" s="48"/>
       <c r="N11" s="48"/>
@@ -8412,38 +8412,38 @@
     </row>
     <row r="12" spans="1:36" ht="27" customHeight="1">
       <c r="A12" s="40" t="s">
+        <v>285</v>
+      </c>
+      <c r="B12" s="41" t="s">
         <v>286</v>
       </c>
-      <c r="B12" s="41" t="s">
-        <v>287</v>
-      </c>
       <c r="C12" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D12" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E12" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F12" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G12" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H12" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I12" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J12" s="56" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="K12" s="55"/>
       <c r="L12" s="40" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="M12" s="48"/>
       <c r="N12" s="48"/>
@@ -8468,38 +8468,38 @@
     </row>
     <row r="13" spans="1:36" ht="27" customHeight="1">
       <c r="A13" s="40" t="s">
+        <v>287</v>
+      </c>
+      <c r="B13" s="41" t="s">
         <v>288</v>
       </c>
-      <c r="B13" s="41" t="s">
-        <v>289</v>
-      </c>
       <c r="C13" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E13" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F13" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G13" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H13" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I13" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J13" s="56" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="K13" s="55"/>
       <c r="L13" s="40" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="M13" s="48"/>
       <c r="N13" s="48"/>
@@ -8524,40 +8524,40 @@
     </row>
     <row r="14" spans="1:36" ht="27" customHeight="1">
       <c r="A14" s="40" t="s">
+        <v>289</v>
+      </c>
+      <c r="B14" s="41" t="s">
         <v>290</v>
       </c>
-      <c r="B14" s="41" t="s">
-        <v>291</v>
-      </c>
       <c r="C14" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D14" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E14" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F14" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G14" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H14" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I14" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J14" s="53" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K14" s="56" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L14" s="40" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="M14" s="48"/>
       <c r="N14" s="48"/>
@@ -8582,40 +8582,40 @@
     </row>
     <row r="15" spans="1:36" ht="27" customHeight="1">
       <c r="A15" s="40" t="s">
+        <v>291</v>
+      </c>
+      <c r="B15" s="41" t="s">
         <v>292</v>
       </c>
-      <c r="B15" s="41" t="s">
-        <v>293</v>
-      </c>
       <c r="C15" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D15" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E15" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F15" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G15" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H15" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I15" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J15" s="53" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K15" s="56" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="L15" s="40" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="M15" s="48"/>
       <c r="N15" s="48"/>
@@ -8640,34 +8640,34 @@
     </row>
     <row r="16" spans="1:36" ht="27" customHeight="1">
       <c r="A16" s="40" t="s">
+        <v>293</v>
+      </c>
+      <c r="B16" s="41" t="s">
         <v>294</v>
       </c>
-      <c r="B16" s="41" t="s">
-        <v>295</v>
-      </c>
       <c r="C16" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D16" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E16" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F16" s="57" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G16" s="55"/>
       <c r="H16" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I16" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J16" s="55"/>
       <c r="K16" s="55"/>
       <c r="L16" s="40" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="M16" s="48"/>
       <c r="N16" s="48"/>
@@ -8692,32 +8692,32 @@
     </row>
     <row r="17" spans="1:32" ht="26">
       <c r="A17" s="40" t="s">
+        <v>295</v>
+      </c>
+      <c r="B17" s="41" t="s">
         <v>296</v>
       </c>
-      <c r="B17" s="41" t="s">
-        <v>297</v>
-      </c>
       <c r="C17" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D17" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E17" s="57" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F17" s="58"/>
       <c r="G17" s="55"/>
       <c r="H17" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I17" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J17" s="55"/>
       <c r="K17" s="55"/>
       <c r="L17" s="40" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="M17" s="48"/>
       <c r="N17" s="48"/>
@@ -8742,40 +8742,40 @@
     </row>
     <row r="18" spans="1:32" ht="31" customHeight="1">
       <c r="A18" s="40" t="s">
+        <v>297</v>
+      </c>
+      <c r="B18" s="41" t="s">
         <v>298</v>
       </c>
-      <c r="B18" s="41" t="s">
-        <v>299</v>
-      </c>
       <c r="C18" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D18" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E18" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F18" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G18" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H18" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I18" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J18" s="53" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K18" s="56" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="L18" s="40" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="M18" s="48"/>
       <c r="N18" s="48"/>
@@ -8800,40 +8800,40 @@
     </row>
     <row r="19" spans="1:32" ht="27" customHeight="1">
       <c r="A19" s="40" t="s">
+        <v>299</v>
+      </c>
+      <c r="B19" s="41" t="s">
         <v>300</v>
       </c>
-      <c r="B19" s="41" t="s">
-        <v>301</v>
-      </c>
       <c r="C19" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D19" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E19" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F19" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G19" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H19" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I19" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J19" s="53" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K19" s="54" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="L19" s="40" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="M19" s="48"/>
       <c r="N19" s="48"/>
@@ -8858,40 +8858,40 @@
     </row>
     <row r="20" spans="1:32" ht="27" customHeight="1">
       <c r="A20" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="B20" s="41" t="s">
         <v>302</v>
       </c>
-      <c r="B20" s="41" t="s">
-        <v>303</v>
-      </c>
       <c r="C20" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D20" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E20" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F20" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G20" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H20" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I20" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J20" s="53" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K20" s="56" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="L20" s="40" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M20" s="48"/>
       <c r="N20" s="48"/>
@@ -8916,40 +8916,40 @@
     </row>
     <row r="21" spans="1:32" ht="27" customHeight="1">
       <c r="A21" s="40" t="s">
+        <v>303</v>
+      </c>
+      <c r="B21" s="41" t="s">
         <v>304</v>
       </c>
-      <c r="B21" s="41" t="s">
-        <v>305</v>
-      </c>
       <c r="C21" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D21" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E21" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F21" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G21" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H21" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I21" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J21" s="53" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K21" s="56" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="L21" s="40" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M21" s="48"/>
       <c r="N21" s="48"/>
@@ -8974,40 +8974,40 @@
     </row>
     <row r="22" spans="1:32" ht="27" customHeight="1">
       <c r="A22" s="40" t="s">
+        <v>305</v>
+      </c>
+      <c r="B22" s="41" t="s">
         <v>306</v>
       </c>
-      <c r="B22" s="41" t="s">
-        <v>307</v>
-      </c>
       <c r="C22" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D22" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E22" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F22" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G22" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H22" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I22" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J22" s="53" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K22" s="56" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L22" s="40" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="M22" s="48"/>
       <c r="N22" s="48"/>
@@ -9032,40 +9032,40 @@
     </row>
     <row r="23" spans="1:32" ht="27" customHeight="1">
       <c r="A23" s="40" t="s">
+        <v>307</v>
+      </c>
+      <c r="B23" s="41" t="s">
         <v>308</v>
       </c>
-      <c r="B23" s="41" t="s">
-        <v>309</v>
-      </c>
       <c r="C23" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D23" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E23" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F23" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G23" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H23" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="I23" s="53" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="J23" s="53" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="K23" s="56" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L23" s="40" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="M23" s="48"/>
       <c r="N23" s="48"/>
@@ -9139,19 +9139,19 @@
       <c r="A1" s="47"/>
       <c r="B1" s="47"/>
       <c r="C1" s="67" t="s">
+        <v>397</v>
+      </c>
+      <c r="D1" s="67" t="s">
         <v>398</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="E1" s="67" t="s">
         <v>399</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="F1" s="67" t="s">
         <v>400</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="G1" s="67" t="s">
         <v>401</v>
-      </c>
-      <c r="G1" s="67" t="s">
-        <v>402</v>
       </c>
       <c r="H1" s="47"/>
       <c r="I1" s="49"/>
@@ -9178,33 +9178,33 @@
       <c r="AD1" s="49"/>
       <c r="AE1" s="49"/>
       <c r="AF1" s="50" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:32" ht="27" customHeight="1">
       <c r="A2" s="40" t="s">
+        <v>268</v>
+      </c>
+      <c r="B2" s="41" t="s">
         <v>269</v>
       </c>
-      <c r="B2" s="41" t="s">
-        <v>270</v>
-      </c>
       <c r="C2" s="68" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D2" s="68" t="s">
+        <v>412</v>
+      </c>
+      <c r="E2" s="68" t="s">
         <v>413</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="F2" s="68" t="s">
         <v>414</v>
       </c>
-      <c r="F2" s="68" t="s">
+      <c r="G2" s="68" t="s">
         <v>415</v>
       </c>
-      <c r="G2" s="68" t="s">
-        <v>416</v>
-      </c>
       <c r="H2" s="40" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I2" s="48"/>
       <c r="J2" s="48"/>
@@ -9229,28 +9229,28 @@
     </row>
     <row r="3" spans="1:32" ht="28" customHeight="1">
       <c r="A3" s="40" t="s">
+        <v>270</v>
+      </c>
+      <c r="B3" s="41" t="s">
         <v>271</v>
       </c>
-      <c r="B3" s="41" t="s">
-        <v>272</v>
-      </c>
       <c r="C3" s="70" t="s">
+        <v>397</v>
+      </c>
+      <c r="D3" s="70" t="s">
         <v>398</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="E3" s="70" t="s">
         <v>399</v>
       </c>
-      <c r="E3" s="70" t="s">
+      <c r="F3" s="70" t="s">
         <v>400</v>
       </c>
-      <c r="F3" s="70" t="s">
+      <c r="G3" s="70" t="s">
         <v>401</v>
       </c>
-      <c r="G3" s="70" t="s">
-        <v>402</v>
-      </c>
       <c r="H3" s="40" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="I3" s="48"/>
       <c r="J3" s="48"/>
@@ -9275,10 +9275,10 @@
     </row>
     <row r="4" spans="1:32" ht="28" customHeight="1">
       <c r="A4" s="40" t="s">
+        <v>272</v>
+      </c>
+      <c r="B4" s="41" t="s">
         <v>273</v>
-      </c>
-      <c r="B4" s="41" t="s">
-        <v>274</v>
       </c>
       <c r="C4" s="69"/>
       <c r="D4" s="69"/>
@@ -9286,7 +9286,7 @@
       <c r="F4" s="69"/>
       <c r="G4" s="69"/>
       <c r="H4" s="40" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I4" s="48"/>
       <c r="J4" s="48"/>
@@ -9311,28 +9311,28 @@
     </row>
     <row r="5" spans="1:32" ht="27" customHeight="1">
       <c r="A5" s="40" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B5" s="41" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C5" s="68" t="s">
+        <v>407</v>
+      </c>
+      <c r="D5" s="68" t="s">
         <v>408</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="E5" s="68" t="s">
         <v>409</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="F5" s="68" t="s">
         <v>410</v>
       </c>
-      <c r="F5" s="68" t="s">
+      <c r="G5" s="68" t="s">
         <v>411</v>
       </c>
-      <c r="G5" s="68" t="s">
-        <v>412</v>
-      </c>
       <c r="H5" s="40" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="I5" s="48"/>
       <c r="J5" s="48"/>
@@ -9357,10 +9357,10 @@
     </row>
     <row r="6" spans="1:32" ht="27" customHeight="1">
       <c r="A6" s="40" t="s">
+        <v>275</v>
+      </c>
+      <c r="B6" s="41" t="s">
         <v>276</v>
-      </c>
-      <c r="B6" s="41" t="s">
-        <v>277</v>
       </c>
       <c r="C6" s="69"/>
       <c r="D6" s="69"/>
@@ -9368,7 +9368,7 @@
       <c r="F6" s="69"/>
       <c r="G6" s="69"/>
       <c r="H6" s="40" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I6" s="48"/>
       <c r="J6" s="48"/>
@@ -9393,28 +9393,28 @@
     </row>
     <row r="7" spans="1:32" ht="27" customHeight="1">
       <c r="A7" s="40" t="s">
+        <v>277</v>
+      </c>
+      <c r="B7" s="41" t="s">
         <v>278</v>
       </c>
-      <c r="B7" s="41" t="s">
-        <v>279</v>
-      </c>
       <c r="C7" s="68" t="s">
+        <v>407</v>
+      </c>
+      <c r="D7" s="68" t="s">
         <v>408</v>
       </c>
-      <c r="D7" s="68" t="s">
+      <c r="E7" s="68" t="s">
         <v>409</v>
       </c>
-      <c r="E7" s="68" t="s">
+      <c r="F7" s="68" t="s">
         <v>410</v>
       </c>
-      <c r="F7" s="68" t="s">
+      <c r="G7" s="68" t="s">
         <v>411</v>
       </c>
-      <c r="G7" s="68" t="s">
-        <v>412</v>
-      </c>
       <c r="H7" s="40" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="I7" s="48"/>
       <c r="J7" s="48"/>
@@ -9439,10 +9439,10 @@
     </row>
     <row r="8" spans="1:32" ht="27" customHeight="1">
       <c r="A8" s="40" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B8" s="41" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C8" s="69"/>
       <c r="D8" s="69"/>
@@ -9450,7 +9450,7 @@
       <c r="F8" s="69"/>
       <c r="G8" s="69"/>
       <c r="H8" s="40" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I8" s="48"/>
       <c r="J8" s="48"/>
@@ -9475,10 +9475,10 @@
     </row>
     <row r="9" spans="1:32" ht="27" customHeight="1">
       <c r="A9" s="40" t="s">
+        <v>281</v>
+      </c>
+      <c r="B9" s="41" t="s">
         <v>282</v>
-      </c>
-      <c r="B9" s="41" t="s">
-        <v>283</v>
       </c>
       <c r="C9" s="69"/>
       <c r="D9" s="69"/>
@@ -9486,7 +9486,7 @@
       <c r="F9" s="69"/>
       <c r="G9" s="69"/>
       <c r="H9" s="40" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I9" s="48"/>
       <c r="J9" s="48"/>
@@ -9511,10 +9511,10 @@
     </row>
     <row r="10" spans="1:32" ht="27" customHeight="1">
       <c r="A10" s="40" t="s">
+        <v>283</v>
+      </c>
+      <c r="B10" s="41" t="s">
         <v>284</v>
-      </c>
-      <c r="B10" s="41" t="s">
-        <v>285</v>
       </c>
       <c r="C10" s="69"/>
       <c r="D10" s="69"/>
@@ -9522,7 +9522,7 @@
       <c r="F10" s="69"/>
       <c r="G10" s="69"/>
       <c r="H10" s="40" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="I10" s="48"/>
       <c r="J10" s="48"/>
@@ -9547,10 +9547,10 @@
     </row>
     <row r="11" spans="1:32" ht="27" customHeight="1">
       <c r="A11" s="40" t="s">
+        <v>285</v>
+      </c>
+      <c r="B11" s="41" t="s">
         <v>286</v>
-      </c>
-      <c r="B11" s="41" t="s">
-        <v>287</v>
       </c>
       <c r="C11" s="69"/>
       <c r="D11" s="69"/>
@@ -9558,7 +9558,7 @@
       <c r="F11" s="69"/>
       <c r="G11" s="69"/>
       <c r="H11" s="40" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="I11" s="48"/>
       <c r="J11" s="48"/>
@@ -9583,28 +9583,28 @@
     </row>
     <row r="12" spans="1:32" ht="27" customHeight="1">
       <c r="A12" s="40" t="s">
+        <v>287</v>
+      </c>
+      <c r="B12" s="41" t="s">
         <v>288</v>
       </c>
-      <c r="B12" s="41" t="s">
-        <v>289</v>
-      </c>
       <c r="C12" s="70" t="s">
+        <v>397</v>
+      </c>
+      <c r="D12" s="70" t="s">
         <v>398</v>
       </c>
-      <c r="D12" s="70" t="s">
+      <c r="E12" s="70" t="s">
         <v>399</v>
       </c>
-      <c r="E12" s="70" t="s">
+      <c r="F12" s="70" t="s">
         <v>400</v>
       </c>
-      <c r="F12" s="70" t="s">
+      <c r="G12" s="70" t="s">
         <v>401</v>
       </c>
-      <c r="G12" s="70" t="s">
-        <v>402</v>
-      </c>
       <c r="H12" s="40" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="I12" s="48"/>
       <c r="J12" s="48"/>
@@ -9629,28 +9629,28 @@
     </row>
     <row r="13" spans="1:32" ht="27" customHeight="1">
       <c r="A13" s="40" t="s">
+        <v>289</v>
+      </c>
+      <c r="B13" s="41" t="s">
         <v>290</v>
       </c>
-      <c r="B13" s="41" t="s">
-        <v>291</v>
-      </c>
       <c r="C13" s="68" t="s">
+        <v>407</v>
+      </c>
+      <c r="D13" s="68" t="s">
         <v>408</v>
       </c>
-      <c r="D13" s="68" t="s">
+      <c r="E13" s="68" t="s">
         <v>409</v>
       </c>
-      <c r="E13" s="68" t="s">
+      <c r="F13" s="68" t="s">
         <v>410</v>
       </c>
-      <c r="F13" s="68" t="s">
+      <c r="G13" s="68" t="s">
         <v>411</v>
       </c>
-      <c r="G13" s="68" t="s">
-        <v>412</v>
-      </c>
       <c r="H13" s="40" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I13" s="48"/>
       <c r="J13" s="48"/>
@@ -9675,28 +9675,28 @@
     </row>
     <row r="14" spans="1:32" ht="27" customHeight="1">
       <c r="A14" s="40" t="s">
+        <v>291</v>
+      </c>
+      <c r="B14" s="41" t="s">
         <v>292</v>
       </c>
-      <c r="B14" s="41" t="s">
-        <v>293</v>
-      </c>
       <c r="C14" s="72" t="s">
+        <v>402</v>
+      </c>
+      <c r="D14" s="68" t="s">
         <v>403</v>
       </c>
-      <c r="D14" s="68" t="s">
+      <c r="E14" s="73" t="s">
         <v>404</v>
       </c>
-      <c r="E14" s="73" t="s">
+      <c r="F14" s="73" t="s">
         <v>405</v>
       </c>
-      <c r="F14" s="73" t="s">
+      <c r="G14" s="73" t="s">
         <v>406</v>
       </c>
-      <c r="G14" s="73" t="s">
-        <v>407</v>
-      </c>
       <c r="H14" s="40" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="I14" s="48"/>
       <c r="J14" s="48"/>
@@ -9721,28 +9721,28 @@
     </row>
     <row r="15" spans="1:32" ht="27" customHeight="1">
       <c r="A15" s="40" t="s">
+        <v>293</v>
+      </c>
+      <c r="B15" s="41" t="s">
         <v>294</v>
       </c>
-      <c r="B15" s="41" t="s">
-        <v>295</v>
-      </c>
       <c r="C15" s="70" t="s">
+        <v>397</v>
+      </c>
+      <c r="D15" s="70" t="s">
         <v>398</v>
       </c>
-      <c r="D15" s="70" t="s">
+      <c r="E15" s="70" t="s">
         <v>399</v>
       </c>
-      <c r="E15" s="70" t="s">
+      <c r="F15" s="70" t="s">
         <v>400</v>
       </c>
-      <c r="F15" s="70" t="s">
+      <c r="G15" s="70" t="s">
         <v>401</v>
       </c>
-      <c r="G15" s="70" t="s">
-        <v>402</v>
-      </c>
       <c r="H15" s="40" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="I15" s="48"/>
       <c r="J15" s="48"/>
@@ -9767,10 +9767,10 @@
     </row>
     <row r="16" spans="1:32">
       <c r="A16" s="40" t="s">
+        <v>295</v>
+      </c>
+      <c r="B16" s="41" t="s">
         <v>296</v>
-      </c>
-      <c r="B16" s="41" t="s">
-        <v>297</v>
       </c>
       <c r="C16" s="69"/>
       <c r="D16" s="69"/>
@@ -9778,7 +9778,7 @@
       <c r="F16" s="69"/>
       <c r="G16" s="69"/>
       <c r="H16" s="40" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I16" s="48"/>
       <c r="J16" s="48"/>
@@ -9803,28 +9803,28 @@
     </row>
     <row r="17" spans="1:28" ht="31" customHeight="1">
       <c r="A17" s="40" t="s">
+        <v>297</v>
+      </c>
+      <c r="B17" s="41" t="s">
         <v>298</v>
       </c>
-      <c r="B17" s="41" t="s">
-        <v>299</v>
-      </c>
       <c r="C17" s="70" t="s">
+        <v>397</v>
+      </c>
+      <c r="D17" s="70" t="s">
         <v>398</v>
       </c>
-      <c r="D17" s="70" t="s">
+      <c r="E17" s="70" t="s">
         <v>399</v>
       </c>
-      <c r="E17" s="70" t="s">
+      <c r="F17" s="70" t="s">
         <v>400</v>
       </c>
-      <c r="F17" s="70" t="s">
+      <c r="G17" s="70" t="s">
         <v>401</v>
       </c>
-      <c r="G17" s="70" t="s">
-        <v>402</v>
-      </c>
       <c r="H17" s="40" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="I17" s="48"/>
       <c r="J17" s="48"/>
@@ -9849,28 +9849,28 @@
     </row>
     <row r="18" spans="1:28" ht="27" customHeight="1">
       <c r="A18" s="40" t="s">
+        <v>299</v>
+      </c>
+      <c r="B18" s="41" t="s">
         <v>300</v>
       </c>
-      <c r="B18" s="41" t="s">
-        <v>301</v>
-      </c>
       <c r="C18" s="68" t="s">
+        <v>407</v>
+      </c>
+      <c r="D18" s="68" t="s">
         <v>408</v>
       </c>
-      <c r="D18" s="68" t="s">
+      <c r="E18" s="68" t="s">
         <v>409</v>
       </c>
-      <c r="E18" s="68" t="s">
+      <c r="F18" s="68" t="s">
         <v>410</v>
       </c>
-      <c r="F18" s="68" t="s">
+      <c r="G18" s="68" t="s">
         <v>411</v>
       </c>
-      <c r="G18" s="68" t="s">
-        <v>412</v>
-      </c>
       <c r="H18" s="40" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I18" s="48"/>
       <c r="J18" s="48"/>
@@ -9895,10 +9895,10 @@
     </row>
     <row r="19" spans="1:28" ht="27" customHeight="1">
       <c r="A19" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="B19" s="41" t="s">
         <v>302</v>
-      </c>
-      <c r="B19" s="41" t="s">
-        <v>303</v>
       </c>
       <c r="C19" s="69"/>
       <c r="D19" s="69"/>
@@ -9906,7 +9906,7 @@
       <c r="F19" s="69"/>
       <c r="G19" s="69"/>
       <c r="H19" s="40" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="I19" s="48"/>
       <c r="J19" s="48"/>
@@ -9931,10 +9931,10 @@
     </row>
     <row r="20" spans="1:28" ht="27" customHeight="1">
       <c r="A20" s="40" t="s">
+        <v>303</v>
+      </c>
+      <c r="B20" s="41" t="s">
         <v>304</v>
-      </c>
-      <c r="B20" s="41" t="s">
-        <v>305</v>
       </c>
       <c r="C20" s="69"/>
       <c r="D20" s="69"/>
@@ -9942,7 +9942,7 @@
       <c r="F20" s="69"/>
       <c r="G20" s="69"/>
       <c r="H20" s="40" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="I20" s="48"/>
       <c r="J20" s="48"/>
@@ -9967,10 +9967,10 @@
     </row>
     <row r="21" spans="1:28" ht="27" customHeight="1">
       <c r="A21" s="40" t="s">
+        <v>305</v>
+      </c>
+      <c r="B21" s="41" t="s">
         <v>306</v>
-      </c>
-      <c r="B21" s="41" t="s">
-        <v>307</v>
       </c>
       <c r="C21" s="69"/>
       <c r="D21" s="69"/>
@@ -9978,7 +9978,7 @@
       <c r="F21" s="69"/>
       <c r="G21" s="69"/>
       <c r="H21" s="40" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I21" s="48"/>
       <c r="J21" s="48"/>
@@ -10003,28 +10003,28 @@
     </row>
     <row r="22" spans="1:28" ht="27" customHeight="1">
       <c r="A22" s="40" t="s">
+        <v>307</v>
+      </c>
+      <c r="B22" s="41" t="s">
         <v>308</v>
       </c>
-      <c r="B22" s="41" t="s">
-        <v>309</v>
-      </c>
       <c r="C22" s="70" t="s">
+        <v>397</v>
+      </c>
+      <c r="D22" s="70" t="s">
         <v>398</v>
       </c>
-      <c r="D22" s="70" t="s">
+      <c r="E22" s="70" t="s">
         <v>399</v>
       </c>
-      <c r="E22" s="70" t="s">
+      <c r="F22" s="70" t="s">
         <v>400</v>
       </c>
-      <c r="F22" s="70" t="s">
+      <c r="G22" s="70" t="s">
         <v>401</v>
       </c>
-      <c r="G22" s="70" t="s">
-        <v>402</v>
-      </c>
       <c r="H22" s="40" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I22" s="48"/>
       <c r="J22" s="48"/>

</xml_diff>

<commit_message>
deploying the Malawi app
</commit_message>
<xml_diff>
--- a/GACPAQ pages.xlsx
+++ b/GACPAQ pages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doncastillo/Code/gacpaq/gacpaq-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B92EE8-3CAD-5C45-9825-9858025E5563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4977A681-8042-2E49-9C9F-97C4FBA60E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21660" yWindow="-17960" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
+    <workbookView xWindow="18260" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="956" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="425">
   <si>
     <t>Page Number</t>
   </si>
@@ -2881,6 +2881,15 @@
   <si>
     <t>transportation_9
 (walk)</t>
+  </si>
+  <si>
+    <t>ready to be deployed</t>
+  </si>
+  <si>
+    <t>deploying…;</t>
+  </si>
+  <si>
+    <t>deploying.,..</t>
   </si>
 </sst>
 </file>
@@ -4354,7 +4363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{460A6040-ECD3-3B44-8E8B-CFDB1F40DF24}">
   <dimension ref="A1:K88"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -7761,11 +7770,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BEEE373-47BE-6F4C-8F66-ACD6798C647F}">
   <dimension ref="A1:AJ23"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="114" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="114" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8050,10 +8059,10 @@
         <v>386</v>
       </c>
       <c r="G5" s="55"/>
-      <c r="H5" s="55" t="s">
+      <c r="H5" s="54" t="s">
         <v>420</v>
       </c>
-      <c r="I5" s="55" t="s">
+      <c r="I5" s="54" t="s">
         <v>420</v>
       </c>
       <c r="J5" s="55"/>
@@ -8280,7 +8289,9 @@
       <c r="I9" s="53" t="s">
         <v>337</v>
       </c>
-      <c r="J9" s="55"/>
+      <c r="J9" s="56" t="s">
+        <v>422</v>
+      </c>
       <c r="K9" s="55"/>
       <c r="L9" s="40" t="s">
         <v>417</v>
@@ -8322,8 +8333,8 @@
       <c r="E10" s="53" t="s">
         <v>337</v>
       </c>
-      <c r="F10" s="57" t="s">
-        <v>344</v>
+      <c r="F10" s="53" t="s">
+        <v>337</v>
       </c>
       <c r="G10" s="53" t="s">
         <v>337</v>
@@ -8334,7 +8345,9 @@
       <c r="I10" s="53" t="s">
         <v>337</v>
       </c>
-      <c r="J10" s="55"/>
+      <c r="J10" s="56" t="s">
+        <v>422</v>
+      </c>
       <c r="K10" s="55"/>
       <c r="L10" s="40" t="s">
         <v>281</v>
@@ -8439,7 +8452,7 @@
         <v>337</v>
       </c>
       <c r="J12" s="56" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="K12" s="55"/>
       <c r="L12" s="40" t="s">
@@ -8495,7 +8508,7 @@
         <v>337</v>
       </c>
       <c r="J13" s="56" t="s">
-        <v>416</v>
+        <v>424</v>
       </c>
       <c r="K13" s="55"/>
       <c r="L13" s="40" t="s">
@@ -8664,7 +8677,9 @@
       <c r="I16" s="53" t="s">
         <v>337</v>
       </c>
-      <c r="J16" s="55"/>
+      <c r="J16" s="56" t="s">
+        <v>422</v>
+      </c>
       <c r="K16" s="55"/>
       <c r="L16" s="40" t="s">
         <v>293</v>
@@ -8714,7 +8729,9 @@
       <c r="I17" s="53" t="s">
         <v>337</v>
       </c>
-      <c r="J17" s="55"/>
+      <c r="J17" s="56" t="s">
+        <v>422</v>
+      </c>
       <c r="K17" s="55"/>
       <c r="L17" s="40" t="s">
         <v>295</v>

</xml_diff>

<commit_message>
updated the GACPAQ pages
</commit_message>
<xml_diff>
--- a/GACPAQ pages.xlsx
+++ b/GACPAQ pages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doncastillo/Code/gacpaq/gacpaq-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4977A681-8042-2E49-9C9F-97C4FBA60E9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AD90A1-4B89-B947-823E-9686A13A40C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18260" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
   </bookViews>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="425">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="961" uniqueCount="422">
   <si>
     <t>Page Number</t>
   </si>
@@ -2873,9 +2873,6 @@
     <t>en-IN</t>
   </si>
   <si>
-    <t>available</t>
-  </si>
-  <si>
     <t>adopt from es-ES</t>
   </si>
   <si>
@@ -2884,12 +2881,6 @@
   </si>
   <si>
     <t>ready to be deployed</t>
-  </si>
-  <si>
-    <t>deploying…;</t>
-  </si>
-  <si>
-    <t>deploying.,..</t>
   </si>
 </sst>
 </file>
@@ -5364,7 +5355,7 @@
       </c>
       <c r="E40" s="31"/>
       <c r="F40" s="32" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G40" s="32"/>
       <c r="H40" s="31" t="s">
@@ -7774,7 +7765,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L12" sqref="L12"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -8060,10 +8051,10 @@
       </c>
       <c r="G5" s="55"/>
       <c r="H5" s="54" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="I5" s="54" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="J5" s="55"/>
       <c r="K5" s="55"/>
@@ -8229,13 +8220,15 @@
       <c r="G8" s="53" t="s">
         <v>337</v>
       </c>
-      <c r="H8" s="56" t="s">
-        <v>419</v>
-      </c>
-      <c r="I8" s="56" t="s">
-        <v>419</v>
-      </c>
-      <c r="J8" s="55"/>
+      <c r="H8" s="53" t="s">
+        <v>337</v>
+      </c>
+      <c r="I8" s="53" t="s">
+        <v>337</v>
+      </c>
+      <c r="J8" s="56" t="s">
+        <v>421</v>
+      </c>
       <c r="K8" s="55"/>
       <c r="L8" s="40" t="s">
         <v>336</v>
@@ -8290,7 +8283,7 @@
         <v>337</v>
       </c>
       <c r="J9" s="56" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K9" s="55"/>
       <c r="L9" s="40" t="s">
@@ -8346,7 +8339,7 @@
         <v>337</v>
       </c>
       <c r="J10" s="56" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K10" s="55"/>
       <c r="L10" s="40" t="s">
@@ -8451,8 +8444,8 @@
       <c r="I12" s="53" t="s">
         <v>337</v>
       </c>
-      <c r="J12" s="56" t="s">
-        <v>423</v>
+      <c r="J12" s="53" t="s">
+        <v>343</v>
       </c>
       <c r="K12" s="55"/>
       <c r="L12" s="40" t="s">
@@ -8507,8 +8500,8 @@
       <c r="I13" s="53" t="s">
         <v>337</v>
       </c>
-      <c r="J13" s="56" t="s">
-        <v>424</v>
+      <c r="J13" s="53" t="s">
+        <v>343</v>
       </c>
       <c r="K13" s="55"/>
       <c r="L13" s="40" t="s">
@@ -8678,7 +8671,7 @@
         <v>337</v>
       </c>
       <c r="J16" s="56" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K16" s="55"/>
       <c r="L16" s="40" t="s">
@@ -8730,7 +8723,7 @@
         <v>337</v>
       </c>
       <c r="J17" s="56" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K17" s="55"/>
       <c r="L17" s="40" t="s">

</xml_diff>

<commit_message>
updated the GACPAQ pages spreadsheet
</commit_message>
<xml_diff>
--- a/GACPAQ pages.xlsx
+++ b/GACPAQ pages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doncastillo/Code/gacpaq/gacpaq-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67AD90A1-4B89-B947-823E-9686A13A40C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43B0C969-3023-2140-845B-90E6B4E5B2FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18260" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
   </bookViews>
@@ -4355,10 +4355,10 @@
   <dimension ref="A1:K88"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="F72" sqref="F72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7765,7 +7765,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>

<commit_message>
updated GAC-PAQ pages document
</commit_message>
<xml_diff>
--- a/GACPAQ pages.xlsx
+++ b/GACPAQ pages.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doncastillo/Code/gacpaq/gacpaq-app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C34F60F0-9F6F-6243-B288-FA40D0D04611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56686A86-3F82-794B-9BE7-36B735D17A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20140" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
+    <workbookView xWindow="-20060" yWindow="-20860" windowWidth="38400" windowHeight="21100" activeTab="5" xr2:uid="{F0D6E043-EC2B-F746-8C39-25C7730C9E54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="969" uniqueCount="422">
   <si>
     <t>Page Number</t>
   </si>
@@ -2666,9 +2666,6 @@
     <t>ok</t>
   </si>
   <si>
-    <t>in review</t>
-  </si>
-  <si>
     <t>on-going (1)</t>
   </si>
   <si>
@@ -2880,7 +2877,10 @@
     <t>ready to be deployed</t>
   </si>
   <si>
-    <t>available</t>
+    <t>on-going (11)</t>
+  </si>
+  <si>
+    <t>on-going (12)</t>
   </si>
 </sst>
 </file>
@@ -3309,7 +3309,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3447,9 +3447,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -5355,7 +5352,7 @@
       </c>
       <c r="E40" s="31"/>
       <c r="F40" s="32" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G40" s="32"/>
       <c r="H40" s="31" t="s">
@@ -5927,7 +5924,7 @@
       </c>
     </row>
     <row r="69" spans="1:11" ht="34">
-      <c r="A69" s="61" t="s">
+      <c r="A69" s="60" t="s">
         <v>149</v>
       </c>
       <c r="B69" s="13">
@@ -5945,7 +5942,7 @@
       </c>
     </row>
     <row r="70" spans="1:11" ht="51">
-      <c r="A70" s="61" t="s">
+      <c r="A70" s="60" t="s">
         <v>149</v>
       </c>
       <c r="B70" s="13">
@@ -6040,7 +6037,7 @@
       </c>
     </row>
     <row r="77" spans="1:11">
-      <c r="A77" s="62" t="s">
+      <c r="A77" s="61" t="s">
         <v>332</v>
       </c>
       <c r="B77" s="13" t="s">
@@ -6054,7 +6051,7 @@
       </c>
     </row>
     <row r="78" spans="1:11">
-      <c r="A78" s="62" t="s">
+      <c r="A78" s="61" t="s">
         <v>332</v>
       </c>
       <c r="B78" s="13" t="s">
@@ -6068,7 +6065,7 @@
       </c>
     </row>
     <row r="79" spans="1:11">
-      <c r="A79" s="62" t="s">
+      <c r="A79" s="61" t="s">
         <v>332</v>
       </c>
       <c r="B79" s="13">
@@ -6082,7 +6079,7 @@
       </c>
     </row>
     <row r="80" spans="1:11">
-      <c r="A80" s="62" t="s">
+      <c r="A80" s="61" t="s">
         <v>332</v>
       </c>
       <c r="B80" s="13">
@@ -6096,7 +6093,7 @@
       </c>
     </row>
     <row r="81" spans="1:8" ht="17" customHeight="1">
-      <c r="A81" s="62" t="s">
+      <c r="A81" s="61" t="s">
         <v>332</v>
       </c>
       <c r="B81" s="13">
@@ -6110,7 +6107,7 @@
       </c>
     </row>
     <row r="82" spans="1:8">
-      <c r="A82" s="62" t="s">
+      <c r="A82" s="61" t="s">
         <v>332</v>
       </c>
       <c r="B82" s="13">
@@ -6119,12 +6116,12 @@
       <c r="F82" s="13" t="s">
         <v>359</v>
       </c>
-      <c r="H82" s="63" t="s">
+      <c r="H82" s="62" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="83" spans="1:8">
-      <c r="A83" s="62" t="s">
+      <c r="A83" s="61" t="s">
         <v>332</v>
       </c>
       <c r="B83" s="13" t="s">
@@ -6138,7 +6135,7 @@
       </c>
     </row>
     <row r="84" spans="1:8">
-      <c r="A84" s="62" t="s">
+      <c r="A84" s="61" t="s">
         <v>332</v>
       </c>
       <c r="B84" s="13">
@@ -6152,7 +6149,7 @@
       </c>
     </row>
     <row r="85" spans="1:8">
-      <c r="A85" s="62" t="s">
+      <c r="A85" s="61" t="s">
         <v>332</v>
       </c>
       <c r="B85" s="13" t="s">
@@ -6166,7 +6163,7 @@
       </c>
     </row>
     <row r="86" spans="1:8">
-      <c r="A86" s="62" t="s">
+      <c r="A86" s="61" t="s">
         <v>332</v>
       </c>
       <c r="B86" s="13">
@@ -6180,7 +6177,7 @@
       </c>
     </row>
     <row r="87" spans="1:8">
-      <c r="A87" s="62" t="s">
+      <c r="A87" s="61" t="s">
         <v>332</v>
       </c>
       <c r="B87" s="13" t="s">
@@ -6260,10 +6257,10 @@
       <c r="B4" s="35">
         <v>0</v>
       </c>
-      <c r="C4" s="64">
+      <c r="C4" s="63">
         <v>5</v>
       </c>
-      <c r="D4" s="65">
+      <c r="D4" s="64">
         <v>5</v>
       </c>
       <c r="E4" s="9">
@@ -6289,10 +6286,10 @@
       <c r="B5" s="35">
         <v>1</v>
       </c>
-      <c r="C5" s="64">
+      <c r="C5" s="63">
         <v>10</v>
       </c>
-      <c r="D5" s="65">
+      <c r="D5" s="64">
         <v>10</v>
       </c>
       <c r="E5" s="9">
@@ -6306,10 +6303,10 @@
       <c r="B6" s="35">
         <v>2</v>
       </c>
-      <c r="C6" s="64">
+      <c r="C6" s="63">
         <v>7</v>
       </c>
-      <c r="D6" s="65">
+      <c r="D6" s="64">
         <v>7</v>
       </c>
       <c r="E6" s="9">
@@ -6323,10 +6320,10 @@
       <c r="B7" s="35">
         <v>3</v>
       </c>
-      <c r="C7" s="64">
+      <c r="C7" s="63">
         <v>6</v>
       </c>
-      <c r="D7" s="65">
+      <c r="D7" s="64">
         <v>6</v>
       </c>
       <c r="E7" s="9">
@@ -6340,10 +6337,10 @@
       <c r="B8" s="35">
         <v>4</v>
       </c>
-      <c r="C8" s="64">
+      <c r="C8" s="63">
         <v>14</v>
       </c>
-      <c r="D8" s="65">
+      <c r="D8" s="64">
         <v>14</v>
       </c>
       <c r="E8" s="9">
@@ -6357,10 +6354,10 @@
       <c r="B9" s="35">
         <v>5</v>
       </c>
-      <c r="C9" s="64">
+      <c r="C9" s="63">
         <v>6</v>
       </c>
-      <c r="D9" s="65">
+      <c r="D9" s="64">
         <v>6</v>
       </c>
       <c r="E9" s="9">
@@ -6374,10 +6371,10 @@
       <c r="B10" s="35">
         <v>6</v>
       </c>
-      <c r="C10" s="64">
+      <c r="C10" s="63">
         <v>5</v>
       </c>
-      <c r="D10" s="65">
+      <c r="D10" s="64">
         <v>5</v>
       </c>
       <c r="E10" s="9">
@@ -6391,10 +6388,10 @@
       <c r="B11" s="35">
         <v>7</v>
       </c>
-      <c r="C11" s="64">
+      <c r="C11" s="63">
         <v>4</v>
       </c>
-      <c r="D11" s="65">
+      <c r="D11" s="64">
         <v>4</v>
       </c>
       <c r="E11" s="9">
@@ -6408,10 +6405,10 @@
       <c r="B12" s="35">
         <v>8</v>
       </c>
-      <c r="C12" s="64">
+      <c r="C12" s="63">
         <v>3</v>
       </c>
-      <c r="D12" s="65">
+      <c r="D12" s="64">
         <v>3</v>
       </c>
       <c r="E12" s="9">
@@ -6419,7 +6416,7 @@
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="61" t="s">
+      <c r="A13" s="60" t="s">
         <v>149</v>
       </c>
       <c r="B13" s="35"/>
@@ -6445,7 +6442,7 @@
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="62" t="s">
+      <c r="A15" s="61" t="s">
         <v>332</v>
       </c>
       <c r="B15" s="35">
@@ -6811,38 +6808,38 @@
     <row r="1" spans="1:31" s="39" customFormat="1" ht="16" customHeight="1">
       <c r="A1" s="38"/>
       <c r="B1" s="38"/>
-      <c r="C1" s="74" t="s">
+      <c r="C1" s="73" t="s">
         <v>253</v>
       </c>
-      <c r="D1" s="74"/>
-      <c r="E1" s="74"/>
-      <c r="F1" s="74"/>
-      <c r="G1" s="79" t="s">
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="73"/>
+      <c r="G1" s="78" t="s">
         <v>254</v>
       </c>
-      <c r="H1" s="80"/>
-      <c r="I1" s="80"/>
-      <c r="J1" s="80"/>
-      <c r="K1" s="80"/>
-      <c r="L1" s="80"/>
-      <c r="M1" s="80"/>
-      <c r="N1" s="80"/>
-      <c r="O1" s="80"/>
-      <c r="P1" s="80"/>
-      <c r="Q1" s="80"/>
-      <c r="R1" s="80"/>
-      <c r="S1" s="80"/>
-      <c r="T1" s="80"/>
-      <c r="U1" s="80"/>
-      <c r="V1" s="80"/>
-      <c r="W1" s="80"/>
-      <c r="X1" s="80"/>
-      <c r="Y1" s="80"/>
-      <c r="Z1" s="80"/>
-      <c r="AA1" s="80"/>
-      <c r="AB1" s="80"/>
-      <c r="AC1" s="80"/>
-      <c r="AD1" s="80"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="79"/>
+      <c r="W1" s="79"/>
+      <c r="X1" s="79"/>
+      <c r="Y1" s="79"/>
+      <c r="Z1" s="79"/>
+      <c r="AA1" s="79"/>
+      <c r="AB1" s="79"/>
+      <c r="AC1" s="79"/>
+      <c r="AD1" s="79"/>
       <c r="AE1" s="39" t="s">
         <v>309</v>
       </c>
@@ -6862,46 +6859,46 @@
       <c r="F2" s="40" t="s">
         <v>258</v>
       </c>
-      <c r="G2" s="75" t="s">
+      <c r="G2" s="74" t="s">
         <v>259</v>
       </c>
-      <c r="H2" s="76"/>
-      <c r="I2" s="77"/>
-      <c r="J2" s="75" t="s">
+      <c r="H2" s="75"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="74" t="s">
         <v>260</v>
       </c>
-      <c r="K2" s="76"/>
-      <c r="L2" s="77"/>
-      <c r="M2" s="75" t="s">
+      <c r="K2" s="75"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="74" t="s">
         <v>261</v>
       </c>
-      <c r="N2" s="76"/>
-      <c r="O2" s="77"/>
-      <c r="P2" s="75" t="s">
+      <c r="N2" s="75"/>
+      <c r="O2" s="76"/>
+      <c r="P2" s="74" t="s">
         <v>262</v>
       </c>
-      <c r="Q2" s="76"/>
-      <c r="R2" s="77"/>
-      <c r="S2" s="75" t="s">
+      <c r="Q2" s="75"/>
+      <c r="R2" s="76"/>
+      <c r="S2" s="74" t="s">
         <v>263</v>
       </c>
-      <c r="T2" s="76"/>
-      <c r="U2" s="77"/>
-      <c r="V2" s="75" t="s">
+      <c r="T2" s="75"/>
+      <c r="U2" s="76"/>
+      <c r="V2" s="74" t="s">
         <v>264</v>
       </c>
-      <c r="W2" s="76"/>
-      <c r="X2" s="77"/>
-      <c r="Y2" s="75" t="s">
+      <c r="W2" s="75"/>
+      <c r="X2" s="76"/>
+      <c r="Y2" s="74" t="s">
         <v>265</v>
       </c>
-      <c r="Z2" s="76"/>
-      <c r="AA2" s="77"/>
-      <c r="AB2" s="78" t="s">
+      <c r="Z2" s="75"/>
+      <c r="AA2" s="76"/>
+      <c r="AB2" s="77" t="s">
         <v>311</v>
       </c>
-      <c r="AC2" s="78"/>
-      <c r="AD2" s="78"/>
+      <c r="AC2" s="77"/>
+      <c r="AD2" s="77"/>
     </row>
     <row r="3" spans="1:31" s="39" customFormat="1">
       <c r="A3" s="40"/>
@@ -7765,14 +7762,14 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomRight" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
-    <col min="3" max="6" width="14.6640625" style="59" customWidth="1"/>
-    <col min="7" max="11" width="14.6640625" style="60" customWidth="1"/>
+    <col min="3" max="6" width="14.6640625" style="58" customWidth="1"/>
+    <col min="7" max="11" width="14.6640625" style="59" customWidth="1"/>
     <col min="12" max="12" width="17.5" customWidth="1"/>
     <col min="13" max="13" width="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="5" customWidth="1"/>
@@ -7888,7 +7885,7 @@
         <v>343</v>
       </c>
       <c r="K2" s="56" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="L2" s="40" t="s">
         <v>268</v>
@@ -7946,7 +7943,7 @@
         <v>343</v>
       </c>
       <c r="K3" s="56" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L3" s="40" t="s">
         <v>270</v>
@@ -8004,7 +8001,7 @@
         <v>343</v>
       </c>
       <c r="K4" s="56" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="L4" s="40" t="s">
         <v>272</v>
@@ -8043,11 +8040,11 @@
       <c r="D5" s="53" t="s">
         <v>337</v>
       </c>
-      <c r="E5" s="57" t="s">
-        <v>345</v>
-      </c>
-      <c r="F5" s="56" t="s">
-        <v>386</v>
+      <c r="E5" s="53" t="s">
+        <v>337</v>
+      </c>
+      <c r="F5" s="53" t="s">
+        <v>337</v>
       </c>
       <c r="G5" s="55"/>
       <c r="H5" s="53" t="s">
@@ -8056,7 +8053,9 @@
       <c r="I5" s="53" t="s">
         <v>337</v>
       </c>
-      <c r="J5" s="55"/>
+      <c r="J5" s="56" t="s">
+        <v>419</v>
+      </c>
       <c r="K5" s="55"/>
       <c r="L5" s="40" t="s">
         <v>335</v>
@@ -8114,7 +8113,7 @@
         <v>343</v>
       </c>
       <c r="K6" s="56" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="L6" s="40" t="s">
         <v>275</v>
@@ -8172,7 +8171,7 @@
         <v>343</v>
       </c>
       <c r="K7" s="56" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="L7" s="40" t="s">
         <v>277</v>
@@ -8226,10 +8225,12 @@
       <c r="I8" s="53" t="s">
         <v>337</v>
       </c>
-      <c r="J8" s="56" t="s">
-        <v>420</v>
-      </c>
-      <c r="K8" s="55"/>
+      <c r="J8" s="53" t="s">
+        <v>343</v>
+      </c>
+      <c r="K8" s="54" t="s">
+        <v>421</v>
+      </c>
       <c r="L8" s="40" t="s">
         <v>336</v>
       </c>
@@ -8256,11 +8257,11 @@
     </row>
     <row r="9" spans="1:36" ht="27" customHeight="1">
       <c r="A9" s="40" t="s">
+        <v>416</v>
+      </c>
+      <c r="B9" s="41" t="s">
         <v>417</v>
       </c>
-      <c r="B9" s="41" t="s">
-        <v>418</v>
-      </c>
       <c r="C9" s="53" t="s">
         <v>337</v>
       </c>
@@ -8283,11 +8284,11 @@
         <v>337</v>
       </c>
       <c r="J9" s="56" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="K9" s="55"/>
       <c r="L9" s="40" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="M9" s="48"/>
       <c r="N9" s="48"/>
@@ -8339,7 +8340,7 @@
         <v>337</v>
       </c>
       <c r="J10" s="56" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="K10" s="55"/>
       <c r="L10" s="40" t="s">
@@ -8386,15 +8387,17 @@
         <v>344</v>
       </c>
       <c r="G11" s="56" t="s">
-        <v>416</v>
-      </c>
-      <c r="H11" s="56" t="s">
-        <v>421</v>
-      </c>
-      <c r="I11" s="56" t="s">
-        <v>421</v>
-      </c>
-      <c r="J11" s="55"/>
+        <v>415</v>
+      </c>
+      <c r="H11" s="53" t="s">
+        <v>337</v>
+      </c>
+      <c r="I11" s="53" t="s">
+        <v>337</v>
+      </c>
+      <c r="J11" s="56" t="s">
+        <v>419</v>
+      </c>
       <c r="K11" s="55"/>
       <c r="L11" s="40" t="s">
         <v>283</v>
@@ -8451,7 +8454,9 @@
       <c r="J12" s="53" t="s">
         <v>343</v>
       </c>
-      <c r="K12" s="55"/>
+      <c r="K12" s="54" t="s">
+        <v>420</v>
+      </c>
       <c r="L12" s="40" t="s">
         <v>285</v>
       </c>
@@ -8507,7 +8512,9 @@
       <c r="J13" s="53" t="s">
         <v>343</v>
       </c>
-      <c r="K13" s="55"/>
+      <c r="K13" s="54" t="s">
+        <v>420</v>
+      </c>
       <c r="L13" s="40" t="s">
         <v>287</v>
       </c>
@@ -8564,7 +8571,7 @@
         <v>343</v>
       </c>
       <c r="K14" s="56" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="L14" s="40" t="s">
         <v>289</v>
@@ -8622,7 +8629,7 @@
         <v>343</v>
       </c>
       <c r="K15" s="56" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L15" s="40" t="s">
         <v>291</v>
@@ -8675,7 +8682,7 @@
         <v>337</v>
       </c>
       <c r="J16" s="56" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="K16" s="55"/>
       <c r="L16" s="40" t="s">
@@ -8718,7 +8725,9 @@
       <c r="E17" s="57" t="s">
         <v>345</v>
       </c>
-      <c r="F17" s="58"/>
+      <c r="F17" s="57" t="s">
+        <v>344</v>
+      </c>
       <c r="G17" s="55"/>
       <c r="H17" s="53" t="s">
         <v>337</v>
@@ -8727,7 +8736,7 @@
         <v>337</v>
       </c>
       <c r="J17" s="56" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="K17" s="55"/>
       <c r="L17" s="40" t="s">
@@ -8786,7 +8795,7 @@
         <v>343</v>
       </c>
       <c r="K18" s="56" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="L18" s="40" t="s">
         <v>297</v>
@@ -8844,7 +8853,7 @@
         <v>343</v>
       </c>
       <c r="K19" s="54" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="L19" s="40" t="s">
         <v>299</v>
@@ -8902,7 +8911,7 @@
         <v>343</v>
       </c>
       <c r="K20" s="56" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="L20" s="40" t="s">
         <v>301</v>
@@ -8960,7 +8969,7 @@
         <v>343</v>
       </c>
       <c r="K21" s="56" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="L21" s="40" t="s">
         <v>303</v>
@@ -9018,7 +9027,7 @@
         <v>343</v>
       </c>
       <c r="K22" s="56" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L22" s="40" t="s">
         <v>305</v>
@@ -9076,7 +9085,7 @@
         <v>343</v>
       </c>
       <c r="K23" s="56" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="L23" s="40" t="s">
         <v>307</v>
@@ -9121,10 +9130,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="17.5" style="66" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="66"/>
-    <col min="3" max="7" width="14.6640625" style="71" customWidth="1"/>
-    <col min="8" max="8" width="17.5" style="66" customWidth="1"/>
+    <col min="1" max="1" width="17.5" style="65" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="65"/>
+    <col min="3" max="7" width="14.6640625" style="70" customWidth="1"/>
+    <col min="8" max="8" width="17.5" style="65" customWidth="1"/>
     <col min="9" max="9" width="5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5" customWidth="1"/>
     <col min="11" max="11" width="5.33203125" bestFit="1" customWidth="1"/>
@@ -9152,20 +9161,20 @@
     <row r="1" spans="1:32" s="50" customFormat="1" ht="49" customHeight="1">
       <c r="A1" s="47"/>
       <c r="B1" s="47"/>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="66" t="s">
+        <v>396</v>
+      </c>
+      <c r="D1" s="66" t="s">
         <v>397</v>
       </c>
-      <c r="D1" s="67" t="s">
+      <c r="E1" s="66" t="s">
         <v>398</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="F1" s="66" t="s">
         <v>399</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="G1" s="66" t="s">
         <v>400</v>
-      </c>
-      <c r="G1" s="67" t="s">
-        <v>401</v>
       </c>
       <c r="H1" s="47"/>
       <c r="I1" s="49"/>
@@ -9202,20 +9211,20 @@
       <c r="B2" s="41" t="s">
         <v>269</v>
       </c>
-      <c r="C2" s="68" t="s">
-        <v>407</v>
-      </c>
-      <c r="D2" s="68" t="s">
+      <c r="C2" s="67" t="s">
+        <v>406</v>
+      </c>
+      <c r="D2" s="67" t="s">
+        <v>411</v>
+      </c>
+      <c r="E2" s="67" t="s">
         <v>412</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="F2" s="67" t="s">
         <v>413</v>
       </c>
-      <c r="F2" s="68" t="s">
+      <c r="G2" s="67" t="s">
         <v>414</v>
-      </c>
-      <c r="G2" s="68" t="s">
-        <v>415</v>
       </c>
       <c r="H2" s="40" t="s">
         <v>268</v>
@@ -9248,20 +9257,20 @@
       <c r="B3" s="41" t="s">
         <v>271</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="C3" s="69" t="s">
+        <v>396</v>
+      </c>
+      <c r="D3" s="69" t="s">
         <v>397</v>
       </c>
-      <c r="D3" s="70" t="s">
+      <c r="E3" s="69" t="s">
         <v>398</v>
       </c>
-      <c r="E3" s="70" t="s">
+      <c r="F3" s="69" t="s">
         <v>399</v>
       </c>
-      <c r="F3" s="70" t="s">
+      <c r="G3" s="69" t="s">
         <v>400</v>
-      </c>
-      <c r="G3" s="70" t="s">
-        <v>401</v>
       </c>
       <c r="H3" s="40" t="s">
         <v>270</v>
@@ -9294,11 +9303,11 @@
       <c r="B4" s="41" t="s">
         <v>273</v>
       </c>
-      <c r="C4" s="69"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
       <c r="H4" s="40" t="s">
         <v>272</v>
       </c>
@@ -9330,20 +9339,20 @@
       <c r="B5" s="41" t="s">
         <v>329</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="C5" s="67" t="s">
+        <v>406</v>
+      </c>
+      <c r="D5" s="67" t="s">
         <v>407</v>
       </c>
-      <c r="D5" s="68" t="s">
+      <c r="E5" s="67" t="s">
         <v>408</v>
       </c>
-      <c r="E5" s="68" t="s">
+      <c r="F5" s="67" t="s">
         <v>409</v>
       </c>
-      <c r="F5" s="68" t="s">
+      <c r="G5" s="67" t="s">
         <v>410</v>
-      </c>
-      <c r="G5" s="68" t="s">
-        <v>411</v>
       </c>
       <c r="H5" s="40" t="s">
         <v>335</v>
@@ -9376,11 +9385,11 @@
       <c r="B6" s="41" t="s">
         <v>276</v>
       </c>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="69"/>
+      <c r="C6" s="68"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
       <c r="H6" s="40" t="s">
         <v>275</v>
       </c>
@@ -9412,20 +9421,20 @@
       <c r="B7" s="41" t="s">
         <v>278</v>
       </c>
-      <c r="C7" s="68" t="s">
+      <c r="C7" s="67" t="s">
+        <v>406</v>
+      </c>
+      <c r="D7" s="67" t="s">
         <v>407</v>
       </c>
-      <c r="D7" s="68" t="s">
+      <c r="E7" s="67" t="s">
         <v>408</v>
       </c>
-      <c r="E7" s="68" t="s">
+      <c r="F7" s="67" t="s">
         <v>409</v>
       </c>
-      <c r="F7" s="68" t="s">
+      <c r="G7" s="67" t="s">
         <v>410</v>
-      </c>
-      <c r="G7" s="68" t="s">
-        <v>411</v>
       </c>
       <c r="H7" s="40" t="s">
         <v>277</v>
@@ -9458,11 +9467,11 @@
       <c r="B8" s="41" t="s">
         <v>330</v>
       </c>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="69"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
       <c r="H8" s="40" t="s">
         <v>336</v>
       </c>
@@ -9494,11 +9503,11 @@
       <c r="B9" s="41" t="s">
         <v>282</v>
       </c>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
       <c r="H9" s="40" t="s">
         <v>281</v>
       </c>
@@ -9530,11 +9539,11 @@
       <c r="B10" s="41" t="s">
         <v>284</v>
       </c>
-      <c r="C10" s="69"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
       <c r="H10" s="40" t="s">
         <v>283</v>
       </c>
@@ -9566,11 +9575,11 @@
       <c r="B11" s="41" t="s">
         <v>286</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
       <c r="H11" s="40" t="s">
         <v>285</v>
       </c>
@@ -9602,20 +9611,20 @@
       <c r="B12" s="41" t="s">
         <v>288</v>
       </c>
-      <c r="C12" s="70" t="s">
+      <c r="C12" s="69" t="s">
+        <v>396</v>
+      </c>
+      <c r="D12" s="69" t="s">
         <v>397</v>
       </c>
-      <c r="D12" s="70" t="s">
+      <c r="E12" s="69" t="s">
         <v>398</v>
       </c>
-      <c r="E12" s="70" t="s">
+      <c r="F12" s="69" t="s">
         <v>399</v>
       </c>
-      <c r="F12" s="70" t="s">
+      <c r="G12" s="69" t="s">
         <v>400</v>
-      </c>
-      <c r="G12" s="70" t="s">
-        <v>401</v>
       </c>
       <c r="H12" s="40" t="s">
         <v>287</v>
@@ -9648,20 +9657,20 @@
       <c r="B13" s="41" t="s">
         <v>290</v>
       </c>
-      <c r="C13" s="68" t="s">
+      <c r="C13" s="67" t="s">
+        <v>406</v>
+      </c>
+      <c r="D13" s="67" t="s">
         <v>407</v>
       </c>
-      <c r="D13" s="68" t="s">
+      <c r="E13" s="67" t="s">
         <v>408</v>
       </c>
-      <c r="E13" s="68" t="s">
+      <c r="F13" s="67" t="s">
         <v>409</v>
       </c>
-      <c r="F13" s="68" t="s">
+      <c r="G13" s="67" t="s">
         <v>410</v>
-      </c>
-      <c r="G13" s="68" t="s">
-        <v>411</v>
       </c>
       <c r="H13" s="40" t="s">
         <v>289</v>
@@ -9694,20 +9703,20 @@
       <c r="B14" s="41" t="s">
         <v>292</v>
       </c>
-      <c r="C14" s="72" t="s">
+      <c r="C14" s="71" t="s">
+        <v>401</v>
+      </c>
+      <c r="D14" s="67" t="s">
         <v>402</v>
       </c>
-      <c r="D14" s="68" t="s">
+      <c r="E14" s="72" t="s">
         <v>403</v>
       </c>
-      <c r="E14" s="73" t="s">
+      <c r="F14" s="72" t="s">
         <v>404</v>
       </c>
-      <c r="F14" s="73" t="s">
+      <c r="G14" s="72" t="s">
         <v>405</v>
-      </c>
-      <c r="G14" s="73" t="s">
-        <v>406</v>
       </c>
       <c r="H14" s="40" t="s">
         <v>291</v>
@@ -9740,20 +9749,20 @@
       <c r="B15" s="41" t="s">
         <v>294</v>
       </c>
-      <c r="C15" s="70" t="s">
+      <c r="C15" s="69" t="s">
+        <v>396</v>
+      </c>
+      <c r="D15" s="69" t="s">
         <v>397</v>
       </c>
-      <c r="D15" s="70" t="s">
+      <c r="E15" s="69" t="s">
         <v>398</v>
       </c>
-      <c r="E15" s="70" t="s">
+      <c r="F15" s="69" t="s">
         <v>399</v>
       </c>
-      <c r="F15" s="70" t="s">
+      <c r="G15" s="69" t="s">
         <v>400</v>
-      </c>
-      <c r="G15" s="70" t="s">
-        <v>401</v>
       </c>
       <c r="H15" s="40" t="s">
         <v>293</v>
@@ -9786,11 +9795,11 @@
       <c r="B16" s="41" t="s">
         <v>296</v>
       </c>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69"/>
-      <c r="G16" s="69"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="68"/>
       <c r="H16" s="40" t="s">
         <v>295</v>
       </c>
@@ -9822,20 +9831,20 @@
       <c r="B17" s="41" t="s">
         <v>298</v>
       </c>
-      <c r="C17" s="70" t="s">
+      <c r="C17" s="69" t="s">
+        <v>396</v>
+      </c>
+      <c r="D17" s="69" t="s">
         <v>397</v>
       </c>
-      <c r="D17" s="70" t="s">
+      <c r="E17" s="69" t="s">
         <v>398</v>
       </c>
-      <c r="E17" s="70" t="s">
+      <c r="F17" s="69" t="s">
         <v>399</v>
       </c>
-      <c r="F17" s="70" t="s">
+      <c r="G17" s="69" t="s">
         <v>400</v>
-      </c>
-      <c r="G17" s="70" t="s">
-        <v>401</v>
       </c>
       <c r="H17" s="40" t="s">
         <v>297</v>
@@ -9868,20 +9877,20 @@
       <c r="B18" s="41" t="s">
         <v>300</v>
       </c>
-      <c r="C18" s="68" t="s">
+      <c r="C18" s="67" t="s">
+        <v>406</v>
+      </c>
+      <c r="D18" s="67" t="s">
         <v>407</v>
       </c>
-      <c r="D18" s="68" t="s">
+      <c r="E18" s="67" t="s">
         <v>408</v>
       </c>
-      <c r="E18" s="68" t="s">
+      <c r="F18" s="67" t="s">
         <v>409</v>
       </c>
-      <c r="F18" s="68" t="s">
+      <c r="G18" s="67" t="s">
         <v>410</v>
-      </c>
-      <c r="G18" s="68" t="s">
-        <v>411</v>
       </c>
       <c r="H18" s="40" t="s">
         <v>299</v>
@@ -9914,11 +9923,11 @@
       <c r="B19" s="41" t="s">
         <v>302</v>
       </c>
-      <c r="C19" s="69"/>
-      <c r="D19" s="69"/>
-      <c r="E19" s="69"/>
-      <c r="F19" s="69"/>
-      <c r="G19" s="69"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="68"/>
+      <c r="F19" s="68"/>
+      <c r="G19" s="68"/>
       <c r="H19" s="40" t="s">
         <v>301</v>
       </c>
@@ -9950,11 +9959,11 @@
       <c r="B20" s="41" t="s">
         <v>304</v>
       </c>
-      <c r="C20" s="69"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="69"/>
+      <c r="C20" s="68"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="68"/>
       <c r="H20" s="40" t="s">
         <v>303</v>
       </c>
@@ -9986,11 +9995,11 @@
       <c r="B21" s="41" t="s">
         <v>306</v>
       </c>
-      <c r="C21" s="69"/>
-      <c r="D21" s="69"/>
-      <c r="E21" s="69"/>
-      <c r="F21" s="69"/>
-      <c r="G21" s="69"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="68"/>
       <c r="H21" s="40" t="s">
         <v>305</v>
       </c>
@@ -10022,20 +10031,20 @@
       <c r="B22" s="41" t="s">
         <v>308</v>
       </c>
-      <c r="C22" s="70" t="s">
+      <c r="C22" s="69" t="s">
+        <v>396</v>
+      </c>
+      <c r="D22" s="69" t="s">
         <v>397</v>
       </c>
-      <c r="D22" s="70" t="s">
+      <c r="E22" s="69" t="s">
         <v>398</v>
       </c>
-      <c r="E22" s="70" t="s">
+      <c r="F22" s="69" t="s">
         <v>399</v>
       </c>
-      <c r="F22" s="70" t="s">
+      <c r="G22" s="69" t="s">
         <v>400</v>
-      </c>
-      <c r="G22" s="70" t="s">
-        <v>401</v>
       </c>
       <c r="H22" s="40" t="s">
         <v>307</v>

</xml_diff>